<commit_message>
Testing different values for analyses to ensure treatment effect modification and standardization to the correct study population.
</commit_message>
<xml_diff>
--- a/Parameters_Abortion05_Preeclampsia05_EMM.xlsx
+++ b/Parameters_Abortion05_Preeclampsia05_EMM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/preg_cohort_construction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537CED76-E1A4-4F40-B423-AE13951F45E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CCC7A5-3E96-5649-B3BD-B0E436C82631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="13" r:id="rId1"/>
@@ -47,29 +47,29 @@
   <authors>
     <author>tc={35C57926-D2D1-1E4D-B53B-E5E2E4FD75E7}</author>
     <author>tc={B783F563-C3A9-B649-91FD-4D4779A4C439}</author>
-    <author>tc={9A5BA4F2-D71D-6E40-92FE-646A717AC649}</author>
+    <author>tc={556F1810-9760-2449-B507-EA2F6F434061}</author>
     <author>tc={9D101A30-74A9-1646-AD4D-4997E6D4FEF1}</author>
-    <author>tc={AA203F26-57EB-FD4D-96A8-1E3EC58078F0}</author>
+    <author>tc={106FED08-507E-AE40-AABC-32A584DFB4BC}</author>
     <author>tc={401823BB-0005-BF4E-AC97-134F0355096C}</author>
-    <author>tc={BCDF96EB-9DF4-1E43-98E7-58F719177DD9}</author>
+    <author>tc={CD7479EC-06BE-2A44-A7C2-D26D19499F4D}</author>
     <author>tc={5475FA44-B533-5A4C-8A1C-9D4718D8077D}</author>
-    <author>tc={55A5B8CF-113A-584F-ABFB-262DB11F1536}</author>
+    <author>tc={1E2B55CA-C05F-0D4E-9254-F77C560A2AA1}</author>
     <author>tc={D494041A-02B2-084B-A234-55CDDEE484ED}</author>
-    <author>tc={20C24BD3-9274-DD49-BA6B-FAD26A6694BF}</author>
+    <author>tc={9BEE7CD4-7771-9A4D-A5F4-780C3DFECABE}</author>
     <author>tc={D6958C4D-ABB4-D443-80B1-D11F54514091}</author>
-    <author>tc={C15EC358-19C4-624D-8519-888D9D36509A}</author>
+    <author>tc={6112BA4E-33B8-404E-BD86-05556FC6BF6E}</author>
     <author>tc={A01D3486-5EA3-2A4B-A81A-30ED1504738B}</author>
-    <author>tc={DDBC1D8C-6502-5148-9760-A3D6248EE286}</author>
+    <author>tc={5B00EB6A-A038-B14E-BD11-42DE39B19C5C}</author>
     <author>tc={932BB171-45A0-CC45-9D2E-98445FA73D9C}</author>
-    <author>tc={70D543EB-93BC-CD46-AD88-602A3D7EB00C}</author>
+    <author>tc={9C276C33-5D87-B941-8825-1472D991ABC6}</author>
     <author>tc={CD3C4424-2A14-124A-BB60-B3A55586BEFC}</author>
-    <author>tc={2346C224-741D-FF43-8E6E-E465088EABEE}</author>
+    <author>tc={F3843E72-8ABE-C340-880D-749310A40CFE}</author>
     <author>tc={50C598DB-CAAF-3640-9DE3-2900861F8316}</author>
-    <author>tc={DA3B56D4-9145-A24D-B943-D5AAB2EEE929}</author>
+    <author>tc={53F55CE7-24B2-F24E-8211-4A7D6C0C1557}</author>
     <author>tc={6672E95F-B9AE-FC40-9C5D-0D9522F5210C}</author>
-    <author>tc={2AA8F2D0-6E32-494D-B542-C416DAEFF657}</author>
+    <author>tc={363E1A57-2DC1-7841-A0F3-90E916F3A285}</author>
     <author>tc={1E35AF4C-5CF6-B94F-97F4-45B0A10C5860}</author>
-    <author>tc={BA1965E4-CB1E-A446-858D-2C189AC85BC3}</author>
+    <author>tc={E7A5FC28-3D5D-B74A-BB77-12A94F89680D}</author>
     <author>tc={FF016499-E73B-CC48-A2D8-F97158353C92}</author>
     <author>tc={266C3BF3-F32A-FA4C-ADA3-E234F64F1019}</author>
     <author>tc={305F3E8D-99B5-E745-90A0-5EB82D9164B0}</author>
@@ -114,7 +114,7 @@
     Another resource. Though not the same population, this was helpful for understanding peaks</t>
       </text>
     </comment>
-    <comment ref="C2" authorId="2" shapeId="0" xr:uid="{9A5BA4F2-D71D-6E40-92FE-646A717AC649}">
+    <comment ref="C2" authorId="2" shapeId="0" xr:uid="{556F1810-9760-2449-B507-EA2F6F434061}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -134,7 +134,7 @@
     Brought it down further for computational efficiency to 0.1</t>
       </text>
     </comment>
-    <comment ref="C4" authorId="4" shapeId="0" xr:uid="{AA203F26-57EB-FD4D-96A8-1E3EC58078F0}">
+    <comment ref="C4" authorId="4" shapeId="0" xr:uid="{106FED08-507E-AE40-AABC-32A584DFB4BC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -154,7 +154,7 @@
     Lowered this even further to 0.05</t>
       </text>
     </comment>
-    <comment ref="C6" authorId="6" shapeId="0" xr:uid="{BCDF96EB-9DF4-1E43-98E7-58F719177DD9}">
+    <comment ref="C6" authorId="6" shapeId="0" xr:uid="{CD7479EC-06BE-2A44-A7C2-D26D19499F4D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -170,7 +170,7 @@
     Was 0.05</t>
       </text>
     </comment>
-    <comment ref="C7" authorId="8" shapeId="0" xr:uid="{55A5B8CF-113A-584F-ABFB-262DB11F1536}">
+    <comment ref="C7" authorId="8" shapeId="0" xr:uid="{1E2B55CA-C05F-0D4E-9254-F77C560A2AA1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -186,7 +186,7 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C8" authorId="10" shapeId="0" xr:uid="{20C24BD3-9274-DD49-BA6B-FAD26A6694BF}">
+    <comment ref="C8" authorId="10" shapeId="0" xr:uid="{9BEE7CD4-7771-9A4D-A5F4-780C3DFECABE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -202,7 +202,7 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C9" authorId="12" shapeId="0" xr:uid="{C15EC358-19C4-624D-8519-888D9D36509A}">
+    <comment ref="C9" authorId="12" shapeId="0" xr:uid="{6112BA4E-33B8-404E-BD86-05556FC6BF6E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -218,7 +218,7 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C10" authorId="14" shapeId="0" xr:uid="{DDBC1D8C-6502-5148-9760-A3D6248EE286}">
+    <comment ref="C10" authorId="14" shapeId="0" xr:uid="{5B00EB6A-A038-B14E-BD11-42DE39B19C5C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -234,7 +234,7 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C11" authorId="16" shapeId="0" xr:uid="{70D543EB-93BC-CD46-AD88-602A3D7EB00C}">
+    <comment ref="C11" authorId="16" shapeId="0" xr:uid="{9C276C33-5D87-B941-8825-1472D991ABC6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -250,7 +250,7 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C12" authorId="18" shapeId="0" xr:uid="{2346C224-741D-FF43-8E6E-E465088EABEE}">
+    <comment ref="C12" authorId="18" shapeId="0" xr:uid="{F3843E72-8ABE-C340-880D-749310A40CFE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -266,7 +266,7 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C13" authorId="20" shapeId="0" xr:uid="{DA3B56D4-9145-A24D-B943-D5AAB2EEE929}">
+    <comment ref="C13" authorId="20" shapeId="0" xr:uid="{53F55CE7-24B2-F24E-8211-4A7D6C0C1557}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -282,7 +282,7 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C20" authorId="22" shapeId="0" xr:uid="{2AA8F2D0-6E32-494D-B542-C416DAEFF657}">
+    <comment ref="C20" authorId="22" shapeId="0" xr:uid="{363E1A57-2DC1-7841-A0F3-90E916F3A285}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -304,7 +304,7 @@
 Wanted to get the prevalence of stillbirth around 1-2%. In general, we see &lt;1% stillbirth in the MarketScan cohorts, though might be higher in a chronic hypertension population.</t>
       </text>
     </comment>
-    <comment ref="C21" authorId="24" shapeId="0" xr:uid="{BA1965E4-CB1E-A446-858D-2C189AC85BC3}">
+    <comment ref="C21" authorId="24" shapeId="0" xr:uid="{E7A5FC28-3D5D-B74A-BB77-12A94F89680D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1254,7 +1254,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1305,6 +1305,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1772,10 +1778,10 @@
   <threadedComment ref="F1" dT="2024-06-21T20:36:49.49" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{0F180160-3AF6-2248-8CD9-0A3FD83760C2}" parentId="{B783F563-C3A9-B649-91FD-4D4779A4C439}">
     <text>Another resource. Though not the same population, this was helpful for understanding peaks</text>
   </threadedComment>
-  <threadedComment ref="C2" dT="2023-11-27T01:39:00.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{9A5BA4F2-D71D-6E40-92FE-646A717AC649}">
+  <threadedComment ref="C2" dT="2023-11-27T01:39:00.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{556F1810-9760-2449-B507-EA2F6F434061}">
     <text>Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.2. Same with gw 1</text>
   </threadedComment>
-  <threadedComment ref="C2" dT="2024-06-21T15:12:38.33" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{87CC0FEB-BD02-B441-89D9-2305B545E9B1}" parentId="{9A5BA4F2-D71D-6E40-92FE-646A717AC649}">
+  <threadedComment ref="C2" dT="2024-06-21T15:12:38.33" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{37A52C8D-F1A6-954D-9AFC-102ED86116AD}" parentId="{556F1810-9760-2449-B507-EA2F6F434061}">
     <text>Brought it down further for computational efficiency to 0.1</text>
   </threadedComment>
   <threadedComment ref="F2" dT="2023-11-27T01:39:00.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{9D101A30-74A9-1646-AD4D-4997E6D4FEF1}">
@@ -1784,10 +1790,10 @@
   <threadedComment ref="F2" dT="2024-06-21T15:12:38.33" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{E197D3DF-12A7-BF46-AEE2-DDFBF083DACD}" parentId="{9D101A30-74A9-1646-AD4D-4997E6D4FEF1}">
     <text>Brought it down further for computational efficiency to 0.1</text>
   </threadedComment>
-  <threadedComment ref="C4" dT="2023-11-27T01:41:40.99" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{AA203F26-57EB-FD4D-96A8-1E3EC58078F0}">
+  <threadedComment ref="C4" dT="2023-11-27T01:41:40.99" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{106FED08-507E-AE40-AABC-32A584DFB4BC}">
     <text>Lowered this slightly from 0.2 to 0.1 to improve sample size.</text>
   </threadedComment>
-  <threadedComment ref="C4" dT="2024-07-05T19:53:57.22" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{8296E04E-70A2-DB43-B659-4C2DE60CCFB5}" parentId="{AA203F26-57EB-FD4D-96A8-1E3EC58078F0}">
+  <threadedComment ref="C4" dT="2024-07-05T19:53:57.22" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{A916E440-4A03-2E47-9C89-58C775EB8E12}" parentId="{106FED08-507E-AE40-AABC-32A584DFB4BC}">
     <text>Lowered this even further to 0.05</text>
   </threadedComment>
   <threadedComment ref="F4" dT="2023-11-27T01:41:40.99" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{401823BB-0005-BF4E-AC97-134F0355096C}">
@@ -1796,58 +1802,58 @@
   <threadedComment ref="F4" dT="2024-07-05T19:53:57.22" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{B69AC2F2-53D3-D34C-A5B4-DB2986C06701}" parentId="{401823BB-0005-BF4E-AC97-134F0355096C}">
     <text>Lowered this even further to 0.05</text>
   </threadedComment>
-  <threadedComment ref="C6" dT="2024-06-21T18:59:28.37" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{BCDF96EB-9DF4-1E43-98E7-58F719177DD9}">
+  <threadedComment ref="C6" dT="2024-06-21T18:59:28.37" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{CD7479EC-06BE-2A44-A7C2-D26D19499F4D}">
     <text>Was 0.05</text>
   </threadedComment>
   <threadedComment ref="F6" dT="2024-06-21T18:59:28.37" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{5475FA44-B533-5A4C-8A1C-9D4718D8077D}">
     <text>Was 0.05</text>
   </threadedComment>
-  <threadedComment ref="C7" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{55A5B8CF-113A-584F-ABFB-262DB11F1536}">
+  <threadedComment ref="C7" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{1E2B55CA-C05F-0D4E-9254-F77C560A2AA1}">
     <text>Was 0.03</text>
   </threadedComment>
   <threadedComment ref="F7" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{D494041A-02B2-084B-A234-55CDDEE484ED}">
     <text>Was 0.03</text>
   </threadedComment>
-  <threadedComment ref="C8" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{20C24BD3-9274-DD49-BA6B-FAD26A6694BF}">
+  <threadedComment ref="C8" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{9BEE7CD4-7771-9A4D-A5F4-780C3DFECABE}">
     <text>Was 0.03</text>
   </threadedComment>
   <threadedComment ref="F8" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{D6958C4D-ABB4-D443-80B1-D11F54514091}">
     <text>Was 0.03</text>
   </threadedComment>
-  <threadedComment ref="C9" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{C15EC358-19C4-624D-8519-888D9D36509A}">
+  <threadedComment ref="C9" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{6112BA4E-33B8-404E-BD86-05556FC6BF6E}">
     <text>Was 0.03</text>
   </threadedComment>
   <threadedComment ref="F9" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{A01D3486-5EA3-2A4B-A81A-30ED1504738B}">
     <text>Was 0.03</text>
   </threadedComment>
-  <threadedComment ref="C10" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{DDBC1D8C-6502-5148-9760-A3D6248EE286}">
+  <threadedComment ref="C10" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{5B00EB6A-A038-B14E-BD11-42DE39B19C5C}">
     <text>Was 0.03</text>
   </threadedComment>
   <threadedComment ref="F10" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{932BB171-45A0-CC45-9D2E-98445FA73D9C}">
     <text>Was 0.03</text>
   </threadedComment>
-  <threadedComment ref="C11" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{70D543EB-93BC-CD46-AD88-602A3D7EB00C}">
+  <threadedComment ref="C11" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{9C276C33-5D87-B941-8825-1472D991ABC6}">
     <text>Was 0.03</text>
   </threadedComment>
   <threadedComment ref="F11" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{CD3C4424-2A14-124A-BB60-B3A55586BEFC}">
     <text>Was 0.03</text>
   </threadedComment>
-  <threadedComment ref="C12" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{2346C224-741D-FF43-8E6E-E465088EABEE}">
+  <threadedComment ref="C12" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{F3843E72-8ABE-C340-880D-749310A40CFE}">
     <text>Was 0.03</text>
   </threadedComment>
   <threadedComment ref="F12" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{50C598DB-CAAF-3640-9DE3-2900861F8316}">
     <text>Was 0.03</text>
   </threadedComment>
-  <threadedComment ref="C13" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{DA3B56D4-9145-A24D-B943-D5AAB2EEE929}">
+  <threadedComment ref="C13" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{53F55CE7-24B2-F24E-8211-4A7D6C0C1557}">
     <text>Was 0.03</text>
   </threadedComment>
   <threadedComment ref="F13" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{6672E95F-B9AE-FC40-9C5D-0D9522F5210C}">
     <text>Was 0.03</text>
   </threadedComment>
-  <threadedComment ref="C20" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{2AA8F2D0-6E32-494D-B542-C416DAEFF657}">
+  <threadedComment ref="C20" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{363E1A57-2DC1-7841-A0F3-90E916F3A285}">
     <text>All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</text>
   </threadedComment>
-  <threadedComment ref="C20" dT="2024-06-19T20:53:57.65" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{044105F4-3C00-3246-A892-C3EC22945EE2}" parentId="{2AA8F2D0-6E32-494D-B542-C416DAEFF657}">
+  <threadedComment ref="C20" dT="2024-06-19T20:53:57.65" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{86196CC3-C390-E541-8857-8D4E33E98D98}" parentId="{363E1A57-2DC1-7841-A0F3-90E916F3A285}">
     <text>This rate is per live births. Needs to be decreased. 
 Wanted to get the prevalence of stillbirth around 1-2%. In general, we see &lt;1% stillbirth in the MarketScan cohorts, though might be higher in a chronic hypertension population.</text>
   </threadedComment>
@@ -1858,7 +1864,7 @@
     <text>This rate is per live births. Needs to be decreased. 
 Wanted to get the prevalence of stillbirth around 1-2%. In general, we see &lt;1% stillbirth in the MarketScan cohorts, though might be higher in a chronic hypertension population.</text>
   </threadedComment>
-  <threadedComment ref="C21" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{BA1965E4-CB1E-A446-858D-2C189AC85BC3}">
+  <threadedComment ref="C21" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{E7A5FC28-3D5D-B74A-BB77-12A94F89680D}">
     <text>Originally 0.003s — https://stacks.cdc.gov/view/cdc/61387</text>
   </threadedComment>
   <threadedComment ref="F21" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{FF016499-E73B-CC48-A2D8-F97158353C92}">
@@ -2227,7 +2233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBAD042-1D8C-E044-AB59-2B80CE0D260D}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4:B6"/>
     </sheetView>
   </sheetViews>
@@ -2420,8 +2426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2608,14 +2614,14 @@
         <v>7</v>
       </c>
       <c r="C9" s="8">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="D9" s="8">
         <v>0</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>0.92</v>
+        <v>0.95</v>
       </c>
       <c r="F9" s="8">
         <v>0.09</v>
@@ -2629,14 +2635,14 @@
         <v>8</v>
       </c>
       <c r="C10" s="8">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D10" s="8">
         <v>0</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="F10" s="8">
         <v>1.4999999999999999E-2</v>
@@ -2650,14 +2656,14 @@
         <v>9</v>
       </c>
       <c r="C11" s="8">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D11" s="8">
         <v>0</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="F11" s="8">
         <v>1.4999999999999999E-2</v>
@@ -2692,14 +2698,14 @@
         <v>11</v>
       </c>
       <c r="C13" s="8">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D13" s="8">
         <v>0</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>0.99</v>
+        <v>0.995</v>
       </c>
       <c r="F13" s="8">
         <v>1.4999999999999999E-2</v>
@@ -2713,14 +2719,14 @@
         <v>12</v>
       </c>
       <c r="C14" s="8">
-        <v>7.4999999999999997E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D14" s="8">
         <v>0</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>0.92500000000000004</v>
+        <v>0.996</v>
       </c>
       <c r="F14" s="8">
         <v>0.01</v>
@@ -2734,14 +2740,14 @@
         <v>13</v>
       </c>
       <c r="C15" s="8">
-        <v>7.4999999999999997E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D15" s="8">
         <v>0</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>0.92500000000000004</v>
+        <v>0.996</v>
       </c>
       <c r="F15" s="8">
         <v>0.01</v>
@@ -2755,14 +2761,14 @@
         <v>14</v>
       </c>
       <c r="C16" s="8">
-        <v>7.4999999999999997E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D16" s="8">
         <v>0</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>0.92500000000000004</v>
+        <v>0.996</v>
       </c>
       <c r="F16" s="8">
         <v>0.01</v>
@@ -2776,14 +2782,14 @@
         <v>15</v>
       </c>
       <c r="C17" s="8">
-        <v>7.4999999999999997E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D17" s="8">
         <v>0</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>0.92500000000000004</v>
+        <v>0.996</v>
       </c>
       <c r="F17" s="8">
         <v>0.01</v>
@@ -3491,7 +3497,7 @@
       </c>
       <c r="C50" s="3">
         <f>C9*SimParameters!B15</f>
-        <v>0.14000000000000001</v>
+        <v>8.7500000000000008E-2</v>
       </c>
       <c r="D50" s="3">
         <f t="shared" si="1"/>
@@ -3499,7 +3505,7 @@
       </c>
       <c r="E50" s="3">
         <f t="shared" si="2"/>
-        <v>0.86</v>
+        <v>0.91249999999999998</v>
       </c>
       <c r="F50" s="3">
         <f>F9*SimParameters!E15</f>
@@ -3515,7 +3521,7 @@
       </c>
       <c r="C51" s="3">
         <f>C10*SimParameters!B15</f>
-        <v>1.7500000000000002E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D51" s="3">
         <f t="shared" si="1"/>
@@ -3523,7 +3529,7 @@
       </c>
       <c r="E51" s="3">
         <f t="shared" si="2"/>
-        <v>0.98250000000000004</v>
+        <v>0.96499999999999997</v>
       </c>
       <c r="F51" s="3">
         <f>F10*SimParameters!E15</f>
@@ -3539,7 +3545,7 @@
       </c>
       <c r="C52" s="3">
         <f>C11*SimParameters!B15</f>
-        <v>1.7500000000000002E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D52" s="3">
         <f t="shared" si="1"/>
@@ -3547,7 +3553,7 @@
       </c>
       <c r="E52" s="3">
         <f t="shared" si="2"/>
-        <v>0.98250000000000004</v>
+        <v>0.96499999999999997</v>
       </c>
       <c r="F52" s="3">
         <f>F11*SimParameters!E15</f>
@@ -3587,7 +3593,7 @@
       </c>
       <c r="C54" s="3">
         <f>C13*SimParameters!B15</f>
-        <v>1.7500000000000002E-2</v>
+        <v>8.7500000000000008E-3</v>
       </c>
       <c r="D54" s="3">
         <f t="shared" si="1"/>
@@ -3595,7 +3601,7 @@
       </c>
       <c r="E54" s="3">
         <f t="shared" si="2"/>
-        <v>0.98250000000000004</v>
+        <v>0.99124999999999996</v>
       </c>
       <c r="F54" s="3">
         <f>F13*SimParameters!E15</f>
@@ -3611,7 +3617,7 @@
       </c>
       <c r="C55" s="3">
         <f>C14*SimParameters!B15</f>
-        <v>0.13125000000000001</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D55" s="3">
         <f t="shared" si="1"/>
@@ -3619,7 +3625,7 @@
       </c>
       <c r="E55" s="3">
         <f t="shared" si="2"/>
-        <v>0.86875000000000002</v>
+        <v>0.99299999999999999</v>
       </c>
       <c r="F55" s="3">
         <f>F14*SimParameters!E15</f>
@@ -3635,7 +3641,7 @@
       </c>
       <c r="C56" s="3">
         <f>C15*SimParameters!B15</f>
-        <v>0.13125000000000001</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D56" s="3">
         <f t="shared" si="1"/>
@@ -3643,7 +3649,7 @@
       </c>
       <c r="E56" s="3">
         <f t="shared" si="2"/>
-        <v>0.86875000000000002</v>
+        <v>0.99299999999999999</v>
       </c>
       <c r="F56" s="3">
         <f>F15*SimParameters!E15</f>
@@ -3659,7 +3665,7 @@
       </c>
       <c r="C57" s="3">
         <f>C16*SimParameters!B15</f>
-        <v>0.13125000000000001</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D57" s="3">
         <f t="shared" si="1"/>
@@ -3667,7 +3673,7 @@
       </c>
       <c r="E57" s="3">
         <f t="shared" si="2"/>
-        <v>0.86875000000000002</v>
+        <v>0.99299999999999999</v>
       </c>
       <c r="F57" s="3">
         <f>F16*SimParameters!E15</f>
@@ -3683,7 +3689,7 @@
       </c>
       <c r="C58" s="3">
         <f>C17*SimParameters!B15</f>
-        <v>0.13125000000000001</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D58" s="3">
         <f t="shared" si="1"/>
@@ -3691,7 +3697,7 @@
       </c>
       <c r="E58" s="3">
         <f t="shared" si="2"/>
-        <v>0.86875000000000002</v>
+        <v>0.99299999999999999</v>
       </c>
       <c r="F58" s="3">
         <f>F17*SimParameters!E15</f>
@@ -4474,7 +4480,7 @@
       </c>
       <c r="C91" s="4">
         <f>C9*SimParameters!B16</f>
-        <v>0.24</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="D91" s="4">
         <f t="shared" si="5"/>
@@ -4482,7 +4488,7 @@
       </c>
       <c r="E91" s="4">
         <f t="shared" si="6"/>
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
       <c r="F91" s="4">
         <f>F9*SimParameters!E16</f>
@@ -4498,7 +4504,7 @@
       </c>
       <c r="C92" s="4">
         <f>C10*SimParameters!B16</f>
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="D92" s="4">
         <f t="shared" si="5"/>
@@ -4506,7 +4512,7 @@
       </c>
       <c r="E92" s="4">
         <f t="shared" si="6"/>
-        <v>0.97</v>
+        <v>0.94</v>
       </c>
       <c r="F92" s="4">
         <f>F10*SimParameters!E16</f>
@@ -4522,7 +4528,7 @@
       </c>
       <c r="C93" s="4">
         <f>C11*SimParameters!B16</f>
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="D93" s="4">
         <f t="shared" si="5"/>
@@ -4530,7 +4536,7 @@
       </c>
       <c r="E93" s="4">
         <f t="shared" si="6"/>
-        <v>0.97</v>
+        <v>0.94</v>
       </c>
       <c r="F93" s="4">
         <f>F11*SimParameters!E16</f>
@@ -4570,7 +4576,7 @@
       </c>
       <c r="C95" s="4">
         <f>C13*SimParameters!B16</f>
-        <v>0.03</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D95" s="4">
         <f t="shared" si="5"/>
@@ -4578,7 +4584,7 @@
       </c>
       <c r="E95" s="4">
         <f t="shared" si="6"/>
-        <v>0.97</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="F95" s="4">
         <f>F13*SimParameters!E16</f>
@@ -4594,7 +4600,7 @@
       </c>
       <c r="C96" s="4">
         <f>C14*SimParameters!B16</f>
-        <v>0.22499999999999998</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D96" s="4">
         <f t="shared" si="5"/>
@@ -4602,7 +4608,7 @@
       </c>
       <c r="E96" s="4">
         <f t="shared" si="6"/>
-        <v>0.77500000000000002</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="F96" s="4">
         <f>F14*SimParameters!E16</f>
@@ -4618,7 +4624,7 @@
       </c>
       <c r="C97" s="4">
         <f>C15*SimParameters!B16</f>
-        <v>0.22499999999999998</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D97" s="4">
         <f t="shared" si="5"/>
@@ -4626,7 +4632,7 @@
       </c>
       <c r="E97" s="4">
         <f t="shared" si="6"/>
-        <v>0.77500000000000002</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="F97" s="4">
         <f>F15*SimParameters!E16</f>
@@ -4642,7 +4648,7 @@
       </c>
       <c r="C98" s="4">
         <f>C16*SimParameters!B16</f>
-        <v>0.22499999999999998</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D98" s="4">
         <f t="shared" si="5"/>
@@ -4650,7 +4656,7 @@
       </c>
       <c r="E98" s="4">
         <f t="shared" si="6"/>
-        <v>0.77500000000000002</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="F98" s="4">
         <f>F16*SimParameters!E16</f>
@@ -4666,7 +4672,7 @@
       </c>
       <c r="C99" s="4">
         <f>C17*SimParameters!B16</f>
-        <v>0.22499999999999998</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D99" s="4">
         <f t="shared" si="5"/>
@@ -4674,7 +4680,7 @@
       </c>
       <c r="E99" s="4">
         <f t="shared" si="6"/>
-        <v>0.77500000000000002</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="F99" s="4">
         <f>F17*SimParameters!E16</f>
@@ -5468,7 +5474,7 @@
       </c>
       <c r="C9" s="2">
         <f>potential_preg_untrt!C9*SimParameters!$B$4</f>
-        <v>0.06</v>
+        <v>3.7500000000000006E-2</v>
       </c>
       <c r="D9" s="2">
         <f>potential_preg_untrt!D9</f>
@@ -5476,7 +5482,7 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>0.94</v>
+        <v>0.96250000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -5488,7 +5494,7 @@
       </c>
       <c r="C10" s="2">
         <f>potential_preg_untrt!C10*SimParameters!$B$4</f>
-        <v>7.4999999999999997E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D10" s="2">
         <f>potential_preg_untrt!D10</f>
@@ -5496,7 +5502,7 @@
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0.99250000000000005</v>
+        <v>0.98499999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -5508,7 +5514,7 @@
       </c>
       <c r="C11" s="2">
         <f>potential_preg_untrt!C11*SimParameters!$B$4</f>
-        <v>7.4999999999999997E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D11" s="2">
         <f>potential_preg_untrt!D11</f>
@@ -5516,7 +5522,7 @@
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>0.99250000000000005</v>
+        <v>0.98499999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -5548,7 +5554,7 @@
       </c>
       <c r="C13" s="2">
         <f>potential_preg_untrt!C13*SimParameters!$B$4</f>
-        <v>7.4999999999999997E-3</v>
+        <v>3.7499999999999999E-3</v>
       </c>
       <c r="D13" s="2">
         <f>potential_preg_untrt!D13</f>
@@ -5556,7 +5562,7 @@
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>0.99250000000000005</v>
+        <v>0.99624999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -5568,7 +5574,7 @@
       </c>
       <c r="C14" s="2">
         <f>potential_preg_untrt!C14*SimParameters!$B$4</f>
-        <v>5.6249999999999994E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D14" s="2">
         <f>potential_preg_untrt!D14</f>
@@ -5576,7 +5582,7 @@
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>0.94374999999999998</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -5588,7 +5594,7 @@
       </c>
       <c r="C15" s="2">
         <f>potential_preg_untrt!C15*SimParameters!$B$4</f>
-        <v>5.6249999999999994E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D15" s="2">
         <f>potential_preg_untrt!D15</f>
@@ -5596,7 +5602,7 @@
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>0.94374999999999998</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -5608,7 +5614,7 @@
       </c>
       <c r="C16" s="2">
         <f>potential_preg_untrt!C16*SimParameters!$B$4</f>
-        <v>5.6249999999999994E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D16" s="2">
         <f>potential_preg_untrt!D16</f>
@@ -5616,7 +5622,7 @@
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>0.94374999999999998</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -5628,7 +5634,7 @@
       </c>
       <c r="C17" s="2">
         <f>potential_preg_untrt!C17*SimParameters!$B$4</f>
-        <v>5.6249999999999994E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D17" s="2">
         <f>potential_preg_untrt!D17</f>
@@ -5636,7 +5642,7 @@
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>0.94374999999999998</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -6287,7 +6293,7 @@
       </c>
       <c r="C50" s="3">
         <f>potential_preg_untrt!C50*SimParameters!$B$5</f>
-        <v>7.0000000000000007E-2</v>
+        <v>4.3750000000000004E-2</v>
       </c>
       <c r="D50" s="3">
         <f>potential_preg_untrt!D50</f>
@@ -6295,7 +6301,7 @@
       </c>
       <c r="E50" s="3">
         <f t="shared" si="1"/>
-        <v>0.92999999999999994</v>
+        <v>0.95625000000000004</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -6307,7 +6313,7 @@
       </c>
       <c r="C51" s="3">
         <f>potential_preg_untrt!C51*SimParameters!$B$5</f>
-        <v>8.7500000000000008E-3</v>
+        <v>1.7500000000000002E-2</v>
       </c>
       <c r="D51" s="3">
         <f>potential_preg_untrt!D51</f>
@@ -6315,7 +6321,7 @@
       </c>
       <c r="E51" s="3">
         <f t="shared" si="1"/>
-        <v>0.99124999999999996</v>
+        <v>0.98250000000000004</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -6327,7 +6333,7 @@
       </c>
       <c r="C52" s="3">
         <f>potential_preg_untrt!C52*SimParameters!$B$5</f>
-        <v>8.7500000000000008E-3</v>
+        <v>1.7500000000000002E-2</v>
       </c>
       <c r="D52" s="3">
         <f>potential_preg_untrt!D52</f>
@@ -6335,7 +6341,7 @@
       </c>
       <c r="E52" s="3">
         <f t="shared" si="1"/>
-        <v>0.99124999999999996</v>
+        <v>0.98250000000000004</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -6367,7 +6373,7 @@
       </c>
       <c r="C54" s="3">
         <f>potential_preg_untrt!C54*SimParameters!$B$5</f>
-        <v>8.7500000000000008E-3</v>
+        <v>4.3750000000000004E-3</v>
       </c>
       <c r="D54" s="3">
         <f>potential_preg_untrt!D54</f>
@@ -6375,7 +6381,7 @@
       </c>
       <c r="E54" s="3">
         <f t="shared" si="1"/>
-        <v>0.99124999999999996</v>
+        <v>0.99562499999999998</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -6387,7 +6393,7 @@
       </c>
       <c r="C55" s="3">
         <f>potential_preg_untrt!C55*SimParameters!$B$5</f>
-        <v>6.5625000000000003E-2</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D55" s="3">
         <f>potential_preg_untrt!D55</f>
@@ -6395,7 +6401,7 @@
       </c>
       <c r="E55" s="3">
         <f t="shared" si="1"/>
-        <v>0.93437499999999996</v>
+        <v>0.99650000000000005</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -6407,7 +6413,7 @@
       </c>
       <c r="C56" s="3">
         <f>potential_preg_untrt!C56*SimParameters!$B$5</f>
-        <v>6.5625000000000003E-2</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D56" s="3">
         <f>potential_preg_untrt!D56</f>
@@ -6415,7 +6421,7 @@
       </c>
       <c r="E56" s="3">
         <f t="shared" si="1"/>
-        <v>0.93437499999999996</v>
+        <v>0.99650000000000005</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -6427,7 +6433,7 @@
       </c>
       <c r="C57" s="3">
         <f>potential_preg_untrt!C57*SimParameters!$B$5</f>
-        <v>6.5625000000000003E-2</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D57" s="3">
         <f>potential_preg_untrt!D57</f>
@@ -6435,7 +6441,7 @@
       </c>
       <c r="E57" s="3">
         <f t="shared" si="1"/>
-        <v>0.93437499999999996</v>
+        <v>0.99650000000000005</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -6447,7 +6453,7 @@
       </c>
       <c r="C58" s="3">
         <f>potential_preg_untrt!C58*SimParameters!$B$5</f>
-        <v>6.5625000000000003E-2</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D58" s="3">
         <f>potential_preg_untrt!D58</f>
@@ -6455,7 +6461,7 @@
       </c>
       <c r="E58" s="3">
         <f t="shared" si="1"/>
-        <v>0.93437499999999996</v>
+        <v>0.99650000000000005</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -7106,7 +7112,7 @@
       </c>
       <c r="C91" s="4">
         <f>potential_preg_untrt!C91*SimParameters!$B$6</f>
-        <v>0.06</v>
+        <v>3.7500000000000006E-2</v>
       </c>
       <c r="D91" s="4">
         <f>potential_preg_untrt!D91</f>
@@ -7114,7 +7120,7 @@
       </c>
       <c r="E91" s="4">
         <f t="shared" si="2"/>
-        <v>0.94</v>
+        <v>0.96250000000000002</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -7126,7 +7132,7 @@
       </c>
       <c r="C92" s="4">
         <f>potential_preg_untrt!C92*SimParameters!$B$6</f>
-        <v>7.4999999999999997E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D92" s="4">
         <f>potential_preg_untrt!D92</f>
@@ -7134,7 +7140,7 @@
       </c>
       <c r="E92" s="4">
         <f t="shared" si="2"/>
-        <v>0.99250000000000005</v>
+        <v>0.98499999999999999</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -7146,7 +7152,7 @@
       </c>
       <c r="C93" s="4">
         <f>potential_preg_untrt!C93*SimParameters!$B$6</f>
-        <v>7.4999999999999997E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D93" s="4">
         <f>potential_preg_untrt!D93</f>
@@ -7154,7 +7160,7 @@
       </c>
       <c r="E93" s="4">
         <f t="shared" si="2"/>
-        <v>0.99250000000000005</v>
+        <v>0.98499999999999999</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -7186,7 +7192,7 @@
       </c>
       <c r="C95" s="4">
         <f>potential_preg_untrt!C95*SimParameters!$B$6</f>
-        <v>7.4999999999999997E-3</v>
+        <v>3.7499999999999999E-3</v>
       </c>
       <c r="D95" s="4">
         <f>potential_preg_untrt!D95</f>
@@ -7194,7 +7200,7 @@
       </c>
       <c r="E95" s="4">
         <f t="shared" si="2"/>
-        <v>0.99250000000000005</v>
+        <v>0.99624999999999997</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -7206,7 +7212,7 @@
       </c>
       <c r="C96" s="4">
         <f>potential_preg_untrt!C96*SimParameters!$B$6</f>
-        <v>5.6249999999999994E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D96" s="4">
         <f>potential_preg_untrt!D96</f>
@@ -7214,7 +7220,7 @@
       </c>
       <c r="E96" s="4">
         <f t="shared" si="2"/>
-        <v>0.94374999999999998</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -7226,7 +7232,7 @@
       </c>
       <c r="C97" s="4">
         <f>potential_preg_untrt!C97*SimParameters!$B$6</f>
-        <v>5.6249999999999994E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D97" s="4">
         <f>potential_preg_untrt!D97</f>
@@ -7234,7 +7240,7 @@
       </c>
       <c r="E97" s="4">
         <f t="shared" si="2"/>
-        <v>0.94374999999999998</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -7246,7 +7252,7 @@
       </c>
       <c r="C98" s="4">
         <f>potential_preg_untrt!C98*SimParameters!$B$6</f>
-        <v>5.6249999999999994E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D98" s="4">
         <f>potential_preg_untrt!D98</f>
@@ -7254,7 +7260,7 @@
       </c>
       <c r="E98" s="4">
         <f t="shared" si="2"/>
-        <v>0.94374999999999998</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -7266,7 +7272,7 @@
       </c>
       <c r="C99" s="4">
         <f>potential_preg_untrt!C99*SimParameters!$B$6</f>
-        <v>5.6249999999999994E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D99" s="4">
         <f>potential_preg_untrt!D99</f>
@@ -7274,7 +7280,7 @@
       </c>
       <c r="E99" s="4">
         <f t="shared" si="2"/>
-        <v>0.94374999999999998</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -16156,6 +16162,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -16380,16 +16395,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16406,12 +16420,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modified data generation parameters to get reasonable parameters.
</commit_message>
<xml_diff>
--- a/Parameters_Abortion05_Preeclampsia05_EMM.xlsx
+++ b/Parameters_Abortion05_Preeclampsia05_EMM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/preg_cohort_construction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CCC7A5-3E96-5649-B3BD-B0E436C82631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3161507B-8247-8245-B4F0-0014E0CEC35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="13" r:id="rId1"/>
@@ -1254,7 +1254,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1305,12 +1305,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2233,8 +2227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBAD042-1D8C-E044-AB59-2B80CE0D260D}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2267,7 +2261,7 @@
         <v>50</v>
       </c>
       <c r="B4" s="8">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2283,7 +2277,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="8">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2297,7 +2291,7 @@
         <v>50</v>
       </c>
       <c r="B8" s="8">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2313,7 +2307,7 @@
         <v>52</v>
       </c>
       <c r="B10" s="8">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2426,7 +2420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C21"/>
     </sheetView>
   </sheetViews>
@@ -5474,7 +5468,7 @@
       </c>
       <c r="C9" s="2">
         <f>potential_preg_untrt!C9*SimParameters!$B$4</f>
-        <v>3.7500000000000006E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D9" s="2">
         <f>potential_preg_untrt!D9</f>
@@ -5482,7 +5476,7 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>0.96250000000000002</v>
+        <v>0.98750000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -5494,7 +5488,7 @@
       </c>
       <c r="C10" s="2">
         <f>potential_preg_untrt!C10*SimParameters!$B$4</f>
-        <v>1.4999999999999999E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D10" s="2">
         <f>potential_preg_untrt!D10</f>
@@ -5502,7 +5496,7 @@
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0.98499999999999999</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -5514,7 +5508,7 @@
       </c>
       <c r="C11" s="2">
         <f>potential_preg_untrt!C11*SimParameters!$B$4</f>
-        <v>1.4999999999999999E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D11" s="2">
         <f>potential_preg_untrt!D11</f>
@@ -5522,7 +5516,7 @@
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>0.98499999999999999</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -5534,7 +5528,7 @@
       </c>
       <c r="C12" s="2">
         <f>potential_preg_untrt!C12*SimParameters!$B$4</f>
-        <v>7.4999999999999997E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="D12" s="2">
         <f>potential_preg_untrt!D12</f>
@@ -5542,7 +5536,7 @@
       </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>0.99250000000000005</v>
+        <v>0.99750000000000005</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -5554,7 +5548,7 @@
       </c>
       <c r="C13" s="2">
         <f>potential_preg_untrt!C13*SimParameters!$B$4</f>
-        <v>3.7499999999999999E-3</v>
+        <v>1.25E-3</v>
       </c>
       <c r="D13" s="2">
         <f>potential_preg_untrt!D13</f>
@@ -5562,7 +5556,7 @@
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>0.99624999999999997</v>
+        <v>0.99875000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -5574,7 +5568,7 @@
       </c>
       <c r="C14" s="2">
         <f>potential_preg_untrt!C14*SimParameters!$B$4</f>
-        <v>3.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D14" s="2">
         <f>potential_preg_untrt!D14</f>
@@ -5582,7 +5576,7 @@
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>0.997</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -5594,7 +5588,7 @@
       </c>
       <c r="C15" s="2">
         <f>potential_preg_untrt!C15*SimParameters!$B$4</f>
-        <v>3.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D15" s="2">
         <f>potential_preg_untrt!D15</f>
@@ -5602,7 +5596,7 @@
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>0.997</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -5614,7 +5608,7 @@
       </c>
       <c r="C16" s="2">
         <f>potential_preg_untrt!C16*SimParameters!$B$4</f>
-        <v>3.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D16" s="2">
         <f>potential_preg_untrt!D16</f>
@@ -5622,7 +5616,7 @@
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>0.997</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -5634,7 +5628,7 @@
       </c>
       <c r="C17" s="2">
         <f>potential_preg_untrt!C17*SimParameters!$B$4</f>
-        <v>3.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D17" s="2">
         <f>potential_preg_untrt!D17</f>
@@ -5642,7 +5636,7 @@
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>0.997</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -5654,7 +5648,7 @@
       </c>
       <c r="C18" s="2">
         <f>potential_preg_untrt!C18*SimParameters!$B$4</f>
-        <v>6.0000000000000006E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="D18" s="2">
         <f>potential_preg_untrt!D18</f>
@@ -5662,7 +5656,7 @@
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>0.99939999999999996</v>
+        <v>0.99980000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -7112,7 +7106,7 @@
       </c>
       <c r="C91" s="4">
         <f>potential_preg_untrt!C91*SimParameters!$B$6</f>
-        <v>3.7500000000000006E-2</v>
+        <v>0.11250000000000002</v>
       </c>
       <c r="D91" s="4">
         <f>potential_preg_untrt!D91</f>
@@ -7120,7 +7114,7 @@
       </c>
       <c r="E91" s="4">
         <f t="shared" si="2"/>
-        <v>0.96250000000000002</v>
+        <v>0.88749999999999996</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -7132,7 +7126,7 @@
       </c>
       <c r="C92" s="4">
         <f>potential_preg_untrt!C92*SimParameters!$B$6</f>
-        <v>1.4999999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D92" s="4">
         <f>potential_preg_untrt!D92</f>
@@ -7140,7 +7134,7 @@
       </c>
       <c r="E92" s="4">
         <f t="shared" si="2"/>
-        <v>0.98499999999999999</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -7152,7 +7146,7 @@
       </c>
       <c r="C93" s="4">
         <f>potential_preg_untrt!C93*SimParameters!$B$6</f>
-        <v>1.4999999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D93" s="4">
         <f>potential_preg_untrt!D93</f>
@@ -7160,7 +7154,7 @@
       </c>
       <c r="E93" s="4">
         <f t="shared" si="2"/>
-        <v>0.98499999999999999</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -7172,7 +7166,7 @@
       </c>
       <c r="C94" s="4">
         <f>potential_preg_untrt!C94*SimParameters!$B$6</f>
-        <v>7.4999999999999997E-3</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="D94" s="4">
         <f>potential_preg_untrt!D94</f>
@@ -7180,7 +7174,7 @@
       </c>
       <c r="E94" s="4">
         <f t="shared" si="2"/>
-        <v>0.99250000000000005</v>
+        <v>0.97750000000000004</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -7192,7 +7186,7 @@
       </c>
       <c r="C95" s="4">
         <f>potential_preg_untrt!C95*SimParameters!$B$6</f>
-        <v>3.7499999999999999E-3</v>
+        <v>1.125E-2</v>
       </c>
       <c r="D95" s="4">
         <f>potential_preg_untrt!D95</f>
@@ -7200,7 +7194,7 @@
       </c>
       <c r="E95" s="4">
         <f t="shared" si="2"/>
-        <v>0.99624999999999997</v>
+        <v>0.98875000000000002</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -7212,7 +7206,7 @@
       </c>
       <c r="C96" s="4">
         <f>potential_preg_untrt!C96*SimParameters!$B$6</f>
-        <v>3.0000000000000001E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="D96" s="4">
         <f>potential_preg_untrt!D96</f>
@@ -7220,7 +7214,7 @@
       </c>
       <c r="E96" s="4">
         <f t="shared" si="2"/>
-        <v>0.997</v>
+        <v>0.99099999999999999</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -7232,7 +7226,7 @@
       </c>
       <c r="C97" s="4">
         <f>potential_preg_untrt!C97*SimParameters!$B$6</f>
-        <v>3.0000000000000001E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="D97" s="4">
         <f>potential_preg_untrt!D97</f>
@@ -7240,7 +7234,7 @@
       </c>
       <c r="E97" s="4">
         <f t="shared" si="2"/>
-        <v>0.997</v>
+        <v>0.99099999999999999</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -7252,7 +7246,7 @@
       </c>
       <c r="C98" s="4">
         <f>potential_preg_untrt!C98*SimParameters!$B$6</f>
-        <v>3.0000000000000001E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="D98" s="4">
         <f>potential_preg_untrt!D98</f>
@@ -7260,7 +7254,7 @@
       </c>
       <c r="E98" s="4">
         <f t="shared" si="2"/>
-        <v>0.997</v>
+        <v>0.99099999999999999</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -7272,7 +7266,7 @@
       </c>
       <c r="C99" s="4">
         <f>potential_preg_untrt!C99*SimParameters!$B$6</f>
-        <v>3.0000000000000001E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="D99" s="4">
         <f>potential_preg_untrt!D99</f>
@@ -7280,7 +7274,7 @@
       </c>
       <c r="E99" s="4">
         <f t="shared" si="2"/>
-        <v>0.997</v>
+        <v>0.99099999999999999</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -7292,7 +7286,7 @@
       </c>
       <c r="C100" s="4">
         <f>potential_preg_untrt!C100*SimParameters!$B$6</f>
-        <v>6.0000000000000006E-4</v>
+        <v>1.8000000000000002E-3</v>
       </c>
       <c r="D100" s="4">
         <f>potential_preg_untrt!D100</f>
@@ -7300,7 +7294,7 @@
       </c>
       <c r="E100" s="4">
         <f t="shared" si="2"/>
-        <v>0.99939999999999996</v>
+        <v>0.99819999999999998</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -10788,19 +10782,19 @@
       </c>
       <c r="C19" s="2">
         <f>potential_preec_untrt!C19*SimParameters!$B$8</f>
-        <v>3.7499999999999998E-8</v>
+        <v>1.2499999999999999E-8</v>
       </c>
       <c r="D19" s="15">
         <f>LOG(C19/(1-C19))</f>
-        <v>-7.4259687159862375</v>
+        <v>-7.9030899815632623</v>
       </c>
       <c r="E19" s="15">
         <f>D19+LOG(SimParameters!$B$25)</f>
-        <v>-8.1249387203222554</v>
+        <v>-8.602059985899281</v>
       </c>
       <c r="F19" s="15">
         <f>EXP(E19)/(1+EXP(E19))</f>
-        <v>2.9597524485730172E-4</v>
+        <v>1.8369317930722469E-4</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -10812,19 +10806,19 @@
       </c>
       <c r="C20" s="2">
         <f>potential_preec_untrt!C20*SimParameters!$B$8</f>
-        <v>7.4999999999999997E-8</v>
+        <v>2.4999999999999999E-8</v>
       </c>
       <c r="D20" s="15">
         <f t="shared" ref="D20:D83" si="1">LOG(C20/(1-C20))</f>
-        <v>-7.1249387040362127</v>
+        <v>-7.6020599804706004</v>
       </c>
       <c r="E20" s="15">
         <f>D20+LOG(SimParameters!$B$25)</f>
-        <v>-7.8239087083722314</v>
+        <v>-8.3010299848066182</v>
       </c>
       <c r="F20" s="15">
         <f t="shared" ref="F20:F83" si="2">EXP(E20)/(1+EXP(E20))</f>
-        <v>3.9989494482212687E-4</v>
+        <v>2.4819937210653916E-4</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -10836,19 +10830,19 @@
       </c>
       <c r="C21" s="2">
         <f>potential_preec_untrt!C21*SimParameters!$B$8</f>
-        <v>7.4999999999999997E-8</v>
+        <v>2.4999999999999999E-8</v>
       </c>
       <c r="D21" s="15">
         <f t="shared" si="1"/>
-        <v>-7.1249387040362127</v>
+        <v>-7.6020599804706004</v>
       </c>
       <c r="E21" s="15">
         <f>D21+LOG(SimParameters!$B$25)</f>
-        <v>-7.8239087083722314</v>
+        <v>-8.3010299848066182</v>
       </c>
       <c r="F21" s="15">
         <f t="shared" si="2"/>
-        <v>3.9989494482212687E-4</v>
+        <v>2.4819937210653916E-4</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -10860,19 +10854,19 @@
       </c>
       <c r="C22" s="2">
         <f>potential_preec_untrt!C22*SimParameters!$B$8</f>
-        <v>5.9999999999999997E-7</v>
+        <v>1.9999999999999999E-7</v>
       </c>
       <c r="D22" s="15">
         <f t="shared" si="1"/>
-        <v>-6.2218484890395889</v>
+        <v>-6.6989699174771138</v>
       </c>
       <c r="E22" s="15">
         <f>D22+LOG(SimParameters!$B$25)</f>
-        <v>-6.9208184933756076</v>
+        <v>-7.3979399218131325</v>
       </c>
       <c r="F22" s="15">
         <f t="shared" si="2"/>
-        <v>9.8604848777436192E-4</v>
+        <v>6.1213834468519502E-4</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -10884,19 +10878,19 @@
       </c>
       <c r="C23" s="2">
         <f>potential_preec_untrt!C23*SimParameters!$B$8</f>
-        <v>7.5000000000000002E-7</v>
+        <v>2.4999999999999999E-7</v>
       </c>
       <c r="D23" s="15">
         <f t="shared" si="1"/>
-        <v>-6.1249384108873164</v>
+        <v>-6.602059882754328</v>
       </c>
       <c r="E23" s="15">
         <f>D23+LOG(SimParameters!$B$25)</f>
-        <v>-6.8239084152233351</v>
+        <v>-7.3010298870903467</v>
       </c>
       <c r="F23" s="15">
         <f t="shared" si="2"/>
-        <v>1.0862810614033383E-3</v>
+        <v>6.7438829817306268E-4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -10908,19 +10902,19 @@
       </c>
       <c r="C24" s="2">
         <f>potential_preec_untrt!C24*SimParameters!$B$8</f>
-        <v>1.125E-6</v>
+        <v>3.7500000000000001E-7</v>
       </c>
       <c r="D24" s="15">
         <f t="shared" si="1"/>
-        <v>-5.9488469889710514</v>
+        <v>-6.42596856941182</v>
       </c>
       <c r="E24" s="15">
         <f>D24+LOG(SimParameters!$B$25)</f>
-        <v>-6.6478169933070701</v>
+        <v>-7.1249385737478388</v>
       </c>
       <c r="F24" s="15">
         <f t="shared" si="2"/>
-        <v>1.2951704081621727E-3</v>
+        <v>8.0413528941263165E-4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -10932,19 +10926,19 @@
       </c>
       <c r="C25" s="2">
         <f>potential_preec_untrt!C25*SimParameters!$B$8</f>
-        <v>1.125E-6</v>
+        <v>3.7500000000000001E-7</v>
       </c>
       <c r="D25" s="15">
         <f t="shared" si="1"/>
-        <v>-5.9488469889710514</v>
+        <v>-6.42596856941182</v>
       </c>
       <c r="E25" s="15">
         <f>D25+LOG(SimParameters!$B$25)</f>
-        <v>-6.6478169933070701</v>
+        <v>-7.1249385737478388</v>
       </c>
       <c r="F25" s="15">
         <f t="shared" si="2"/>
-        <v>1.2951704081621727E-3</v>
+        <v>8.0413528941263165E-4</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -10956,19 +10950,19 @@
       </c>
       <c r="C26" s="2">
         <f>potential_preec_untrt!C26*SimParameters!$B$8</f>
-        <v>1.5E-6</v>
+        <v>4.9999999999999998E-7</v>
       </c>
       <c r="D26" s="15">
         <f t="shared" si="1"/>
-        <v>-5.8239080895021074</v>
+        <v>-6.3010297785166856</v>
       </c>
       <c r="E26" s="15">
         <f>D26+LOG(SimParameters!$B$25)</f>
-        <v>-6.5228780938381261</v>
+        <v>-6.9999997828527043</v>
       </c>
       <c r="F26" s="15">
         <f t="shared" si="2"/>
-        <v>1.4672777744354514E-3</v>
+        <v>9.1105139205273453E-4</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -10980,19 +10974,19 @@
       </c>
       <c r="C27" s="2">
         <f>potential_preec_untrt!C27*SimParameters!$B$8</f>
-        <v>6.0000000000000002E-6</v>
+        <v>1.9999999999999999E-6</v>
       </c>
       <c r="D27" s="15">
         <f t="shared" si="1"/>
-        <v>-5.2218461438416472</v>
+        <v>-5.6989691357461867</v>
       </c>
       <c r="E27" s="15">
         <f>D27+LOG(SimParameters!$B$25)</f>
-        <v>-5.920816148177666</v>
+        <v>-6.3979391400822054</v>
       </c>
       <c r="F27" s="15">
         <f t="shared" si="2"/>
-        <v>2.6758302716101885E-3</v>
+        <v>1.6622174735925067E-3</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -11004,19 +10998,19 @@
       </c>
       <c r="C28" s="2">
         <f>potential_preec_untrt!C28*SimParameters!$B$8</f>
-        <v>1.5000000000000002E-5</v>
+        <v>5.0000000000000004E-6</v>
       </c>
       <c r="D28" s="15">
         <f t="shared" si="1"/>
-        <v>-4.8239022264782312</v>
+        <v>-5.3010278241861428</v>
       </c>
       <c r="E28" s="15">
         <f>D28+LOG(SimParameters!$B$25)</f>
-        <v>-5.5228722308142499</v>
+        <v>-5.9999978285221616</v>
       </c>
       <c r="F28" s="15">
         <f t="shared" si="2"/>
-        <v>3.9784673043183711E-3</v>
+        <v>2.4726285126108255E-3</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -11028,19 +11022,19 @@
       </c>
       <c r="C29" s="2">
         <f>potential_preec_untrt!C29*SimParameters!$B$8</f>
-        <v>1.5000000000000002E-5</v>
+        <v>5.0000000000000004E-6</v>
       </c>
       <c r="D29" s="15">
         <f t="shared" si="1"/>
-        <v>-4.8239022264782312</v>
+        <v>-5.3010278241861428</v>
       </c>
       <c r="E29" s="15">
         <f>D29+LOG(SimParameters!$B$25)</f>
-        <v>-5.5228722308142499</v>
+        <v>-5.9999978285221616</v>
       </c>
       <c r="F29" s="15">
         <f t="shared" si="2"/>
-        <v>3.9784673043183711E-3</v>
+        <v>2.4726285126108255E-3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -11052,19 +11046,19 @@
       </c>
       <c r="C30" s="2">
         <f>potential_preec_untrt!C30*SimParameters!$B$8</f>
-        <v>3.0000000000000004E-5</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D30" s="15">
         <f t="shared" si="1"/>
-        <v>-4.5228657162504442</v>
+        <v>-4.999995657033466</v>
       </c>
       <c r="E30" s="15">
         <f>D30+LOG(SimParameters!$B$25)</f>
-        <v>-5.2218357205864629</v>
+        <v>-5.6989656613694848</v>
       </c>
       <c r="F30" s="15">
         <f t="shared" si="2"/>
-        <v>5.3684362249790734E-3</v>
+        <v>3.3382468912954684E-3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -11076,19 +11070,19 @@
       </c>
       <c r="C31" s="2">
         <f>potential_preec_untrt!C31*SimParameters!$B$8</f>
-        <v>1.5000000000000001E-4</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="D31" s="15">
         <f t="shared" si="1"/>
-        <v>-3.8238435918857316</v>
+        <v>-4.3010082803970002</v>
       </c>
       <c r="E31" s="15">
         <f>D31+LOG(SimParameters!$B$25)</f>
-        <v>-4.5228135962217504</v>
+        <v>-4.999978284733019</v>
       </c>
       <c r="F31" s="15">
         <f t="shared" si="2"/>
-        <v>1.07417904395706E-2</v>
+        <v>6.692995290156851E-3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -11100,19 +11094,19 @@
       </c>
       <c r="C32" s="2">
         <f>potential_preec_untrt!C32*SimParameters!$B$8</f>
-        <v>4.4999999999999999E-4</v>
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="D32" s="15">
         <f t="shared" si="1"/>
-        <v>-3.3465920097222877</v>
+        <v>-3.8238435918857316</v>
       </c>
       <c r="E32" s="15">
         <f>D32+LOG(SimParameters!$B$25)</f>
-        <v>-4.0455620140583068</v>
+        <v>-4.5228135962217504</v>
       </c>
       <c r="F32" s="15">
         <f t="shared" si="2"/>
-        <v>1.7198888464540228E-2</v>
+        <v>1.07417904395706E-2</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -11124,19 +11118,19 @@
       </c>
       <c r="C33" s="2">
         <f>potential_preec_untrt!C33*SimParameters!$B$8</f>
-        <v>7.5000000000000002E-4</v>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="D33" s="15">
         <f t="shared" si="1"/>
-        <v>-3.1246128935404425</v>
+        <v>-3.6019514041335219</v>
       </c>
       <c r="E33" s="15">
         <f>D33+LOG(SimParameters!$B$25)</f>
-        <v>-3.8235828978764612</v>
+        <v>-4.3009214084695406</v>
       </c>
       <c r="F33" s="15">
         <f t="shared" si="2"/>
-        <v>2.1382188906687895E-2</v>
+        <v>1.3374753588345438E-2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -11148,19 +11142,19 @@
       </c>
       <c r="C34" s="2">
         <f>potential_preec_untrt!C34*SimParameters!$B$8</f>
-        <v>8.9999999999999998E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="D34" s="15">
         <f t="shared" si="1"/>
-        <v>-3.045366449532092</v>
+        <v>-3.5227484373886053</v>
       </c>
       <c r="E34" s="15">
         <f>D34+LOG(SimParameters!$B$25)</f>
-        <v>-3.7443364538681108</v>
+        <v>-4.2217184417246241</v>
       </c>
       <c r="F34" s="15">
         <f t="shared" si="2"/>
-        <v>2.3104857265484235E-2</v>
+        <v>1.4461212173152351E-2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -11172,19 +11166,19 @@
       </c>
       <c r="C35" s="2">
         <f>potential_preec_untrt!C35*SimParameters!$B$8</f>
-        <v>2.2499999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="D35" s="15">
         <f t="shared" si="1"/>
-        <v>-1.637934247956542</v>
+        <v>-2.1216692520434526</v>
       </c>
       <c r="E35" s="15">
         <f>D35+LOG(SimParameters!$B$25)</f>
-        <v>-2.3369042522925607</v>
+        <v>-2.8206392563794713</v>
       </c>
       <c r="F35" s="15">
         <f t="shared" si="2"/>
-        <v>8.8112336716316256E-2</v>
+        <v>5.6219006009956503E-2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -11196,19 +11190,19 @@
       </c>
       <c r="C36" s="2">
         <f>potential_preec_untrt!C36*SimParameters!$B$8</f>
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="D36" s="15">
         <f t="shared" si="1"/>
-        <v>-1.5096504795465824</v>
+        <v>-1.9956351945975499</v>
       </c>
       <c r="E36" s="15">
         <f>D36+LOG(SimParameters!$B$25)</f>
-        <v>-2.2086204838826013</v>
+        <v>-2.6946051989335684</v>
       </c>
       <c r="F36" s="15">
         <f t="shared" si="2"/>
-        <v>9.8979033395933586E-2</v>
+        <v>6.3292442454347467E-2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -11220,19 +11214,19 @@
       </c>
       <c r="C37" s="2">
         <f>potential_preec_untrt!C37*SimParameters!$B$8</f>
-        <v>3.7500000000000006E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D37" s="15">
         <f t="shared" si="1"/>
-        <v>-1.4093694704528195</v>
+        <v>-1.8976270912904414</v>
       </c>
       <c r="E37" s="15">
         <f>D37+LOG(SimParameters!$B$25)</f>
-        <v>-2.1083394747888384</v>
+        <v>-2.5965970956264601</v>
       </c>
       <c r="F37" s="15">
         <f t="shared" si="2"/>
-        <v>0.10828890682965885</v>
+        <v>6.9357746841730766E-2</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -11244,19 +11238,19 @@
       </c>
       <c r="C38" s="2">
         <f>potential_preec_untrt!C38*SimParameters!$B$8</f>
-        <v>4.4999999999999998E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D38" s="15">
         <f t="shared" si="1"/>
-        <v>-1.3267908578084027</v>
+        <v>-1.8173449714419305</v>
       </c>
       <c r="E38" s="15">
         <f>D38+LOG(SimParameters!$B$25)</f>
-        <v>-2.0257608621444216</v>
+        <v>-2.5163149757779495</v>
       </c>
       <c r="F38" s="15">
         <f t="shared" si="2"/>
-        <v>0.11652461810949209</v>
+        <v>7.4722324742277316E-2</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -11268,19 +11262,19 @@
       </c>
       <c r="C39" s="2">
         <f>potential_preec_untrt!C39*SimParameters!$B$8</f>
-        <v>7.5000000000000011E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D39" s="15">
         <f t="shared" si="1"/>
-        <v>-1.0910804693473326</v>
+        <v>-1.5910646070264991</v>
       </c>
       <c r="E39" s="15">
         <f>D39+LOG(SimParameters!$B$25)</f>
-        <v>-1.7900504736833514</v>
+        <v>-2.2900346113625178</v>
       </c>
       <c r="F39" s="15">
         <f t="shared" si="2"/>
-        <v>0.14306653537063813</v>
+        <v>9.1951659960752385E-2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -11292,19 +11286,19 @@
       </c>
       <c r="C40" s="2">
         <f>potential_preec_untrt!C40*SimParameters!$B$8</f>
-        <v>9.7500000000000003E-2</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="D40" s="15">
         <f t="shared" si="1"/>
-        <v>-0.96644259487915873</v>
+        <v>-1.4737676127120747</v>
       </c>
       <c r="E40" s="15">
         <f>D40+LOG(SimParameters!$B$25)</f>
-        <v>-1.6654125992151774</v>
+        <v>-2.1727376170480932</v>
       </c>
       <c r="F40" s="15">
         <f t="shared" si="2"/>
-        <v>0.15903675725368813</v>
+        <v>0.10222551364920184</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -11316,19 +11310,19 @@
       </c>
       <c r="C41" s="2">
         <f>potential_preec_untrt!C41*SimParameters!$B$8</f>
-        <v>0.11249999999999999</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="D41" s="15">
         <f t="shared" si="1"/>
-        <v>-0.89701583927975037</v>
+        <v>-1.4093694704528195</v>
       </c>
       <c r="E41" s="15">
         <f>D41+LOG(SimParameters!$B$25)</f>
-        <v>-1.595985843615769</v>
+        <v>-2.1083394747888384</v>
       </c>
       <c r="F41" s="15">
         <f t="shared" si="2"/>
-        <v>0.16854339655726924</v>
+        <v>0.10828890682965885</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -11340,19 +11334,19 @@
       </c>
       <c r="C42" s="2">
         <f>potential_preec_untrt!C42*SimParameters!$B$8</f>
-        <v>0.15000000000000002</v>
+        <v>0.05</v>
       </c>
       <c r="D42" s="15">
         <f t="shared" si="1"/>
-        <v>-0.75332766665861139</v>
+        <v>-1.2787536009528289</v>
       </c>
       <c r="E42" s="15">
         <f>D42+LOG(SimParameters!$B$25)</f>
-        <v>-1.4522976709946303</v>
+        <v>-1.9777236052888476</v>
       </c>
       <c r="F42" s="15">
         <f t="shared" si="2"/>
-        <v>0.18964820406450195</v>
+        <v>0.12156171214195612</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -12552,19 +12546,19 @@
       </c>
       <c r="C101" s="4">
         <f>potential_preec_untrt!C101*SimParameters!$B$10</f>
-        <v>3.7499999999999998E-8</v>
+        <v>1.1249999999999999E-7</v>
       </c>
       <c r="D101" s="13">
         <f t="shared" ref="D101:D124" si="5">LOG(C101/(1-C101))</f>
-        <v>-7.4259687159862375</v>
+        <v>-6.9488474286944868</v>
       </c>
       <c r="E101" s="13">
         <f>D101+LOG(SimParameters!$B$25)</f>
-        <v>-8.1249387203222554</v>
+        <v>-7.6478174330305055</v>
       </c>
       <c r="F101" s="13">
         <f t="shared" ref="F101:F124" si="6">EXP(E101)/(1+EXP(E101))</f>
-        <v>2.9597524485730172E-4</v>
+        <v>4.7685676102535136E-4</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -12576,19 +12570,19 @@
       </c>
       <c r="C102" s="4">
         <f>potential_preec_untrt!C102*SimParameters!$B$10</f>
-        <v>7.4999999999999997E-8</v>
+        <v>2.2499999999999999E-7</v>
       </c>
       <c r="D102" s="13">
         <f t="shared" si="5"/>
-        <v>-7.1249387040362127</v>
+        <v>-6.6478173841723684</v>
       </c>
       <c r="E102" s="13">
         <f>D102+LOG(SimParameters!$B$25)</f>
-        <v>-7.8239087083722314</v>
+        <v>-7.3467873885083872</v>
       </c>
       <c r="F102" s="13">
         <f t="shared" si="6"/>
-        <v>3.9989494482212687E-4</v>
+        <v>6.442447606890342E-4</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -12600,19 +12594,19 @@
       </c>
       <c r="C103" s="4">
         <f>potential_preec_untrt!C103*SimParameters!$B$10</f>
-        <v>7.4999999999999997E-8</v>
+        <v>2.2499999999999999E-7</v>
       </c>
       <c r="D103" s="13">
         <f t="shared" si="5"/>
-        <v>-7.1249387040362127</v>
+        <v>-6.6478173841723684</v>
       </c>
       <c r="E103" s="13">
         <f>D103+LOG(SimParameters!$B$25)</f>
-        <v>-7.8239087083722314</v>
+        <v>-7.3467873885083872</v>
       </c>
       <c r="F103" s="13">
         <f t="shared" si="6"/>
-        <v>3.9989494482212687E-4</v>
+        <v>6.442447606890342E-4</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -12624,19 +12618,19 @@
       </c>
       <c r="C104" s="4">
         <f>potential_preec_untrt!C104*SimParameters!$B$10</f>
-        <v>5.9999999999999997E-7</v>
+        <v>1.7999999999999999E-6</v>
       </c>
       <c r="D104" s="13">
         <f t="shared" si="5"/>
-        <v>-6.2218484890395889</v>
+        <v>-5.7447267131659228</v>
       </c>
       <c r="E104" s="13">
         <f>D104+LOG(SimParameters!$B$25)</f>
-        <v>-6.9208184933756076</v>
+        <v>-6.4436967175019415</v>
       </c>
       <c r="F104" s="13">
         <f t="shared" si="6"/>
-        <v>9.8604848777436192E-4</v>
+        <v>1.5879903863973272E-3</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -12648,19 +12642,19 @@
       </c>
       <c r="C105" s="4">
         <f>potential_preec_untrt!C105*SimParameters!$B$10</f>
-        <v>7.5000000000000002E-7</v>
+        <v>2.2500000000000001E-6</v>
       </c>
       <c r="D105" s="13">
         <f t="shared" si="5"/>
-        <v>-6.1249384108873164</v>
+        <v>-5.647816504724954</v>
       </c>
       <c r="E105" s="13">
         <f>D105+LOG(SimParameters!$B$25)</f>
-        <v>-6.8239084152233351</v>
+        <v>-6.3467865090609727</v>
       </c>
       <c r="F105" s="13">
         <f t="shared" si="6"/>
-        <v>1.0862810614033383E-3</v>
+        <v>1.7493038944602403E-3</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -12672,19 +12666,19 @@
       </c>
       <c r="C106" s="4">
         <f>potential_preec_untrt!C106*SimParameters!$B$10</f>
-        <v>1.125E-6</v>
+        <v>3.3749999999999999E-6</v>
       </c>
       <c r="D106" s="13">
         <f t="shared" si="5"/>
-        <v>-5.9488469889710514</v>
+        <v>-5.4717247570866068</v>
       </c>
       <c r="E106" s="13">
         <f>D106+LOG(SimParameters!$B$25)</f>
-        <v>-6.6478169933070701</v>
+        <v>-6.1706947614226255</v>
       </c>
       <c r="F106" s="13">
         <f t="shared" si="6"/>
-        <v>1.2951704081621727E-3</v>
+        <v>2.0854255069992778E-3</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -12696,19 +12690,19 @@
       </c>
       <c r="C107" s="4">
         <f>potential_preec_untrt!C107*SimParameters!$B$10</f>
-        <v>1.125E-6</v>
+        <v>3.3749999999999999E-6</v>
       </c>
       <c r="D107" s="13">
         <f t="shared" si="5"/>
-        <v>-5.9488469889710514</v>
+        <v>-5.4717247570866068</v>
       </c>
       <c r="E107" s="13">
         <f>D107+LOG(SimParameters!$B$25)</f>
-        <v>-6.6478169933070701</v>
+        <v>-6.1706947614226255</v>
       </c>
       <c r="F107" s="13">
         <f t="shared" si="6"/>
-        <v>1.2951704081621727E-3</v>
+        <v>2.0854255069992778E-3</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -12720,19 +12714,19 @@
       </c>
       <c r="C108" s="4">
         <f>potential_preec_untrt!C108*SimParameters!$B$10</f>
-        <v>1.5E-6</v>
+        <v>4.5000000000000001E-6</v>
       </c>
       <c r="D108" s="13">
         <f t="shared" si="5"/>
-        <v>-5.8239080895021074</v>
+        <v>-5.3467855318950903</v>
       </c>
       <c r="E108" s="13">
         <f>D108+LOG(SimParameters!$B$25)</f>
-        <v>-6.5228780938381261</v>
+        <v>-6.0457555362311091</v>
       </c>
       <c r="F108" s="13">
         <f t="shared" si="6"/>
-        <v>1.4672777744354514E-3</v>
+        <v>2.3622974721857759E-3</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -12744,19 +12738,19 @@
       </c>
       <c r="C109" s="4">
         <f>potential_preec_untrt!C109*SimParameters!$B$10</f>
-        <v>6.0000000000000002E-6</v>
+        <v>1.8E-5</v>
       </c>
       <c r="D109" s="13">
         <f t="shared" si="5"/>
-        <v>-5.2218461438416472</v>
+        <v>-4.744719677525663</v>
       </c>
       <c r="E109" s="13">
         <f>D109+LOG(SimParameters!$B$25)</f>
-        <v>-5.920816148177666</v>
+        <v>-5.4436896818616818</v>
       </c>
       <c r="F109" s="13">
         <f t="shared" si="6"/>
-        <v>2.6758302716101885E-3</v>
+        <v>4.3048892650325628E-3</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -12768,19 +12762,19 @@
       </c>
       <c r="C110" s="4">
         <f>potential_preec_untrt!C110*SimParameters!$B$10</f>
-        <v>1.5000000000000002E-5</v>
+        <v>4.500000000000001E-5</v>
       </c>
       <c r="D110" s="13">
         <f t="shared" si="5"/>
-        <v>-4.8239022264782312</v>
+        <v>-4.3467679425332344</v>
       </c>
       <c r="E110" s="13">
         <f>D110+LOG(SimParameters!$B$25)</f>
-        <v>-5.5228722308142499</v>
+        <v>-5.0457379468692531</v>
       </c>
       <c r="F110" s="13">
         <f t="shared" si="6"/>
-        <v>3.9784673043183711E-3</v>
+        <v>6.3955424185268344E-3</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -12792,19 +12786,19 @@
       </c>
       <c r="C111" s="4">
         <f>potential_preec_untrt!C111*SimParameters!$B$10</f>
-        <v>1.5000000000000002E-5</v>
+        <v>4.500000000000001E-5</v>
       </c>
       <c r="D111" s="13">
         <f t="shared" si="5"/>
-        <v>-4.8239022264782312</v>
+        <v>-4.3467679425332344</v>
       </c>
       <c r="E111" s="13">
         <f>D111+LOG(SimParameters!$B$25)</f>
-        <v>-5.5228722308142499</v>
+        <v>-5.0457379468692531</v>
       </c>
       <c r="F111" s="13">
         <f t="shared" si="6"/>
-        <v>3.9784673043183711E-3</v>
+        <v>6.3955424185268344E-3</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -12816,19 +12810,19 @@
       </c>
       <c r="C112" s="4">
         <f>potential_preec_untrt!C112*SimParameters!$B$10</f>
-        <v>3.0000000000000004E-5</v>
+        <v>9.0000000000000019E-5</v>
       </c>
       <c r="D112" s="13">
         <f t="shared" si="5"/>
-        <v>-4.5228657162504442</v>
+        <v>-4.0457184022983057</v>
       </c>
       <c r="E112" s="13">
         <f>D112+LOG(SimParameters!$B$25)</f>
-        <v>-5.2218357205864629</v>
+        <v>-4.7446884066343245</v>
       </c>
       <c r="F112" s="13">
         <f t="shared" si="6"/>
-        <v>5.3684362249790734E-3</v>
+        <v>8.6227728415366866E-3</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -12840,19 +12834,19 @@
       </c>
       <c r="C113" s="4">
         <f>potential_preec_untrt!C113*SimParameters!$B$10</f>
-        <v>1.5000000000000001E-4</v>
+        <v>4.5000000000000004E-4</v>
       </c>
       <c r="D113" s="13">
         <f t="shared" si="5"/>
-        <v>-3.8238435918857316</v>
+        <v>-3.3465920097222872</v>
       </c>
       <c r="E113" s="13">
         <f>D113+LOG(SimParameters!$B$25)</f>
-        <v>-4.5228135962217504</v>
+        <v>-4.045562014058306</v>
       </c>
       <c r="F113" s="13">
         <f t="shared" si="6"/>
-        <v>1.07417904395706E-2</v>
+        <v>1.7198888464540246E-2</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -12864,19 +12858,19 @@
       </c>
       <c r="C114" s="4">
         <f>potential_preec_untrt!C114*SimParameters!$B$10</f>
-        <v>4.4999999999999999E-4</v>
+        <v>1.3500000000000001E-3</v>
       </c>
       <c r="D114" s="13">
         <f t="shared" si="5"/>
-        <v>-3.3465920097222877</v>
+        <v>-2.8690795378470413</v>
       </c>
       <c r="E114" s="13">
         <f>D114+LOG(SimParameters!$B$25)</f>
-        <v>-4.0455620140583068</v>
+        <v>-3.56804954218306</v>
       </c>
       <c r="F114" s="13">
         <f t="shared" si="6"/>
-        <v>1.7198888464540228E-2</v>
+        <v>2.7436809082256087E-2</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -12888,19 +12882,19 @@
       </c>
       <c r="C115" s="4">
         <f>potential_preec_untrt!C115*SimParameters!$B$10</f>
-        <v>7.5000000000000002E-4</v>
+        <v>2.2500000000000003E-3</v>
       </c>
       <c r="D115" s="13">
         <f t="shared" si="5"/>
-        <v>-3.1246128935404425</v>
+        <v>-2.6468392183446983</v>
       </c>
       <c r="E115" s="13">
         <f>D115+LOG(SimParameters!$B$25)</f>
-        <v>-3.8235828978764612</v>
+        <v>-3.345809222680717</v>
       </c>
       <c r="F115" s="13">
         <f t="shared" si="6"/>
-        <v>2.1382188906687895E-2</v>
+        <v>3.4032664919811821E-2</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -12912,19 +12906,19 @@
       </c>
       <c r="C116" s="4">
         <f>potential_preec_untrt!C116*SimParameters!$B$10</f>
-        <v>8.9999999999999998E-4</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="D116" s="13">
         <f t="shared" si="5"/>
-        <v>-3.045366449532092</v>
+        <v>-2.5674620548812985</v>
       </c>
       <c r="E116" s="13">
         <f>D116+LOG(SimParameters!$B$25)</f>
-        <v>-3.7443364538681108</v>
+        <v>-3.2664320592173173</v>
       </c>
       <c r="F116" s="13">
         <f t="shared" si="6"/>
-        <v>2.3104857265484235E-2</v>
+        <v>3.6740892761823921E-2</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -12936,19 +12930,19 @@
       </c>
       <c r="C117" s="4">
         <f>potential_preec_untrt!C117*SimParameters!$B$10</f>
-        <v>2.2499999999999999E-2</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="D117" s="13">
         <f t="shared" si="5"/>
-        <v>-1.637934247956542</v>
+        <v>-1.1403450676497002</v>
       </c>
       <c r="E117" s="13">
         <f>D117+LOG(SimParameters!$B$25)</f>
-        <v>-2.3369042522925607</v>
+        <v>-1.839315071985719</v>
       </c>
       <c r="F117" s="13">
         <f t="shared" si="6"/>
-        <v>8.8112336716316256E-2</v>
+        <v>0.13713231794257544</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -12960,19 +12954,19 @@
       </c>
       <c r="C118" s="4">
         <f>potential_preec_untrt!C118*SimParameters!$B$10</f>
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="D118" s="13">
         <f t="shared" si="5"/>
-        <v>-1.5096504795465824</v>
+        <v>-1.0047988828817687</v>
       </c>
       <c r="E118" s="13">
         <f>D118+LOG(SimParameters!$B$25)</f>
-        <v>-2.2086204838826013</v>
+        <v>-1.7037688872177874</v>
       </c>
       <c r="F118" s="13">
         <f t="shared" si="6"/>
-        <v>9.8979033395933586E-2</v>
+        <v>0.15397366753350078</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -12984,19 +12978,19 @@
       </c>
       <c r="C119" s="4">
         <f>potential_preec_untrt!C119*SimParameters!$B$10</f>
-        <v>3.7500000000000006E-2</v>
+        <v>0.11250000000000002</v>
       </c>
       <c r="D119" s="13">
         <f t="shared" si="5"/>
-        <v>-1.4093694704528195</v>
+        <v>-0.89701583927975037</v>
       </c>
       <c r="E119" s="13">
         <f>D119+LOG(SimParameters!$B$25)</f>
-        <v>-2.1083394747888384</v>
+        <v>-1.595985843615769</v>
       </c>
       <c r="F119" s="13">
         <f t="shared" si="6"/>
-        <v>0.10828890682965885</v>
+        <v>0.16854339655726924</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -13008,19 +13002,19 @@
       </c>
       <c r="C120" s="4">
         <f>potential_preec_untrt!C120*SimParameters!$B$10</f>
-        <v>4.4999999999999998E-2</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="D120" s="13">
         <f t="shared" si="5"/>
-        <v>-1.3267908578084027</v>
+        <v>-0.80668233896980812</v>
       </c>
       <c r="E120" s="13">
         <f>D120+LOG(SimParameters!$B$25)</f>
-        <v>-2.0257608621444216</v>
+        <v>-1.5056523433058269</v>
       </c>
       <c r="F120" s="13">
         <f t="shared" si="6"/>
-        <v>0.11652461810949209</v>
+        <v>0.18158400964841215</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -13032,19 +13026,19 @@
       </c>
       <c r="C121" s="4">
         <f>potential_preec_untrt!C121*SimParameters!$B$10</f>
-        <v>7.5000000000000011E-2</v>
+        <v>0.22500000000000003</v>
       </c>
       <c r="D121" s="13">
         <f t="shared" si="5"/>
-        <v>-1.0910804693473326</v>
+        <v>-0.53711918439494766</v>
       </c>
       <c r="E121" s="13">
         <f>D121+LOG(SimParameters!$B$25)</f>
-        <v>-1.7900504736833514</v>
+        <v>-1.2360891887309664</v>
       </c>
       <c r="F121" s="13">
         <f t="shared" si="6"/>
-        <v>0.14306653537063813</v>
+        <v>0.22511745257138824</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -13056,19 +13050,19 @@
       </c>
       <c r="C122" s="4">
         <f>potential_preec_untrt!C122*SimParameters!$B$10</f>
-        <v>9.7500000000000003E-2</v>
+        <v>0.29249999999999998</v>
       </c>
       <c r="D122" s="13">
         <f t="shared" si="5"/>
-        <v>-0.96644259487915873</v>
+        <v>-0.38360057377812867</v>
       </c>
       <c r="E122" s="13">
         <f>D122+LOG(SimParameters!$B$25)</f>
-        <v>-1.6654125992151774</v>
+        <v>-1.0825705781141475</v>
       </c>
       <c r="F122" s="13">
         <f t="shared" si="6"/>
-        <v>0.15903675725368813</v>
+        <v>0.25301986692677358</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -13080,19 +13074,19 @@
       </c>
       <c r="C123" s="4">
         <f>potential_preec_untrt!C123*SimParameters!$B$10</f>
-        <v>0.11249999999999999</v>
+        <v>0.33749999999999997</v>
       </c>
       <c r="D123" s="13">
         <f t="shared" si="5"/>
-        <v>-0.89701583927975037</v>
+        <v>-0.29291210544180185</v>
       </c>
       <c r="E123" s="13">
         <f>D123+LOG(SimParameters!$B$25)</f>
-        <v>-1.595985843615769</v>
+        <v>-0.99188210977782054</v>
       </c>
       <c r="F123" s="13">
         <f t="shared" si="6"/>
-        <v>0.16854339655726924</v>
+        <v>0.27054048605758929</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -13104,19 +13098,19 @@
       </c>
       <c r="C124" s="4">
         <f>potential_preec_untrt!C124*SimParameters!$B$10</f>
-        <v>0.15000000000000002</v>
+        <v>0.45000000000000007</v>
       </c>
       <c r="D124" s="13">
         <f t="shared" si="5"/>
-        <v>-0.75332766665861139</v>
+        <v>-8.7150175718900019E-2</v>
       </c>
       <c r="E124" s="13">
         <f>D124+LOG(SimParameters!$B$25)</f>
-        <v>-1.4522976709946303</v>
+        <v>-0.78612018005491879</v>
       </c>
       <c r="F124" s="13">
         <f t="shared" si="6"/>
-        <v>0.18964820406450195</v>
+        <v>0.3130023484932315</v>
       </c>
     </row>
   </sheetData>
@@ -16162,15 +16156,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -16395,15 +16380,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16420,4 +16406,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating the parameters for the effect of severity on abortion.
</commit_message>
<xml_diff>
--- a/Parameters_Abortion05_Preeclampsia05_EMM.xlsx
+++ b/Parameters_Abortion05_Preeclampsia05_EMM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/preg_cohort_construction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3161507B-8247-8245-B4F0-0014E0CEC35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1350D555-B402-134E-B0B3-69E40FB8FDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
@@ -2228,7 +2228,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2337,7 +2337,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="8">
-        <v>1.75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -3491,7 +3491,7 @@
       </c>
       <c r="C50" s="3">
         <f>C9*SimParameters!B15</f>
-        <v>8.7500000000000008E-2</v>
+        <v>0.1</v>
       </c>
       <c r="D50" s="3">
         <f t="shared" si="1"/>
@@ -3499,7 +3499,7 @@
       </c>
       <c r="E50" s="3">
         <f t="shared" si="2"/>
-        <v>0.91249999999999998</v>
+        <v>0.9</v>
       </c>
       <c r="F50" s="3">
         <f>F9*SimParameters!E15</f>
@@ -3515,7 +3515,7 @@
       </c>
       <c r="C51" s="3">
         <f>C10*SimParameters!B15</f>
-        <v>3.5000000000000003E-2</v>
+        <v>0.04</v>
       </c>
       <c r="D51" s="3">
         <f t="shared" si="1"/>
@@ -3523,7 +3523,7 @@
       </c>
       <c r="E51" s="3">
         <f t="shared" si="2"/>
-        <v>0.96499999999999997</v>
+        <v>0.96</v>
       </c>
       <c r="F51" s="3">
         <f>F10*SimParameters!E15</f>
@@ -3539,7 +3539,7 @@
       </c>
       <c r="C52" s="3">
         <f>C11*SimParameters!B15</f>
-        <v>3.5000000000000003E-2</v>
+        <v>0.04</v>
       </c>
       <c r="D52" s="3">
         <f t="shared" si="1"/>
@@ -3547,7 +3547,7 @@
       </c>
       <c r="E52" s="3">
         <f t="shared" si="2"/>
-        <v>0.96499999999999997</v>
+        <v>0.96</v>
       </c>
       <c r="F52" s="3">
         <f>F11*SimParameters!E15</f>
@@ -3563,7 +3563,7 @@
       </c>
       <c r="C53" s="3">
         <f>C12*SimParameters!B15</f>
-        <v>1.7500000000000002E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D53" s="3">
         <f t="shared" si="1"/>
@@ -3571,7 +3571,7 @@
       </c>
       <c r="E53" s="3">
         <f t="shared" si="2"/>
-        <v>0.98250000000000004</v>
+        <v>0.98</v>
       </c>
       <c r="F53" s="3">
         <f>F12*SimParameters!E15</f>
@@ -3587,7 +3587,7 @@
       </c>
       <c r="C54" s="3">
         <f>C13*SimParameters!B15</f>
-        <v>8.7500000000000008E-3</v>
+        <v>0.01</v>
       </c>
       <c r="D54" s="3">
         <f t="shared" si="1"/>
@@ -3595,7 +3595,7 @@
       </c>
       <c r="E54" s="3">
         <f t="shared" si="2"/>
-        <v>0.99124999999999996</v>
+        <v>0.99</v>
       </c>
       <c r="F54" s="3">
         <f>F13*SimParameters!E15</f>
@@ -3611,7 +3611,7 @@
       </c>
       <c r="C55" s="3">
         <f>C14*SimParameters!B15</f>
-        <v>7.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D55" s="3">
         <f t="shared" si="1"/>
@@ -3619,7 +3619,7 @@
       </c>
       <c r="E55" s="3">
         <f t="shared" si="2"/>
-        <v>0.99299999999999999</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="F55" s="3">
         <f>F14*SimParameters!E15</f>
@@ -3635,7 +3635,7 @@
       </c>
       <c r="C56" s="3">
         <f>C15*SimParameters!B15</f>
-        <v>7.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D56" s="3">
         <f t="shared" si="1"/>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="E56" s="3">
         <f t="shared" si="2"/>
-        <v>0.99299999999999999</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="F56" s="3">
         <f>F15*SimParameters!E15</f>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="C57" s="3">
         <f>C16*SimParameters!B15</f>
-        <v>7.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D57" s="3">
         <f t="shared" si="1"/>
@@ -3667,7 +3667,7 @@
       </c>
       <c r="E57" s="3">
         <f t="shared" si="2"/>
-        <v>0.99299999999999999</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="F57" s="3">
         <f>F16*SimParameters!E15</f>
@@ -3683,7 +3683,7 @@
       </c>
       <c r="C58" s="3">
         <f>C17*SimParameters!B15</f>
-        <v>7.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D58" s="3">
         <f t="shared" si="1"/>
@@ -3691,7 +3691,7 @@
       </c>
       <c r="E58" s="3">
         <f t="shared" si="2"/>
-        <v>0.99299999999999999</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="F58" s="3">
         <f>F17*SimParameters!E15</f>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="C59" s="3">
         <f>C18*SimParameters!B15</f>
-        <v>1.4E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="D59" s="3">
         <f t="shared" si="1"/>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="E59" s="3">
         <f t="shared" si="2"/>
-        <v>0.99860000000000004</v>
+        <v>0.99839999999999995</v>
       </c>
       <c r="F59" s="3">
         <f>F18*SimParameters!E15</f>
@@ -6287,7 +6287,7 @@
       </c>
       <c r="C50" s="3">
         <f>potential_preg_untrt!C50*SimParameters!$B$5</f>
-        <v>4.3750000000000004E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D50" s="3">
         <f>potential_preg_untrt!D50</f>
@@ -6295,7 +6295,7 @@
       </c>
       <c r="E50" s="3">
         <f t="shared" si="1"/>
-        <v>0.95625000000000004</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -6307,7 +6307,7 @@
       </c>
       <c r="C51" s="3">
         <f>potential_preg_untrt!C51*SimParameters!$B$5</f>
-        <v>1.7500000000000002E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D51" s="3">
         <f>potential_preg_untrt!D51</f>
@@ -6315,7 +6315,7 @@
       </c>
       <c r="E51" s="3">
         <f t="shared" si="1"/>
-        <v>0.98250000000000004</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -6327,7 +6327,7 @@
       </c>
       <c r="C52" s="3">
         <f>potential_preg_untrt!C52*SimParameters!$B$5</f>
-        <v>1.7500000000000002E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D52" s="3">
         <f>potential_preg_untrt!D52</f>
@@ -6335,7 +6335,7 @@
       </c>
       <c r="E52" s="3">
         <f t="shared" si="1"/>
-        <v>0.98250000000000004</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -6347,7 +6347,7 @@
       </c>
       <c r="C53" s="3">
         <f>potential_preg_untrt!C53*SimParameters!$B$5</f>
-        <v>8.7500000000000008E-3</v>
+        <v>0.01</v>
       </c>
       <c r="D53" s="3">
         <f>potential_preg_untrt!D53</f>
@@ -6355,7 +6355,7 @@
       </c>
       <c r="E53" s="3">
         <f t="shared" si="1"/>
-        <v>0.99124999999999996</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -6367,7 +6367,7 @@
       </c>
       <c r="C54" s="3">
         <f>potential_preg_untrt!C54*SimParameters!$B$5</f>
-        <v>4.3750000000000004E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D54" s="3">
         <f>potential_preg_untrt!D54</f>
@@ -6375,7 +6375,7 @@
       </c>
       <c r="E54" s="3">
         <f t="shared" si="1"/>
-        <v>0.99562499999999998</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -6387,7 +6387,7 @@
       </c>
       <c r="C55" s="3">
         <f>potential_preg_untrt!C55*SimParameters!$B$5</f>
-        <v>3.5000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D55" s="3">
         <f>potential_preg_untrt!D55</f>
@@ -6395,7 +6395,7 @@
       </c>
       <c r="E55" s="3">
         <f t="shared" si="1"/>
-        <v>0.99650000000000005</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -6407,7 +6407,7 @@
       </c>
       <c r="C56" s="3">
         <f>potential_preg_untrt!C56*SimParameters!$B$5</f>
-        <v>3.5000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D56" s="3">
         <f>potential_preg_untrt!D56</f>
@@ -6415,7 +6415,7 @@
       </c>
       <c r="E56" s="3">
         <f t="shared" si="1"/>
-        <v>0.99650000000000005</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -6427,7 +6427,7 @@
       </c>
       <c r="C57" s="3">
         <f>potential_preg_untrt!C57*SimParameters!$B$5</f>
-        <v>3.5000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D57" s="3">
         <f>potential_preg_untrt!D57</f>
@@ -6435,7 +6435,7 @@
       </c>
       <c r="E57" s="3">
         <f t="shared" si="1"/>
-        <v>0.99650000000000005</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -6447,7 +6447,7 @@
       </c>
       <c r="C58" s="3">
         <f>potential_preg_untrt!C58*SimParameters!$B$5</f>
-        <v>3.5000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D58" s="3">
         <f>potential_preg_untrt!D58</f>
@@ -6455,7 +6455,7 @@
       </c>
       <c r="E58" s="3">
         <f t="shared" si="1"/>
-        <v>0.99650000000000005</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -6467,7 +6467,7 @@
       </c>
       <c r="C59" s="3">
         <f>potential_preg_untrt!C59*SimParameters!$B$5</f>
-        <v>6.9999999999999999E-4</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D59" s="3">
         <f>potential_preg_untrt!D59</f>
@@ -6475,7 +6475,7 @@
       </c>
       <c r="E59" s="3">
         <f t="shared" si="1"/>
-        <v>0.99929999999999997</v>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Explored different data generating parameters to get expected distributions.
</commit_message>
<xml_diff>
--- a/Parameters_Abortion05_Preeclampsia05_EMM.xlsx
+++ b/Parameters_Abortion05_Preeclampsia05_EMM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/preg_cohort_construction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1350D555-B402-134E-B0B3-69E40FB8FDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB823214-4315-7F4F-A030-BC9CA3922F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
@@ -2228,7 +2228,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2261,7 +2261,7 @@
         <v>50</v>
       </c>
       <c r="B4" s="8">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2291,7 +2291,7 @@
         <v>50</v>
       </c>
       <c r="B8" s="8">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -5468,7 +5468,7 @@
       </c>
       <c r="C9" s="2">
         <f>potential_preg_untrt!C9*SimParameters!$B$4</f>
-        <v>1.2500000000000001E-2</v>
+        <v>5.000000000000001E-3</v>
       </c>
       <c r="D9" s="2">
         <f>potential_preg_untrt!D9</f>
@@ -5476,7 +5476,7 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>0.98750000000000004</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -5488,7 +5488,7 @@
       </c>
       <c r="C10" s="2">
         <f>potential_preg_untrt!C10*SimParameters!$B$4</f>
-        <v>5.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="D10" s="2">
         <f>potential_preg_untrt!D10</f>
@@ -5496,7 +5496,7 @@
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0.995</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -5508,7 +5508,7 @@
       </c>
       <c r="C11" s="2">
         <f>potential_preg_untrt!C11*SimParameters!$B$4</f>
-        <v>5.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="D11" s="2">
         <f>potential_preg_untrt!D11</f>
@@ -5516,7 +5516,7 @@
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>0.995</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -5528,7 +5528,7 @@
       </c>
       <c r="C12" s="2">
         <f>potential_preg_untrt!C12*SimParameters!$B$4</f>
-        <v>2.5000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D12" s="2">
         <f>potential_preg_untrt!D12</f>
@@ -5536,7 +5536,7 @@
       </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>0.99750000000000005</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -5548,7 +5548,7 @@
       </c>
       <c r="C13" s="2">
         <f>potential_preg_untrt!C13*SimParameters!$B$4</f>
-        <v>1.25E-3</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="D13" s="2">
         <f>potential_preg_untrt!D13</f>
@@ -5556,7 +5556,7 @@
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>0.99875000000000003</v>
+        <v>0.99950000000000006</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -5568,7 +5568,7 @@
       </c>
       <c r="C14" s="2">
         <f>potential_preg_untrt!C14*SimParameters!$B$4</f>
-        <v>1E-3</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="D14" s="2">
         <f>potential_preg_untrt!D14</f>
@@ -5576,7 +5576,7 @@
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>0.999</v>
+        <v>0.99960000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -5588,7 +5588,7 @@
       </c>
       <c r="C15" s="2">
         <f>potential_preg_untrt!C15*SimParameters!$B$4</f>
-        <v>1E-3</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="D15" s="2">
         <f>potential_preg_untrt!D15</f>
@@ -5596,7 +5596,7 @@
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>0.999</v>
+        <v>0.99960000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -5608,7 +5608,7 @@
       </c>
       <c r="C16" s="2">
         <f>potential_preg_untrt!C16*SimParameters!$B$4</f>
-        <v>1E-3</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="D16" s="2">
         <f>potential_preg_untrt!D16</f>
@@ -5616,7 +5616,7 @@
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>0.999</v>
+        <v>0.99960000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -5628,7 +5628,7 @@
       </c>
       <c r="C17" s="2">
         <f>potential_preg_untrt!C17*SimParameters!$B$4</f>
-        <v>1E-3</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="D17" s="2">
         <f>potential_preg_untrt!D17</f>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>0.999</v>
+        <v>0.99960000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -5648,7 +5648,7 @@
       </c>
       <c r="C18" s="2">
         <f>potential_preg_untrt!C18*SimParameters!$B$4</f>
-        <v>2.0000000000000001E-4</v>
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="D18" s="2">
         <f>potential_preg_untrt!D18</f>
@@ -5656,7 +5656,7 @@
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>0.99980000000000002</v>
+        <v>0.99992000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -10782,19 +10782,19 @@
       </c>
       <c r="C19" s="2">
         <f>potential_preec_untrt!C19*SimParameters!$B$8</f>
-        <v>1.2499999999999999E-8</v>
+        <v>5.0000000000000001E-9</v>
       </c>
       <c r="D19" s="15">
         <f>LOG(C19/(1-C19))</f>
-        <v>-7.9030899815632623</v>
+        <v>-8.3010299934925094</v>
       </c>
       <c r="E19" s="15">
         <f>D19+LOG(SimParameters!$B$25)</f>
-        <v>-8.602059985899281</v>
+        <v>-8.9999999978285281</v>
       </c>
       <c r="F19" s="15">
         <f>EXP(E19)/(1+EXP(E19))</f>
-        <v>1.8369317930722469E-4</v>
+        <v>1.2339457625414648E-4</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -10806,19 +10806,19 @@
       </c>
       <c r="C20" s="2">
         <f>potential_preec_untrt!C20*SimParameters!$B$8</f>
-        <v>2.4999999999999999E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="D20" s="15">
         <f t="shared" ref="D20:D83" si="1">LOG(C20/(1-C20))</f>
-        <v>-7.6020599804706004</v>
+        <v>-7.9999999956570553</v>
       </c>
       <c r="E20" s="15">
         <f>D20+LOG(SimParameters!$B$25)</f>
-        <v>-8.3010299848066182</v>
+        <v>-8.698969999993075</v>
       </c>
       <c r="F20" s="15">
         <f t="shared" ref="F20:F83" si="2">EXP(E20)/(1+EXP(E20))</f>
-        <v>2.4819937210653916E-4</v>
+        <v>1.6672967934826437E-4</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -10830,19 +10830,19 @@
       </c>
       <c r="C21" s="2">
         <f>potential_preec_untrt!C21*SimParameters!$B$8</f>
-        <v>2.4999999999999999E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="D21" s="15">
         <f t="shared" si="1"/>
-        <v>-7.6020599804706004</v>
+        <v>-7.9999999956570553</v>
       </c>
       <c r="E21" s="15">
         <f>D21+LOG(SimParameters!$B$25)</f>
-        <v>-8.3010299848066182</v>
+        <v>-8.698969999993075</v>
       </c>
       <c r="F21" s="15">
         <f t="shared" si="2"/>
-        <v>2.4819937210653916E-4</v>
+        <v>1.6672967934826437E-4</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -10854,19 +10854,19 @@
       </c>
       <c r="C22" s="2">
         <f>potential_preec_untrt!C22*SimParameters!$B$8</f>
-        <v>1.9999999999999999E-7</v>
+        <v>8.0000000000000002E-8</v>
       </c>
       <c r="D22" s="15">
         <f t="shared" si="1"/>
-        <v>-6.6989699174771138</v>
+        <v>-7.0969099782644962</v>
       </c>
       <c r="E22" s="15">
         <f>D22+LOG(SimParameters!$B$25)</f>
-        <v>-7.3979399218131325</v>
+        <v>-7.795879982600515</v>
       </c>
       <c r="F22" s="15">
         <f t="shared" si="2"/>
-        <v>6.1213834468519502E-4</v>
+        <v>4.1125737432160908E-4</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -10878,19 +10878,19 @@
       </c>
       <c r="C23" s="2">
         <f>potential_preec_untrt!C23*SimParameters!$B$8</f>
-        <v>2.4999999999999999E-7</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="D23" s="15">
         <f t="shared" si="1"/>
-        <v>-6.602059882754328</v>
+        <v>-6.9999999565705497</v>
       </c>
       <c r="E23" s="15">
         <f>D23+LOG(SimParameters!$B$25)</f>
-        <v>-7.3010298870903467</v>
+        <v>-7.6989699609065685</v>
       </c>
       <c r="F23" s="15">
         <f t="shared" si="2"/>
-        <v>6.7438829817306268E-4</v>
+        <v>4.5308847067208077E-4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -10902,19 +10902,19 @@
       </c>
       <c r="C24" s="2">
         <f>potential_preec_untrt!C24*SimParameters!$B$8</f>
-        <v>3.7500000000000001E-7</v>
+        <v>1.5000000000000002E-7</v>
       </c>
       <c r="D24" s="15">
         <f t="shared" si="1"/>
-        <v>-6.42596856941182</v>
+        <v>-6.8239086758001415</v>
       </c>
       <c r="E24" s="15">
         <f>D24+LOG(SimParameters!$B$25)</f>
-        <v>-7.1249385737478388</v>
+        <v>-7.5228786801361602</v>
       </c>
       <c r="F24" s="15">
         <f t="shared" si="2"/>
-        <v>8.0413528941263165E-4</v>
+        <v>5.4028212114853597E-4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -10926,19 +10926,19 @@
       </c>
       <c r="C25" s="2">
         <f>potential_preec_untrt!C25*SimParameters!$B$8</f>
-        <v>3.7500000000000001E-7</v>
+        <v>1.5000000000000002E-7</v>
       </c>
       <c r="D25" s="15">
         <f t="shared" si="1"/>
-        <v>-6.42596856941182</v>
+        <v>-6.8239086758001415</v>
       </c>
       <c r="E25" s="15">
         <f>D25+LOG(SimParameters!$B$25)</f>
-        <v>-7.1249385737478388</v>
+        <v>-7.5228786801361602</v>
       </c>
       <c r="F25" s="15">
         <f t="shared" si="2"/>
-        <v>8.0413528941263165E-4</v>
+        <v>5.4028212114853597E-4</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -10950,19 +10950,19 @@
       </c>
       <c r="C26" s="2">
         <f>potential_preec_untrt!C26*SimParameters!$B$8</f>
-        <v>4.9999999999999998E-7</v>
+        <v>1.9999999999999999E-7</v>
       </c>
       <c r="D26" s="15">
         <f t="shared" si="1"/>
-        <v>-6.3010297785166856</v>
+        <v>-6.6989699174771138</v>
       </c>
       <c r="E26" s="15">
         <f>D26+LOG(SimParameters!$B$25)</f>
-        <v>-6.9999997828527043</v>
+        <v>-7.3979399218131325</v>
       </c>
       <c r="F26" s="15">
         <f t="shared" si="2"/>
-        <v>9.1105139205273453E-4</v>
+        <v>6.1213834468519502E-4</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -10974,19 +10974,19 @@
       </c>
       <c r="C27" s="2">
         <f>potential_preec_untrt!C27*SimParameters!$B$8</f>
-        <v>1.9999999999999999E-6</v>
+        <v>7.9999999999999996E-7</v>
       </c>
       <c r="D27" s="15">
         <f t="shared" si="1"/>
-        <v>-5.6989691357461867</v>
+        <v>-6.0969096655723316</v>
       </c>
       <c r="E27" s="15">
         <f>D27+LOG(SimParameters!$B$25)</f>
-        <v>-6.3979391400822054</v>
+        <v>-6.7958796699083504</v>
       </c>
       <c r="F27" s="15">
         <f t="shared" si="2"/>
-        <v>1.6622174735925067E-3</v>
+        <v>1.1171243738873006E-3</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -10998,19 +10998,19 @@
       </c>
       <c r="C28" s="2">
         <f>potential_preec_untrt!C28*SimParameters!$B$8</f>
-        <v>5.0000000000000004E-6</v>
+        <v>2.0000000000000003E-6</v>
       </c>
       <c r="D28" s="15">
         <f t="shared" si="1"/>
-        <v>-5.3010278241861428</v>
+        <v>-5.6989691357461867</v>
       </c>
       <c r="E28" s="15">
         <f>D28+LOG(SimParameters!$B$25)</f>
-        <v>-5.9999978285221616</v>
+        <v>-6.3979391400822054</v>
       </c>
       <c r="F28" s="15">
         <f t="shared" si="2"/>
-        <v>2.4726285126108255E-3</v>
+        <v>1.6622174735925067E-3</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -11022,19 +11022,19 @@
       </c>
       <c r="C29" s="2">
         <f>potential_preec_untrt!C29*SimParameters!$B$8</f>
-        <v>5.0000000000000004E-6</v>
+        <v>2.0000000000000003E-6</v>
       </c>
       <c r="D29" s="15">
         <f t="shared" si="1"/>
-        <v>-5.3010278241861428</v>
+        <v>-5.6989691357461867</v>
       </c>
       <c r="E29" s="15">
         <f>D29+LOG(SimParameters!$B$25)</f>
-        <v>-5.9999978285221616</v>
+        <v>-6.3979391400822054</v>
       </c>
       <c r="F29" s="15">
         <f t="shared" si="2"/>
-        <v>2.4726285126108255E-3</v>
+        <v>1.6622174735925067E-3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -11046,19 +11046,19 @@
       </c>
       <c r="C30" s="2">
         <f>potential_preec_untrt!C30*SimParameters!$B$8</f>
-        <v>1.0000000000000001E-5</v>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="D30" s="15">
         <f t="shared" si="1"/>
-        <v>-4.999995657033466</v>
+        <v>-5.3979382714906352</v>
       </c>
       <c r="E30" s="15">
         <f>D30+LOG(SimParameters!$B$25)</f>
-        <v>-5.6989656613694848</v>
+        <v>-6.096908275826654</v>
       </c>
       <c r="F30" s="15">
         <f t="shared" si="2"/>
-        <v>3.3382468912954684E-3</v>
+        <v>2.2447624830839253E-3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -11070,19 +11070,19 @@
       </c>
       <c r="C31" s="2">
         <f>potential_preec_untrt!C31*SimParameters!$B$8</f>
-        <v>5.0000000000000002E-5</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="D31" s="15">
         <f t="shared" si="1"/>
-        <v>-4.3010082803970002</v>
+        <v>-4.6989613183595207</v>
       </c>
       <c r="E31" s="15">
         <f>D31+LOG(SimParameters!$B$25)</f>
-        <v>-4.999978284733019</v>
+        <v>-5.3979313226955394</v>
       </c>
       <c r="F31" s="15">
         <f t="shared" si="2"/>
-        <v>6.692995290156851E-3</v>
+        <v>4.5055421756067648E-3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -11094,19 +11094,19 @@
       </c>
       <c r="C32" s="2">
         <f>potential_preec_untrt!C32*SimParameters!$B$8</f>
-        <v>1.4999999999999999E-4</v>
+        <v>5.9999999999999995E-5</v>
       </c>
       <c r="D32" s="15">
         <f t="shared" si="1"/>
-        <v>-3.8238435918857316</v>
+        <v>-4.2218226911656807</v>
       </c>
       <c r="E32" s="15">
         <f>D32+LOG(SimParameters!$B$25)</f>
-        <v>-4.5228135962217504</v>
+        <v>-4.9207926955016994</v>
       </c>
       <c r="F32" s="15">
         <f t="shared" si="2"/>
-        <v>1.07417904395706E-2</v>
+        <v>7.2405393839679588E-3</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -11118,19 +11118,19 @@
       </c>
       <c r="C33" s="2">
         <f>potential_preec_untrt!C33*SimParameters!$B$8</f>
-        <v>2.5000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="D33" s="15">
         <f t="shared" si="1"/>
-        <v>-3.6019514041335219</v>
+        <v>-3.9999565683801923</v>
       </c>
       <c r="E33" s="15">
         <f>D33+LOG(SimParameters!$B$25)</f>
-        <v>-4.3009214084695406</v>
+        <v>-4.6989265727162106</v>
       </c>
       <c r="F33" s="15">
         <f t="shared" si="2"/>
-        <v>1.3374753588345438E-2</v>
+        <v>9.0228916237305098E-3</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -11142,19 +11142,19 @@
       </c>
       <c r="C34" s="2">
         <f>potential_preec_untrt!C34*SimParameters!$B$8</f>
-        <v>2.9999999999999997E-4</v>
+        <v>1.1999999999999999E-4</v>
       </c>
       <c r="D34" s="15">
         <f t="shared" si="1"/>
-        <v>-3.5227484373886053</v>
+        <v>-3.9207666354873765</v>
       </c>
       <c r="E34" s="15">
         <f>D34+LOG(SimParameters!$B$25)</f>
-        <v>-4.2217184417246241</v>
+        <v>-4.6197366398233957</v>
       </c>
       <c r="F34" s="15">
         <f t="shared" si="2"/>
-        <v>1.4461212173152351E-2</v>
+        <v>9.7592104003560946E-3</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -11166,19 +11166,19 @@
       </c>
       <c r="C35" s="2">
         <f>potential_preec_untrt!C35*SimParameters!$B$8</f>
-        <v>7.4999999999999997E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D35" s="15">
         <f t="shared" si="1"/>
-        <v>-2.1216692520434526</v>
+        <v>-2.5215739035919933</v>
       </c>
       <c r="E35" s="15">
         <f>D35+LOG(SimParameters!$B$25)</f>
-        <v>-2.8206392563794713</v>
+        <v>-3.220543907928012</v>
       </c>
       <c r="F35" s="15">
         <f t="shared" si="2"/>
-        <v>5.6219006009956503E-2</v>
+        <v>3.8399896470773139E-2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -11190,19 +11190,19 @@
       </c>
       <c r="C36" s="2">
         <f>potential_preec_untrt!C36*SimParameters!$B$8</f>
-        <v>0.01</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D36" s="15">
         <f t="shared" si="1"/>
-        <v>-1.9956351945975499</v>
+        <v>-2.3961993470957363</v>
       </c>
       <c r="E36" s="15">
         <f>D36+LOG(SimParameters!$B$25)</f>
-        <v>-2.6946051989335684</v>
+        <v>-3.0951693514317551</v>
       </c>
       <c r="F36" s="15">
         <f t="shared" si="2"/>
-        <v>6.3292442454347467E-2</v>
+        <v>4.3306954825074587E-2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -11214,19 +11214,19 @@
       </c>
       <c r="C37" s="2">
         <f>potential_preec_untrt!C37*SimParameters!$B$8</f>
-        <v>1.2500000000000001E-2</v>
+        <v>5.000000000000001E-3</v>
       </c>
       <c r="D37" s="15">
         <f t="shared" si="1"/>
-        <v>-1.8976270912904414</v>
+        <v>-2.2988530764097064</v>
       </c>
       <c r="E37" s="15">
         <f>D37+LOG(SimParameters!$B$25)</f>
-        <v>-2.5965970956264601</v>
+        <v>-2.9978230807457251</v>
       </c>
       <c r="F37" s="15">
         <f t="shared" si="2"/>
-        <v>6.9357746841730766E-2</v>
+        <v>4.7524316066742768E-2</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -11238,19 +11238,19 @@
       </c>
       <c r="C38" s="2">
         <f>potential_preec_untrt!C38*SimParameters!$B$8</f>
-        <v>1.4999999999999999E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D38" s="15">
         <f t="shared" si="1"/>
-        <v>-1.8173449714419305</v>
+        <v>-2.2192351340136698</v>
       </c>
       <c r="E38" s="15">
         <f>D38+LOG(SimParameters!$B$25)</f>
-        <v>-2.5163149757779495</v>
+        <v>-2.9182051383496885</v>
       </c>
       <c r="F38" s="15">
         <f t="shared" si="2"/>
-        <v>7.4722324742277316E-2</v>
+        <v>5.1260920579713251E-2</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -11262,19 +11262,19 @@
       </c>
       <c r="C39" s="2">
         <f>potential_preec_untrt!C39*SimParameters!$B$8</f>
-        <v>2.5000000000000001E-2</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="D39" s="15">
         <f t="shared" si="1"/>
-        <v>-1.5910646070264991</v>
+        <v>-1.9956351945975499</v>
       </c>
       <c r="E39" s="15">
         <f>D39+LOG(SimParameters!$B$25)</f>
-        <v>-2.2900346113625178</v>
+        <v>-2.6946051989335684</v>
       </c>
       <c r="F39" s="15">
         <f t="shared" si="2"/>
-        <v>9.1951659960752385E-2</v>
+        <v>6.3292442454347467E-2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -11286,19 +11286,19 @@
       </c>
       <c r="C40" s="2">
         <f>potential_preec_untrt!C40*SimParameters!$B$8</f>
-        <v>3.2500000000000001E-2</v>
+        <v>1.3000000000000001E-2</v>
       </c>
       <c r="D40" s="15">
         <f t="shared" si="1"/>
-        <v>-1.4737676127120747</v>
+        <v>-1.8803738003627999</v>
       </c>
       <c r="E40" s="15">
         <f>D40+LOG(SimParameters!$B$25)</f>
-        <v>-2.1727376170480932</v>
+        <v>-2.5793438046988184</v>
       </c>
       <c r="F40" s="15">
         <f t="shared" si="2"/>
-        <v>0.10222551364920184</v>
+        <v>7.0479707653854196E-2</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -11310,19 +11310,19 @@
       </c>
       <c r="C41" s="2">
         <f>potential_preec_untrt!C41*SimParameters!$B$8</f>
-        <v>3.7499999999999999E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D41" s="15">
         <f t="shared" si="1"/>
-        <v>-1.4093694704528195</v>
+        <v>-1.8173449714419305</v>
       </c>
       <c r="E41" s="15">
         <f>D41+LOG(SimParameters!$B$25)</f>
-        <v>-2.1083394747888384</v>
+        <v>-2.5163149757779495</v>
       </c>
       <c r="F41" s="15">
         <f t="shared" si="2"/>
-        <v>0.10828890682965885</v>
+        <v>7.4722324742277316E-2</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -11334,19 +11334,19 @@
       </c>
       <c r="C42" s="2">
         <f>potential_preec_untrt!C42*SimParameters!$B$8</f>
-        <v>0.05</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="D42" s="15">
         <f t="shared" si="1"/>
-        <v>-1.2787536009528289</v>
+        <v>-1.6901960800285136</v>
       </c>
       <c r="E42" s="15">
         <f>D42+LOG(SimParameters!$B$25)</f>
-        <v>-1.9777236052888476</v>
+        <v>-2.3891660843645326</v>
       </c>
       <c r="F42" s="15">
         <f t="shared" si="2"/>
-        <v>0.12156171214195612</v>
+        <v>8.4002576233824053E-2</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -16156,6 +16156,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -16380,16 +16389,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16406,12 +16414,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Made the EMM stronger.
</commit_message>
<xml_diff>
--- a/Parameters_Abortion05_Preeclampsia05_EMM.xlsx
+++ b/Parameters_Abortion05_Preeclampsia05_EMM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/preg_cohort_construction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB823214-4315-7F4F-A030-BC9CA3922F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C6DE78-AE8F-BD4B-B5C6-3572ED8AE4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
@@ -2228,7 +2228,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2277,7 +2277,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="8">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2307,7 +2307,7 @@
         <v>52</v>
       </c>
       <c r="B10" s="8">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -7106,7 +7106,7 @@
       </c>
       <c r="C91" s="4">
         <f>potential_preg_untrt!C91*SimParameters!$B$6</f>
-        <v>0.11250000000000002</v>
+        <v>0.12000000000000002</v>
       </c>
       <c r="D91" s="4">
         <f>potential_preg_untrt!D91</f>
@@ -7114,7 +7114,7 @@
       </c>
       <c r="E91" s="4">
         <f t="shared" si="2"/>
-        <v>0.88749999999999996</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -7126,7 +7126,7 @@
       </c>
       <c r="C92" s="4">
         <f>potential_preg_untrt!C92*SimParameters!$B$6</f>
-        <v>4.4999999999999998E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D92" s="4">
         <f>potential_preg_untrt!D92</f>
@@ -7134,7 +7134,7 @@
       </c>
       <c r="E92" s="4">
         <f t="shared" si="2"/>
-        <v>0.95499999999999996</v>
+        <v>0.95199999999999996</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -7146,7 +7146,7 @@
       </c>
       <c r="C93" s="4">
         <f>potential_preg_untrt!C93*SimParameters!$B$6</f>
-        <v>4.4999999999999998E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D93" s="4">
         <f>potential_preg_untrt!D93</f>
@@ -7154,7 +7154,7 @@
       </c>
       <c r="E93" s="4">
         <f t="shared" si="2"/>
-        <v>0.95499999999999996</v>
+        <v>0.95199999999999996</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -7166,7 +7166,7 @@
       </c>
       <c r="C94" s="4">
         <f>potential_preg_untrt!C94*SimParameters!$B$6</f>
-        <v>2.2499999999999999E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="D94" s="4">
         <f>potential_preg_untrt!D94</f>
@@ -7174,7 +7174,7 @@
       </c>
       <c r="E94" s="4">
         <f t="shared" si="2"/>
-        <v>0.97750000000000004</v>
+        <v>0.97599999999999998</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -7186,7 +7186,7 @@
       </c>
       <c r="C95" s="4">
         <f>potential_preg_untrt!C95*SimParameters!$B$6</f>
-        <v>1.125E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D95" s="4">
         <f>potential_preg_untrt!D95</f>
@@ -7194,7 +7194,7 @@
       </c>
       <c r="E95" s="4">
         <f t="shared" si="2"/>
-        <v>0.98875000000000002</v>
+        <v>0.98799999999999999</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -7206,7 +7206,7 @@
       </c>
       <c r="C96" s="4">
         <f>potential_preg_untrt!C96*SimParameters!$B$6</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.6000000000000009E-3</v>
       </c>
       <c r="D96" s="4">
         <f>potential_preg_untrt!D96</f>
@@ -7214,7 +7214,7 @@
       </c>
       <c r="E96" s="4">
         <f t="shared" si="2"/>
-        <v>0.99099999999999999</v>
+        <v>0.99039999999999995</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -7226,7 +7226,7 @@
       </c>
       <c r="C97" s="4">
         <f>potential_preg_untrt!C97*SimParameters!$B$6</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.6000000000000009E-3</v>
       </c>
       <c r="D97" s="4">
         <f>potential_preg_untrt!D97</f>
@@ -7234,7 +7234,7 @@
       </c>
       <c r="E97" s="4">
         <f t="shared" si="2"/>
-        <v>0.99099999999999999</v>
+        <v>0.99039999999999995</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -7246,7 +7246,7 @@
       </c>
       <c r="C98" s="4">
         <f>potential_preg_untrt!C98*SimParameters!$B$6</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.6000000000000009E-3</v>
       </c>
       <c r="D98" s="4">
         <f>potential_preg_untrt!D98</f>
@@ -7254,7 +7254,7 @@
       </c>
       <c r="E98" s="4">
         <f t="shared" si="2"/>
-        <v>0.99099999999999999</v>
+        <v>0.99039999999999995</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -7266,7 +7266,7 @@
       </c>
       <c r="C99" s="4">
         <f>potential_preg_untrt!C99*SimParameters!$B$6</f>
-        <v>9.0000000000000011E-3</v>
+        <v>9.6000000000000009E-3</v>
       </c>
       <c r="D99" s="4">
         <f>potential_preg_untrt!D99</f>
@@ -7274,7 +7274,7 @@
       </c>
       <c r="E99" s="4">
         <f t="shared" si="2"/>
-        <v>0.99099999999999999</v>
+        <v>0.99039999999999995</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -7286,7 +7286,7 @@
       </c>
       <c r="C100" s="4">
         <f>potential_preg_untrt!C100*SimParameters!$B$6</f>
-        <v>1.8000000000000002E-3</v>
+        <v>1.9200000000000003E-3</v>
       </c>
       <c r="D100" s="4">
         <f>potential_preg_untrt!D100</f>
@@ -7294,7 +7294,7 @@
       </c>
       <c r="E100" s="4">
         <f t="shared" si="2"/>
-        <v>0.99819999999999998</v>
+        <v>0.99807999999999997</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -12546,19 +12546,19 @@
       </c>
       <c r="C101" s="4">
         <f>potential_preec_untrt!C101*SimParameters!$B$10</f>
-        <v>1.1249999999999999E-7</v>
+        <v>1.1999999999999999E-7</v>
       </c>
       <c r="D101" s="13">
         <f t="shared" ref="D101:D124" si="5">LOG(C101/(1-C101))</f>
-        <v>-6.9488474286944868</v>
+        <v>-6.9208187018370344</v>
       </c>
       <c r="E101" s="13">
         <f>D101+LOG(SimParameters!$B$25)</f>
-        <v>-7.6478174330305055</v>
+        <v>-7.6197887061730531</v>
       </c>
       <c r="F101" s="13">
         <f t="shared" ref="F101:F124" si="6">EXP(E101)/(1+EXP(E101))</f>
-        <v>4.7685676102535136E-4</v>
+        <v>4.9040487558389863E-4</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -12570,19 +12570,19 @@
       </c>
       <c r="C102" s="4">
         <f>potential_preec_untrt!C102*SimParameters!$B$10</f>
-        <v>2.2499999999999999E-7</v>
+        <v>2.3999999999999998E-7</v>
       </c>
       <c r="D102" s="13">
         <f t="shared" si="5"/>
-        <v>-6.6478173841723684</v>
+        <v>-6.6197886540577056</v>
       </c>
       <c r="E102" s="13">
         <f>D102+LOG(SimParameters!$B$25)</f>
-        <v>-7.3467873885083872</v>
+        <v>-7.3187586583937243</v>
       </c>
       <c r="F102" s="13">
         <f t="shared" si="6"/>
-        <v>6.442447606890342E-4</v>
+        <v>6.6254543361914738E-4</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -12594,19 +12594,19 @@
       </c>
       <c r="C103" s="4">
         <f>potential_preec_untrt!C103*SimParameters!$B$10</f>
-        <v>2.2499999999999999E-7</v>
+        <v>2.3999999999999998E-7</v>
       </c>
       <c r="D103" s="13">
         <f t="shared" si="5"/>
-        <v>-6.6478173841723684</v>
+        <v>-6.6197886540577056</v>
       </c>
       <c r="E103" s="13">
         <f>D103+LOG(SimParameters!$B$25)</f>
-        <v>-7.3467873885083872</v>
+        <v>-7.3187586583937243</v>
       </c>
       <c r="F103" s="13">
         <f t="shared" si="6"/>
-        <v>6.442447606890342E-4</v>
+        <v>6.6254543361914738E-4</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -12618,19 +12618,19 @@
       </c>
       <c r="C104" s="4">
         <f>potential_preec_untrt!C104*SimParameters!$B$10</f>
-        <v>1.7999999999999999E-6</v>
+        <v>1.9199999999999998E-6</v>
       </c>
       <c r="D104" s="13">
         <f t="shared" si="5"/>
-        <v>-5.7447267131659228</v>
+        <v>-5.7166979374502445</v>
       </c>
       <c r="E104" s="13">
         <f>D104+LOG(SimParameters!$B$25)</f>
-        <v>-6.4436967175019415</v>
+        <v>-6.4156679417862632</v>
       </c>
       <c r="F104" s="13">
         <f t="shared" si="6"/>
-        <v>1.5879903863973272E-3</v>
+        <v>1.6330557394528848E-3</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -12642,19 +12642,19 @@
       </c>
       <c r="C105" s="4">
         <f>potential_preec_untrt!C105*SimParameters!$B$10</f>
-        <v>2.2500000000000001E-6</v>
+        <v>2.4000000000000003E-6</v>
       </c>
       <c r="D105" s="13">
         <f t="shared" si="5"/>
-        <v>-5.647816504724954</v>
+        <v>-5.6197877159803866</v>
       </c>
       <c r="E105" s="13">
         <f>D105+LOG(SimParameters!$B$25)</f>
-        <v>-6.3467865090609727</v>
+        <v>-6.3187577203164054</v>
       </c>
       <c r="F105" s="13">
         <f t="shared" si="6"/>
-        <v>1.7493038944602403E-3</v>
+        <v>1.798938915538727E-3</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -12666,19 +12666,19 @@
       </c>
       <c r="C106" s="4">
         <f>potential_preec_untrt!C106*SimParameters!$B$10</f>
-        <v>3.3749999999999999E-6</v>
+        <v>3.6000000000000003E-6</v>
       </c>
       <c r="D106" s="13">
         <f t="shared" si="5"/>
-        <v>-5.4717247570866068</v>
+        <v>-5.4436959357697638</v>
       </c>
       <c r="E106" s="13">
         <f>D106+LOG(SimParameters!$B$25)</f>
-        <v>-6.1706947614226255</v>
+        <v>-6.1426659401057826</v>
       </c>
       <c r="F106" s="13">
         <f t="shared" si="6"/>
-        <v>2.0854255069992778E-3</v>
+        <v>2.1445772757196064E-3</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -12690,19 +12690,19 @@
       </c>
       <c r="C107" s="4">
         <f>potential_preec_untrt!C107*SimParameters!$B$10</f>
-        <v>3.3749999999999999E-6</v>
+        <v>3.6000000000000003E-6</v>
       </c>
       <c r="D107" s="13">
         <f t="shared" si="5"/>
-        <v>-5.4717247570866068</v>
+        <v>-5.4436959357697638</v>
       </c>
       <c r="E107" s="13">
         <f>D107+LOG(SimParameters!$B$25)</f>
-        <v>-6.1706947614226255</v>
+        <v>-6.1426659401057826</v>
       </c>
       <c r="F107" s="13">
         <f t="shared" si="6"/>
-        <v>2.0854255069992778E-3</v>
+        <v>2.1445772757196064E-3</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -12714,19 +12714,19 @@
       </c>
       <c r="C108" s="4">
         <f>potential_preec_untrt!C108*SimParameters!$B$10</f>
-        <v>4.5000000000000001E-6</v>
+        <v>4.8000000000000006E-6</v>
       </c>
       <c r="D108" s="13">
         <f t="shared" si="5"/>
-        <v>-5.3467855318950903</v>
+        <v>-5.3187566780058964</v>
       </c>
       <c r="E108" s="13">
         <f>D108+LOG(SimParameters!$B$25)</f>
-        <v>-6.0457555362311091</v>
+        <v>-6.0177266823419151</v>
       </c>
       <c r="F108" s="13">
         <f t="shared" si="6"/>
-        <v>2.3622974721857759E-3</v>
+        <v>2.4292834993621315E-3</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -12738,19 +12738,19 @@
       </c>
       <c r="C109" s="4">
         <f>potential_preec_untrt!C109*SimParameters!$B$10</f>
-        <v>1.8E-5</v>
+        <v>1.9200000000000003E-5</v>
       </c>
       <c r="D109" s="13">
         <f t="shared" si="5"/>
-        <v>-4.744719677525663</v>
+        <v>-4.7166904327623476</v>
       </c>
       <c r="E109" s="13">
         <f>D109+LOG(SimParameters!$B$25)</f>
-        <v>-5.4436896818616818</v>
+        <v>-5.4156604370983663</v>
       </c>
       <c r="F109" s="13">
         <f t="shared" si="6"/>
-        <v>4.3048892650325628E-3</v>
+        <v>4.426717318032041E-3</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -12762,19 +12762,19 @@
       </c>
       <c r="C110" s="4">
         <f>potential_preec_untrt!C110*SimParameters!$B$10</f>
-        <v>4.500000000000001E-5</v>
+        <v>4.8000000000000008E-5</v>
       </c>
       <c r="D110" s="13">
         <f t="shared" si="5"/>
-        <v>-4.3467679425332344</v>
+        <v>-4.3187379159889581</v>
       </c>
       <c r="E110" s="13">
         <f>D110+LOG(SimParameters!$B$25)</f>
-        <v>-5.0457379468692531</v>
+        <v>-5.0177079203249768</v>
       </c>
       <c r="F110" s="13">
         <f t="shared" si="6"/>
-        <v>6.3955424185268344E-3</v>
+        <v>6.5761501489709634E-3</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -12786,19 +12786,19 @@
       </c>
       <c r="C111" s="4">
         <f>potential_preec_untrt!C111*SimParameters!$B$10</f>
-        <v>4.500000000000001E-5</v>
+        <v>4.8000000000000008E-5</v>
       </c>
       <c r="D111" s="13">
         <f t="shared" si="5"/>
-        <v>-4.3467679425332344</v>
+        <v>-4.3187379159889581</v>
       </c>
       <c r="E111" s="13">
         <f>D111+LOG(SimParameters!$B$25)</f>
-        <v>-5.0457379468692531</v>
+        <v>-5.0177079203249768</v>
       </c>
       <c r="F111" s="13">
         <f t="shared" si="6"/>
-        <v>6.3955424185268344E-3</v>
+        <v>6.5761501489709634E-3</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -12810,19 +12810,19 @@
       </c>
       <c r="C112" s="4">
         <f>potential_preec_untrt!C112*SimParameters!$B$10</f>
-        <v>9.0000000000000019E-5</v>
+        <v>9.6000000000000016E-5</v>
       </c>
       <c r="D112" s="13">
         <f t="shared" si="5"/>
-        <v>-4.0457184022983057</v>
+        <v>-4.0176870726888119</v>
       </c>
       <c r="E112" s="13">
         <f>D112+LOG(SimParameters!$B$25)</f>
-        <v>-4.7446884066343245</v>
+        <v>-4.7166570770248306</v>
       </c>
       <c r="F112" s="13">
         <f t="shared" si="6"/>
-        <v>8.6227728415366866E-3</v>
+        <v>8.8657269692349119E-3</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -12834,19 +12834,19 @@
       </c>
       <c r="C113" s="4">
         <f>potential_preec_untrt!C113*SimParameters!$B$10</f>
-        <v>4.5000000000000004E-4</v>
+        <v>4.8000000000000007E-4</v>
       </c>
       <c r="D113" s="13">
         <f t="shared" si="5"/>
-        <v>-3.3465920097222872</v>
+        <v>-3.3185502512263594</v>
       </c>
       <c r="E113" s="13">
         <f>D113+LOG(SimParameters!$B$25)</f>
-        <v>-4.045562014058306</v>
+        <v>-4.0175202555623777</v>
       </c>
       <c r="F113" s="13">
         <f t="shared" si="6"/>
-        <v>1.7198888464540246E-2</v>
+        <v>1.7679354083987433E-2</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -12858,19 +12858,19 @@
       </c>
       <c r="C114" s="4">
         <f>potential_preec_untrt!C114*SimParameters!$B$10</f>
-        <v>1.3500000000000001E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D114" s="13">
         <f t="shared" si="5"/>
-        <v>-2.8690795378470413</v>
+        <v>-2.841011673141558</v>
       </c>
       <c r="E114" s="13">
         <f>D114+LOG(SimParameters!$B$25)</f>
-        <v>-3.56804954218306</v>
+        <v>-3.5399816774775767</v>
       </c>
       <c r="F114" s="13">
         <f t="shared" si="6"/>
-        <v>2.7436809082256087E-2</v>
+        <v>2.8195790017344867E-2</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -12882,19 +12882,19 @@
       </c>
       <c r="C115" s="4">
         <f>potential_preec_untrt!C115*SimParameters!$B$10</f>
-        <v>2.2500000000000003E-3</v>
+        <v>2.4000000000000002E-3</v>
       </c>
       <c r="D115" s="13">
         <f t="shared" si="5"/>
-        <v>-2.6468392183446983</v>
+        <v>-2.6187451987588801</v>
       </c>
       <c r="E115" s="13">
         <f>D115+LOG(SimParameters!$B$25)</f>
-        <v>-3.345809222680717</v>
+        <v>-3.3177152030948989</v>
       </c>
       <c r="F115" s="13">
         <f t="shared" si="6"/>
-        <v>3.4032664919811821E-2</v>
+        <v>3.4968428592545168E-2</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -12906,19 +12906,19 @@
       </c>
       <c r="C116" s="4">
         <f>potential_preec_untrt!C116*SimParameters!$B$10</f>
-        <v>2.7000000000000001E-3</v>
+        <v>2.8800000000000002E-3</v>
       </c>
       <c r="D116" s="13">
         <f t="shared" si="5"/>
-        <v>-2.5674620548812985</v>
+        <v>-2.5393549395612021</v>
       </c>
       <c r="E116" s="13">
         <f>D116+LOG(SimParameters!$B$25)</f>
-        <v>-3.2664320592173173</v>
+        <v>-3.2383249438972208</v>
       </c>
       <c r="F116" s="13">
         <f t="shared" si="6"/>
-        <v>3.6740892761823921E-2</v>
+        <v>3.7748687695336874E-2</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -12930,19 +12930,19 @@
       </c>
       <c r="C117" s="4">
         <f>potential_preec_untrt!C117*SimParameters!$B$10</f>
-        <v>6.7500000000000004E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="D117" s="13">
         <f t="shared" si="5"/>
-        <v>-1.1403450676497002</v>
+        <v>-1.1102154797875936</v>
       </c>
       <c r="E117" s="13">
         <f>D117+LOG(SimParameters!$B$25)</f>
-        <v>-1.839315071985719</v>
+        <v>-1.8091854841236124</v>
       </c>
       <c r="F117" s="13">
         <f t="shared" si="6"/>
-        <v>0.13713231794257544</v>
+        <v>0.14073659616116271</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -12954,19 +12954,19 @@
       </c>
       <c r="C118" s="4">
         <f>potential_preec_untrt!C118*SimParameters!$B$10</f>
-        <v>0.09</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="D118" s="13">
         <f t="shared" si="5"/>
-        <v>-1.0047988828817687</v>
+        <v>-0.97389719743579495</v>
       </c>
       <c r="E118" s="13">
         <f>D118+LOG(SimParameters!$B$25)</f>
-        <v>-1.7037688872177874</v>
+        <v>-1.6728672017718136</v>
       </c>
       <c r="F118" s="13">
         <f t="shared" si="6"/>
-        <v>0.15397366753350078</v>
+        <v>0.15804228070078649</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -12978,19 +12978,19 @@
       </c>
       <c r="C119" s="4">
         <f>potential_preec_untrt!C119*SimParameters!$B$10</f>
-        <v>0.11250000000000002</v>
+        <v>0.12000000000000002</v>
       </c>
       <c r="D119" s="13">
         <f t="shared" si="5"/>
-        <v>-0.89701583927975037</v>
+        <v>-0.86530142610254379</v>
       </c>
       <c r="E119" s="13">
         <f>D119+LOG(SimParameters!$B$25)</f>
-        <v>-1.595985843615769</v>
+        <v>-1.5642714304385625</v>
       </c>
       <c r="F119" s="13">
         <f t="shared" si="6"/>
-        <v>0.16854339655726924</v>
+        <v>0.17303457871352046</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -13002,19 +13002,19 @@
       </c>
       <c r="C120" s="4">
         <f>potential_preec_untrt!C120*SimParameters!$B$10</f>
-        <v>0.13500000000000001</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="D120" s="13">
         <f t="shared" si="5"/>
-        <v>-0.80668233896980812</v>
+        <v>-0.7741112725819036</v>
       </c>
       <c r="E120" s="13">
         <f>D120+LOG(SimParameters!$B$25)</f>
-        <v>-1.5056523433058269</v>
+        <v>-1.4730812769179225</v>
       </c>
       <c r="F120" s="13">
         <f t="shared" si="6"/>
-        <v>0.18158400964841215</v>
+        <v>0.18647472675972418</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -13026,19 +13026,19 @@
       </c>
       <c r="C121" s="4">
         <f>potential_preec_untrt!C121*SimParameters!$B$10</f>
-        <v>0.22500000000000003</v>
+        <v>0.24000000000000005</v>
       </c>
       <c r="D121" s="13">
         <f t="shared" si="5"/>
-        <v>-0.53711918439494766</v>
+        <v>-0.50060235056918523</v>
       </c>
       <c r="E121" s="13">
         <f>D121+LOG(SimParameters!$B$25)</f>
-        <v>-1.2360891887309664</v>
+        <v>-1.199572354905204</v>
       </c>
       <c r="F121" s="13">
         <f t="shared" si="6"/>
-        <v>0.22511745257138824</v>
+        <v>0.23155130092178253</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -13050,19 +13050,19 @@
       </c>
       <c r="C122" s="4">
         <f>potential_preec_untrt!C122*SimParameters!$B$10</f>
-        <v>0.29249999999999998</v>
+        <v>0.31200000000000006</v>
       </c>
       <c r="D122" s="13">
         <f t="shared" si="5"/>
-        <v>-0.38360057377812867</v>
+        <v>-0.34343384421706841</v>
       </c>
       <c r="E122" s="13">
         <f>D122+LOG(SimParameters!$B$25)</f>
-        <v>-1.0825705781141475</v>
+        <v>-1.0424038485530871</v>
       </c>
       <c r="F122" s="13">
         <f t="shared" si="6"/>
-        <v>0.25301986692677358</v>
+        <v>0.26068643609504077</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -13074,19 +13074,19 @@
       </c>
       <c r="C123" s="4">
         <f>potential_preec_untrt!C123*SimParameters!$B$10</f>
-        <v>0.33749999999999997</v>
+        <v>0.36</v>
       </c>
       <c r="D123" s="13">
         <f t="shared" si="5"/>
-        <v>-0.29291210544180185</v>
+        <v>-0.24987747321659989</v>
       </c>
       <c r="E123" s="13">
         <f>D123+LOG(SimParameters!$B$25)</f>
-        <v>-0.99188210977782054</v>
+        <v>-0.94884747755261867</v>
       </c>
       <c r="F123" s="13">
         <f t="shared" si="6"/>
-        <v>0.27054048605758929</v>
+        <v>0.27911666260808804</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -13098,19 +13098,19 @@
       </c>
       <c r="C124" s="4">
         <f>potential_preec_untrt!C124*SimParameters!$B$10</f>
-        <v>0.45000000000000007</v>
+        <v>0.48000000000000009</v>
       </c>
       <c r="D124" s="13">
         <f t="shared" si="5"/>
-        <v>-8.7150175718900019E-2</v>
+        <v>-3.4762106259211764E-2</v>
       </c>
       <c r="E124" s="13">
         <f>D124+LOG(SimParameters!$B$25)</f>
-        <v>-0.78612018005491879</v>
+        <v>-0.73373211059523047</v>
       </c>
       <c r="F124" s="13">
         <f t="shared" si="6"/>
-        <v>0.3130023484932315</v>
+        <v>0.32437627633831295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data generation procedures and associated analysis procedures. In particular, added predictor of outcome and censoring, which necessitated additional standardization.
</commit_message>
<xml_diff>
--- a/Parameters_Abortion05_Preeclampsia05_EMM.xlsx
+++ b/Parameters_Abortion05_Preeclampsia05_EMM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/preg_cohort_construction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA555C8E-E419-F14E-9510-3F8901378278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE29BB13-51FC-AE43-A1CA-2810B68C04AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="13" r:id="rId1"/>
@@ -680,7 +680,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
   <si>
     <t>p_fetaldeath</t>
   </si>
@@ -1204,6 +1204,24 @@
   <si>
     <t>OR</t>
   </si>
+  <si>
+    <t>Weeks 7-9</t>
+  </si>
+  <si>
+    <t>Weeks 10-13</t>
+  </si>
+  <si>
+    <t>Weeks 14-16</t>
+  </si>
+  <si>
+    <t>Weeks 17-25</t>
+  </si>
+  <si>
+    <t>Weeks 26-34</t>
+  </si>
+  <si>
+    <t>Weeks 35-40</t>
+  </si>
 </sst>
 </file>
 
@@ -1362,7 +1380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1393,6 +1411,16 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2172,10 +2200,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBAD042-1D8C-E044-AB59-2B80CE0D260D}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2184,10 +2212,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2206,159 +2234,377 @@
       <c r="A4" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="8">
-        <v>0.8</v>
-      </c>
-    </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>53</v>
+      <c r="A7" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="8">
-        <v>0.2</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B8" s="18"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>50</v>
+      <c r="A9" s="21" t="s">
+        <v>54</v>
       </c>
       <c r="B9" s="8">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B12" s="18"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="8">
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="18"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>17</v>
+      <c r="A15" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="B15" s="8">
-        <v>2</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="8"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="8"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="22"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="8">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B37" s="18"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="8">
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="8">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="18"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B42" s="22"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>16</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B44" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="8">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="8">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="B49" s="18"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="8">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="8">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B55" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="8">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B58" s="8">
         <v>2.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A42:B42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2368,8 +2614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98:C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3270,7 +3516,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="3">
-        <f>C2*SimParameters!B15</f>
+        <f>C2*SimParameters!B35</f>
         <v>0</v>
       </c>
       <c r="D43" s="3">
@@ -3282,7 +3528,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="3">
-        <f>F2*SimParameters!E15</f>
+        <f>F2*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3294,7 +3540,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="3">
-        <f>C3*SimParameters!B15</f>
+        <f>C3*SimParameters!B35</f>
         <v>0</v>
       </c>
       <c r="D44" s="3">
@@ -3306,7 +3552,7 @@
         <v>1</v>
       </c>
       <c r="F44" s="3">
-        <f>F3*SimParameters!E15</f>
+        <f>F3*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3318,7 +3564,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="3">
-        <f>C4*SimParameters!B15</f>
+        <f>C4*SimParameters!B35</f>
         <v>0</v>
       </c>
       <c r="D45" s="3">
@@ -3330,7 +3576,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="3">
-        <f>F4*SimParameters!E15</f>
+        <f>F4*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3342,7 +3588,7 @@
         <v>3</v>
       </c>
       <c r="C46" s="3">
-        <f>C5*SimParameters!B15</f>
+        <f>C5*SimParameters!B35</f>
         <v>0</v>
       </c>
       <c r="D46" s="3">
@@ -3354,7 +3600,7 @@
         <v>1</v>
       </c>
       <c r="F46" s="3">
-        <f>F5*SimParameters!E15</f>
+        <f>F5*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3366,7 +3612,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="3">
-        <f>C6*SimParameters!B15</f>
+        <f>C6*SimParameters!B35</f>
         <v>0</v>
       </c>
       <c r="D47" s="3">
@@ -3378,7 +3624,7 @@
         <v>1</v>
       </c>
       <c r="F47" s="3">
-        <f>F6*SimParameters!E15</f>
+        <f>F6*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3390,7 +3636,7 @@
         <v>5</v>
       </c>
       <c r="C48" s="3">
-        <f>C7*SimParameters!B15</f>
+        <f>C7*SimParameters!B35</f>
         <v>0</v>
       </c>
       <c r="D48" s="3">
@@ -3402,7 +3648,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="3">
-        <f>F7*SimParameters!E15</f>
+        <f>F7*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3414,7 +3660,7 @@
         <v>6</v>
       </c>
       <c r="C49" s="3">
-        <f>C8*SimParameters!B15</f>
+        <f>C8*SimParameters!B35</f>
         <v>0</v>
       </c>
       <c r="D49" s="3">
@@ -3426,7 +3672,7 @@
         <v>1</v>
       </c>
       <c r="F49" s="3">
-        <f>F8*SimParameters!E15</f>
+        <f>F8*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3438,8 +3684,8 @@
         <v>7</v>
       </c>
       <c r="C50" s="3">
-        <f>C9*SimParameters!B15</f>
-        <v>0.1</v>
+        <f>C9*SimParameters!$B$34</f>
+        <v>6.25E-2</v>
       </c>
       <c r="D50" s="3">
         <f t="shared" si="1"/>
@@ -3447,10 +3693,10 @@
       </c>
       <c r="E50" s="3">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>0.9375</v>
       </c>
       <c r="F50" s="3">
-        <f>F9*SimParameters!E15</f>
+        <f>F9*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3462,8 +3708,8 @@
         <v>8</v>
       </c>
       <c r="C51" s="3">
-        <f>C10*SimParameters!B15</f>
-        <v>0.04</v>
+        <f>C10*SimParameters!$B$34</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D51" s="3">
         <f t="shared" si="1"/>
@@ -3471,10 +3717,10 @@
       </c>
       <c r="E51" s="3">
         <f t="shared" si="2"/>
-        <v>0.96</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="F51" s="3">
-        <f>F10*SimParameters!E15</f>
+        <f>F10*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3486,8 +3732,8 @@
         <v>9</v>
       </c>
       <c r="C52" s="3">
-        <f>C11*SimParameters!B15</f>
-        <v>0.04</v>
+        <f>C11*SimParameters!$B$34</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D52" s="3">
         <f t="shared" si="1"/>
@@ -3495,10 +3741,10 @@
       </c>
       <c r="E52" s="3">
         <f t="shared" si="2"/>
-        <v>0.96</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="F52" s="3">
-        <f>F11*SimParameters!E15</f>
+        <f>F11*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3510,7 +3756,7 @@
         <v>10</v>
       </c>
       <c r="C53" s="3">
-        <f>C12*SimParameters!B15</f>
+        <f>C12*SimParameters!$B$35</f>
         <v>0.02</v>
       </c>
       <c r="D53" s="3">
@@ -3522,7 +3768,7 @@
         <v>0.98</v>
       </c>
       <c r="F53" s="3">
-        <f>F12*SimParameters!E15</f>
+        <f>F12*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3534,7 +3780,7 @@
         <v>11</v>
       </c>
       <c r="C54" s="3">
-        <f>C13*SimParameters!B15</f>
+        <f>C13*SimParameters!$B$35</f>
         <v>0.01</v>
       </c>
       <c r="D54" s="3">
@@ -3546,7 +3792,7 @@
         <v>0.99</v>
       </c>
       <c r="F54" s="3">
-        <f>F13*SimParameters!E15</f>
+        <f>F13*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3558,7 +3804,7 @@
         <v>12</v>
       </c>
       <c r="C55" s="3">
-        <f>C14*SimParameters!B15</f>
+        <f>C14*SimParameters!$B$35</f>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D55" s="3">
@@ -3570,7 +3816,7 @@
         <v>0.99199999999999999</v>
       </c>
       <c r="F55" s="3">
-        <f>F14*SimParameters!E15</f>
+        <f>F14*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3582,7 +3828,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="3">
-        <f>C15*SimParameters!B15</f>
+        <f>C15*SimParameters!$B$35</f>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D56" s="3">
@@ -3594,7 +3840,7 @@
         <v>0.99199999999999999</v>
       </c>
       <c r="F56" s="3">
-        <f>F15*SimParameters!E15</f>
+        <f>F15*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3606,8 +3852,8 @@
         <v>14</v>
       </c>
       <c r="C57" s="3">
-        <f>C16*SimParameters!B15</f>
-        <v>8.0000000000000002E-3</v>
+        <f>C16*SimParameters!$B$36</f>
+        <v>1.2E-2</v>
       </c>
       <c r="D57" s="3">
         <f t="shared" si="1"/>
@@ -3615,10 +3861,10 @@
       </c>
       <c r="E57" s="3">
         <f t="shared" si="2"/>
-        <v>0.99199999999999999</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="F57" s="3">
-        <f>F16*SimParameters!E15</f>
+        <f>F16*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3630,8 +3876,8 @@
         <v>15</v>
       </c>
       <c r="C58" s="3">
-        <f>C17*SimParameters!B15</f>
-        <v>8.0000000000000002E-3</v>
+        <f>C17*SimParameters!$B$36</f>
+        <v>1.2E-2</v>
       </c>
       <c r="D58" s="3">
         <f t="shared" si="1"/>
@@ -3639,10 +3885,10 @@
       </c>
       <c r="E58" s="3">
         <f t="shared" si="2"/>
-        <v>0.99199999999999999</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="F58" s="3">
-        <f>F17*SimParameters!E15</f>
+        <f>F17*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -3654,8 +3900,8 @@
         <v>16</v>
       </c>
       <c r="C59" s="3">
-        <f>C18*SimParameters!B15</f>
-        <v>1.6000000000000001E-3</v>
+        <f>C18*SimParameters!$B$36</f>
+        <v>2.4000000000000002E-3</v>
       </c>
       <c r="D59" s="3">
         <f t="shared" si="1"/>
@@ -3663,10 +3909,10 @@
       </c>
       <c r="E59" s="3">
         <f t="shared" si="2"/>
-        <v>0.99839999999999995</v>
+        <v>0.99760000000000004</v>
       </c>
       <c r="F59" s="3">
-        <f>F18*SimParameters!E15</f>
+        <f>F18*SimParameters!E34</f>
         <v>0</v>
       </c>
     </row>
@@ -4253,7 +4499,7 @@
         <v>0</v>
       </c>
       <c r="C84" s="4">
-        <f>C2*SimParameters!B16</f>
+        <f>C2*SimParameters!B39</f>
         <v>0</v>
       </c>
       <c r="D84" s="4">
@@ -4265,7 +4511,7 @@
         <v>1</v>
       </c>
       <c r="F84" s="4">
-        <f>F2*SimParameters!E16</f>
+        <f>F2*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4277,7 +4523,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="4">
-        <f>C3*SimParameters!B16</f>
+        <f>C3*SimParameters!B39</f>
         <v>0</v>
       </c>
       <c r="D85" s="4">
@@ -4289,7 +4535,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="4">
-        <f>F3*SimParameters!E16</f>
+        <f>F3*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4301,7 +4547,7 @@
         <v>2</v>
       </c>
       <c r="C86" s="4">
-        <f>C4*SimParameters!B16</f>
+        <f>C4*SimParameters!B39</f>
         <v>0</v>
       </c>
       <c r="D86" s="4">
@@ -4313,7 +4559,7 @@
         <v>1</v>
       </c>
       <c r="F86" s="4">
-        <f>F4*SimParameters!E16</f>
+        <f>F4*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4325,7 +4571,7 @@
         <v>3</v>
       </c>
       <c r="C87" s="4">
-        <f>C5*SimParameters!B16</f>
+        <f>C5*SimParameters!B39</f>
         <v>0</v>
       </c>
       <c r="D87" s="4">
@@ -4337,7 +4583,7 @@
         <v>1</v>
       </c>
       <c r="F87" s="4">
-        <f>F5*SimParameters!E16</f>
+        <f>F5*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4349,7 +4595,7 @@
         <v>4</v>
       </c>
       <c r="C88" s="4">
-        <f>C6*SimParameters!B16</f>
+        <f>C6*SimParameters!B39</f>
         <v>0</v>
       </c>
       <c r="D88" s="4">
@@ -4361,7 +4607,7 @@
         <v>1</v>
       </c>
       <c r="F88" s="4">
-        <f>F6*SimParameters!E16</f>
+        <f>F6*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4373,7 +4619,7 @@
         <v>5</v>
       </c>
       <c r="C89" s="4">
-        <f>C7*SimParameters!B16</f>
+        <f>C7*SimParameters!B39</f>
         <v>0</v>
       </c>
       <c r="D89" s="4">
@@ -4385,7 +4631,7 @@
         <v>1</v>
       </c>
       <c r="F89" s="4">
-        <f>F7*SimParameters!E16</f>
+        <f>F7*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4397,7 +4643,7 @@
         <v>6</v>
       </c>
       <c r="C90" s="4">
-        <f>C8*SimParameters!B16</f>
+        <f>C8*SimParameters!B39</f>
         <v>0</v>
       </c>
       <c r="D90" s="4">
@@ -4409,7 +4655,7 @@
         <v>1</v>
       </c>
       <c r="F90" s="4">
-        <f>F8*SimParameters!E16</f>
+        <f>F8*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4421,8 +4667,8 @@
         <v>7</v>
       </c>
       <c r="C91" s="4">
-        <f>C9*SimParameters!B16</f>
-        <v>0.15000000000000002</v>
+        <f>C9*SimParameters!$B$38</f>
+        <v>9.375E-2</v>
       </c>
       <c r="D91" s="4">
         <f t="shared" si="5"/>
@@ -4430,10 +4676,10 @@
       </c>
       <c r="E91" s="4">
         <f t="shared" si="6"/>
-        <v>0.85</v>
+        <v>0.90625</v>
       </c>
       <c r="F91" s="4">
-        <f>F9*SimParameters!E16</f>
+        <f>F9*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4445,8 +4691,8 @@
         <v>8</v>
       </c>
       <c r="C92" s="4">
-        <f>C10*SimParameters!B16</f>
-        <v>0.06</v>
+        <f>C10*SimParameters!$B$38</f>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="D92" s="4">
         <f t="shared" si="5"/>
@@ -4454,10 +4700,10 @@
       </c>
       <c r="E92" s="4">
         <f t="shared" si="6"/>
-        <v>0.94</v>
+        <v>0.96250000000000002</v>
       </c>
       <c r="F92" s="4">
-        <f>F10*SimParameters!E16</f>
+        <f>F10*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4469,8 +4715,8 @@
         <v>9</v>
       </c>
       <c r="C93" s="4">
-        <f>C11*SimParameters!B16</f>
-        <v>0.06</v>
+        <f>C11*SimParameters!$B$38</f>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="D93" s="4">
         <f t="shared" si="5"/>
@@ -4478,10 +4724,10 @@
       </c>
       <c r="E93" s="4">
         <f t="shared" si="6"/>
-        <v>0.94</v>
+        <v>0.96250000000000002</v>
       </c>
       <c r="F93" s="4">
-        <f>F11*SimParameters!E16</f>
+        <f>F11*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4493,7 +4739,7 @@
         <v>10</v>
       </c>
       <c r="C94" s="4">
-        <f>C12*SimParameters!B16</f>
+        <f>C12*SimParameters!$B$39</f>
         <v>0.03</v>
       </c>
       <c r="D94" s="4">
@@ -4505,7 +4751,7 @@
         <v>0.97</v>
       </c>
       <c r="F94" s="4">
-        <f>F12*SimParameters!E16</f>
+        <f>F12*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4517,7 +4763,7 @@
         <v>11</v>
       </c>
       <c r="C95" s="4">
-        <f>C13*SimParameters!B16</f>
+        <f>C13*SimParameters!$B$39</f>
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D95" s="4">
@@ -4529,7 +4775,7 @@
         <v>0.98499999999999999</v>
       </c>
       <c r="F95" s="4">
-        <f>F13*SimParameters!E16</f>
+        <f>F13*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4541,7 +4787,7 @@
         <v>12</v>
       </c>
       <c r="C96" s="4">
-        <f>C14*SimParameters!B16</f>
+        <f>C14*SimParameters!$B$39</f>
         <v>1.2E-2</v>
       </c>
       <c r="D96" s="4">
@@ -4553,7 +4799,7 @@
         <v>0.98799999999999999</v>
       </c>
       <c r="F96" s="4">
-        <f>F14*SimParameters!E16</f>
+        <f>F14*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4565,7 +4811,7 @@
         <v>13</v>
       </c>
       <c r="C97" s="4">
-        <f>C15*SimParameters!B16</f>
+        <f>C15*SimParameters!$B$39</f>
         <v>1.2E-2</v>
       </c>
       <c r="D97" s="4">
@@ -4577,7 +4823,7 @@
         <v>0.98799999999999999</v>
       </c>
       <c r="F97" s="4">
-        <f>F15*SimParameters!E16</f>
+        <f>F15*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4589,8 +4835,8 @@
         <v>14</v>
       </c>
       <c r="C98" s="4">
-        <f>C16*SimParameters!B16</f>
-        <v>1.2E-2</v>
+        <f>C16*SimParameters!$B$40</f>
+        <v>1.9199999999999998E-2</v>
       </c>
       <c r="D98" s="4">
         <f t="shared" si="5"/>
@@ -4598,10 +4844,10 @@
       </c>
       <c r="E98" s="4">
         <f t="shared" si="6"/>
-        <v>0.98799999999999999</v>
+        <v>0.98080000000000001</v>
       </c>
       <c r="F98" s="4">
-        <f>F16*SimParameters!E16</f>
+        <f>F16*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4613,8 +4859,8 @@
         <v>15</v>
       </c>
       <c r="C99" s="4">
-        <f>C17*SimParameters!B16</f>
-        <v>1.2E-2</v>
+        <f>C17*SimParameters!$B$40</f>
+        <v>1.9199999999999998E-2</v>
       </c>
       <c r="D99" s="4">
         <f t="shared" si="5"/>
@@ -4622,10 +4868,10 @@
       </c>
       <c r="E99" s="4">
         <f t="shared" si="6"/>
-        <v>0.98799999999999999</v>
+        <v>0.98080000000000001</v>
       </c>
       <c r="F99" s="4">
-        <f>F17*SimParameters!E16</f>
+        <f>F17*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -4637,8 +4883,8 @@
         <v>16</v>
       </c>
       <c r="C100" s="4">
-        <f>C18*SimParameters!B16</f>
-        <v>2.4000000000000002E-3</v>
+        <f>C18*SimParameters!$B$40</f>
+        <v>3.8400000000000001E-3</v>
       </c>
       <c r="D100" s="4">
         <f t="shared" si="5"/>
@@ -4646,10 +4892,10 @@
       </c>
       <c r="E100" s="4">
         <f t="shared" si="6"/>
-        <v>0.99760000000000004</v>
+        <v>0.99616000000000005</v>
       </c>
       <c r="F100" s="4">
-        <f>F18*SimParameters!E16</f>
+        <f>F18*SimParameters!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -5238,8 +5484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E296094E-C959-F34D-935C-7330539695AA}">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5275,7 +5521,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <f>potential_preg_untrt!C2*SimParameters!$B$4</f>
+        <f>potential_preg_untrt!C2*SimParameters!$B$5</f>
         <v>0</v>
       </c>
       <c r="D2" s="2">
@@ -5295,7 +5541,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <f>potential_preg_untrt!C3*SimParameters!$B$4</f>
+        <f>potential_preg_untrt!C3*SimParameters!$B$5</f>
         <v>0</v>
       </c>
       <c r="D3" s="2">
@@ -5315,7 +5561,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <f>potential_preg_untrt!C4*SimParameters!$B$4</f>
+        <f>potential_preg_untrt!C4*SimParameters!$B$5</f>
         <v>0</v>
       </c>
       <c r="D4" s="2">
@@ -5335,7 +5581,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2">
-        <f>potential_preg_untrt!C5*SimParameters!$B$4</f>
+        <f>potential_preg_untrt!C5*SimParameters!$B$5</f>
         <v>0</v>
       </c>
       <c r="D5" s="2">
@@ -5355,7 +5601,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="2">
-        <f>potential_preg_untrt!C6*SimParameters!$B$4</f>
+        <f>potential_preg_untrt!C6*SimParameters!$B$5</f>
         <v>0</v>
       </c>
       <c r="D6" s="2">
@@ -5375,7 +5621,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="2">
-        <f>potential_preg_untrt!C7*SimParameters!$B$4</f>
+        <f>potential_preg_untrt!C7*SimParameters!$B$5</f>
         <v>0</v>
       </c>
       <c r="D7" s="2">
@@ -5395,7 +5641,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="2">
-        <f>potential_preg_untrt!C8*SimParameters!$B$4</f>
+        <f>potential_preg_untrt!C8*SimParameters!$B$5</f>
         <v>0</v>
       </c>
       <c r="D8" s="2">
@@ -5415,8 +5661,8 @@
         <v>7</v>
       </c>
       <c r="C9" s="2">
-        <f>potential_preg_untrt!C9*SimParameters!$B$4</f>
-        <v>5.000000000000001E-3</v>
+        <f>potential_preg_untrt!C9*SimParameters!$B$5</f>
+        <v>2.5000000000000005E-3</v>
       </c>
       <c r="D9" s="2">
         <f>potential_preg_untrt!D9</f>
@@ -5424,7 +5670,7 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>0.995</v>
+        <v>0.99750000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -5435,8 +5681,8 @@
         <v>8</v>
       </c>
       <c r="C10" s="2">
-        <f>potential_preg_untrt!C10*SimParameters!$B$4</f>
-        <v>2E-3</v>
+        <f>potential_preg_untrt!C10*SimParameters!$B$5</f>
+        <v>1E-3</v>
       </c>
       <c r="D10" s="2">
         <f>potential_preg_untrt!D10</f>
@@ -5444,7 +5690,7 @@
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0.998</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -5455,8 +5701,8 @@
         <v>9</v>
       </c>
       <c r="C11" s="2">
-        <f>potential_preg_untrt!C11*SimParameters!$B$4</f>
-        <v>2E-3</v>
+        <f>potential_preg_untrt!C11*SimParameters!$B$5</f>
+        <v>1E-3</v>
       </c>
       <c r="D11" s="2">
         <f>potential_preg_untrt!D11</f>
@@ -5464,7 +5710,7 @@
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>0.998</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -5475,7 +5721,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="2">
-        <f>potential_preg_untrt!C12*SimParameters!$B$4</f>
+        <f>potential_preg_untrt!C12*SimParameters!$B$6</f>
         <v>1E-3</v>
       </c>
       <c r="D12" s="2">
@@ -5495,7 +5741,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="2">
-        <f>potential_preg_untrt!C13*SimParameters!$B$4</f>
+        <f>potential_preg_untrt!C13*SimParameters!$B$6</f>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="D13" s="2">
@@ -5515,7 +5761,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="2">
-        <f>potential_preg_untrt!C14*SimParameters!$B$4</f>
+        <f>potential_preg_untrt!C14*SimParameters!$B$6</f>
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="D14" s="2">
@@ -5535,7 +5781,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="2">
-        <f>potential_preg_untrt!C15*SimParameters!$B$4</f>
+        <f>potential_preg_untrt!C15*SimParameters!$B$6</f>
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="D15" s="2">
@@ -5555,8 +5801,8 @@
         <v>14</v>
       </c>
       <c r="C16" s="2">
-        <f>potential_preg_untrt!C16*SimParameters!$B$4</f>
-        <v>4.0000000000000002E-4</v>
+        <f>potential_preg_untrt!C16*SimParameters!$B$7</f>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D16" s="2">
         <f>potential_preg_untrt!D16</f>
@@ -5564,7 +5810,7 @@
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>0.99960000000000004</v>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -5575,8 +5821,8 @@
         <v>15</v>
       </c>
       <c r="C17" s="2">
-        <f>potential_preg_untrt!C17*SimParameters!$B$4</f>
-        <v>4.0000000000000002E-4</v>
+        <f>potential_preg_untrt!C17*SimParameters!$B$7</f>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D17" s="2">
         <f>potential_preg_untrt!D17</f>
@@ -5584,7 +5830,7 @@
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>0.99960000000000004</v>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -5595,8 +5841,8 @@
         <v>16</v>
       </c>
       <c r="C18" s="2">
-        <f>potential_preg_untrt!C18*SimParameters!$B$4</f>
-        <v>8.0000000000000007E-5</v>
+        <f>potential_preg_untrt!C18*SimParameters!$B$7</f>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="D18" s="2">
         <f>potential_preg_untrt!D18</f>
@@ -5604,7 +5850,7 @@
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>0.99992000000000003</v>
+        <v>0.99983999999999995</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -6094,7 +6340,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="3">
-        <f>potential_preg_untrt!C43*SimParameters!$B$5</f>
+        <f>potential_preg_untrt!C43*SimParameters!$B$9</f>
         <v>0</v>
       </c>
       <c r="D43" s="3">
@@ -6114,7 +6360,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="3">
-        <f>potential_preg_untrt!C44*SimParameters!$B$5</f>
+        <f>potential_preg_untrt!C44*SimParameters!$B$9</f>
         <v>0</v>
       </c>
       <c r="D44" s="3">
@@ -6134,7 +6380,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="3">
-        <f>potential_preg_untrt!C45*SimParameters!$B$5</f>
+        <f>potential_preg_untrt!C45*SimParameters!$B$9</f>
         <v>0</v>
       </c>
       <c r="D45" s="3">
@@ -6154,7 +6400,7 @@
         <v>3</v>
       </c>
       <c r="C46" s="3">
-        <f>potential_preg_untrt!C46*SimParameters!$B$5</f>
+        <f>potential_preg_untrt!C46*SimParameters!$B$9</f>
         <v>0</v>
       </c>
       <c r="D46" s="3">
@@ -6174,7 +6420,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="3">
-        <f>potential_preg_untrt!C47*SimParameters!$B$5</f>
+        <f>potential_preg_untrt!C47*SimParameters!$B$9</f>
         <v>0</v>
       </c>
       <c r="D47" s="3">
@@ -6194,7 +6440,7 @@
         <v>5</v>
       </c>
       <c r="C48" s="3">
-        <f>potential_preg_untrt!C48*SimParameters!$B$5</f>
+        <f>potential_preg_untrt!C48*SimParameters!$B$9</f>
         <v>0</v>
       </c>
       <c r="D48" s="3">
@@ -6214,7 +6460,7 @@
         <v>6</v>
       </c>
       <c r="C49" s="3">
-        <f>potential_preg_untrt!C49*SimParameters!$B$5</f>
+        <f>potential_preg_untrt!C49*SimParameters!$B$9</f>
         <v>0</v>
       </c>
       <c r="D49" s="3">
@@ -6234,8 +6480,8 @@
         <v>7</v>
       </c>
       <c r="C50" s="3">
-        <f>potential_preg_untrt!C50*SimParameters!$B$5</f>
-        <v>0.05</v>
+        <f>potential_preg_untrt!C50*SimParameters!$B$9</f>
+        <v>2.34375E-2</v>
       </c>
       <c r="D50" s="3">
         <f>potential_preg_untrt!D50</f>
@@ -6243,7 +6489,7 @@
       </c>
       <c r="E50" s="3">
         <f t="shared" si="1"/>
-        <v>0.95</v>
+        <v>0.9765625</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -6254,8 +6500,8 @@
         <v>8</v>
       </c>
       <c r="C51" s="3">
-        <f>potential_preg_untrt!C51*SimParameters!$B$5</f>
-        <v>0.02</v>
+        <f>potential_preg_untrt!C51*SimParameters!$B$9</f>
+        <v>9.3750000000000014E-3</v>
       </c>
       <c r="D51" s="3">
         <f>potential_preg_untrt!D51</f>
@@ -6263,7 +6509,7 @@
       </c>
       <c r="E51" s="3">
         <f t="shared" si="1"/>
-        <v>0.98</v>
+        <v>0.99062499999999998</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -6274,8 +6520,8 @@
         <v>9</v>
       </c>
       <c r="C52" s="3">
-        <f>potential_preg_untrt!C52*SimParameters!$B$5</f>
-        <v>0.02</v>
+        <f>potential_preg_untrt!C52*SimParameters!$B$9</f>
+        <v>9.3750000000000014E-3</v>
       </c>
       <c r="D52" s="3">
         <f>potential_preg_untrt!D52</f>
@@ -6283,7 +6529,7 @@
       </c>
       <c r="E52" s="3">
         <f t="shared" si="1"/>
-        <v>0.98</v>
+        <v>0.99062499999999998</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -6294,7 +6540,7 @@
         <v>10</v>
       </c>
       <c r="C53" s="3">
-        <f>potential_preg_untrt!C53*SimParameters!$B$5</f>
+        <f>potential_preg_untrt!C53*SimParameters!$B$10</f>
         <v>0.01</v>
       </c>
       <c r="D53" s="3">
@@ -6314,7 +6560,7 @@
         <v>11</v>
       </c>
       <c r="C54" s="3">
-        <f>potential_preg_untrt!C54*SimParameters!$B$5</f>
+        <f>potential_preg_untrt!C54*SimParameters!$B$10</f>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D54" s="3">
@@ -6334,7 +6580,7 @@
         <v>12</v>
       </c>
       <c r="C55" s="3">
-        <f>potential_preg_untrt!C55*SimParameters!$B$5</f>
+        <f>potential_preg_untrt!C55*SimParameters!$B$10</f>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D55" s="3">
@@ -6354,7 +6600,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="3">
-        <f>potential_preg_untrt!C56*SimParameters!$B$5</f>
+        <f>potential_preg_untrt!C56*SimParameters!$B$10</f>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D56" s="3">
@@ -6374,8 +6620,8 @@
         <v>14</v>
       </c>
       <c r="C57" s="3">
-        <f>potential_preg_untrt!C57*SimParameters!$B$5</f>
-        <v>4.0000000000000001E-3</v>
+        <f>potential_preg_untrt!C57*SimParameters!$B$11</f>
+        <v>8.0400000000000003E-3</v>
       </c>
       <c r="D57" s="3">
         <f>potential_preg_untrt!D57</f>
@@ -6383,7 +6629,7 @@
       </c>
       <c r="E57" s="3">
         <f t="shared" si="1"/>
-        <v>0.996</v>
+        <v>0.99195999999999995</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -6394,8 +6640,8 @@
         <v>15</v>
       </c>
       <c r="C58" s="3">
-        <f>potential_preg_untrt!C58*SimParameters!$B$5</f>
-        <v>4.0000000000000001E-3</v>
+        <f>potential_preg_untrt!C58*SimParameters!$B$11</f>
+        <v>8.0400000000000003E-3</v>
       </c>
       <c r="D58" s="3">
         <f>potential_preg_untrt!D58</f>
@@ -6403,7 +6649,7 @@
       </c>
       <c r="E58" s="3">
         <f t="shared" si="1"/>
-        <v>0.996</v>
+        <v>0.99195999999999995</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -6414,8 +6660,8 @@
         <v>16</v>
       </c>
       <c r="C59" s="3">
-        <f>potential_preg_untrt!C59*SimParameters!$B$5</f>
-        <v>8.0000000000000004E-4</v>
+        <f>potential_preg_untrt!C59*SimParameters!$B$11</f>
+        <v>1.6080000000000003E-3</v>
       </c>
       <c r="D59" s="3">
         <f>potential_preg_untrt!D59</f>
@@ -6423,7 +6669,7 @@
       </c>
       <c r="E59" s="3">
         <f t="shared" si="1"/>
-        <v>0.99919999999999998</v>
+        <v>0.99839199999999995</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -6913,7 +7159,7 @@
         <v>0</v>
       </c>
       <c r="C84" s="4">
-        <f>potential_preg_untrt!C84*SimParameters!$B$6</f>
+        <f>potential_preg_untrt!C84*SimParameters!$B$13</f>
         <v>0</v>
       </c>
       <c r="D84" s="4">
@@ -6933,7 +7179,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="4">
-        <f>potential_preg_untrt!C85*SimParameters!$B$6</f>
+        <f>potential_preg_untrt!C85*SimParameters!$B$13</f>
         <v>0</v>
       </c>
       <c r="D85" s="4">
@@ -6953,7 +7199,7 @@
         <v>2</v>
       </c>
       <c r="C86" s="4">
-        <f>potential_preg_untrt!C86*SimParameters!$B$6</f>
+        <f>potential_preg_untrt!C86*SimParameters!$B$13</f>
         <v>0</v>
       </c>
       <c r="D86" s="4">
@@ -6973,7 +7219,7 @@
         <v>3</v>
       </c>
       <c r="C87" s="4">
-        <f>potential_preg_untrt!C87*SimParameters!$B$6</f>
+        <f>potential_preg_untrt!C87*SimParameters!$B$13</f>
         <v>0</v>
       </c>
       <c r="D87" s="4">
@@ -6993,7 +7239,7 @@
         <v>4</v>
       </c>
       <c r="C88" s="4">
-        <f>potential_preg_untrt!C88*SimParameters!$B$6</f>
+        <f>potential_preg_untrt!C88*SimParameters!$B$13</f>
         <v>0</v>
       </c>
       <c r="D88" s="4">
@@ -7013,7 +7259,7 @@
         <v>5</v>
       </c>
       <c r="C89" s="4">
-        <f>potential_preg_untrt!C89*SimParameters!$B$6</f>
+        <f>potential_preg_untrt!C89*SimParameters!$B$13</f>
         <v>0</v>
       </c>
       <c r="D89" s="4">
@@ -7033,7 +7279,7 @@
         <v>6</v>
       </c>
       <c r="C90" s="4">
-        <f>potential_preg_untrt!C90*SimParameters!$B$6</f>
+        <f>potential_preg_untrt!C90*SimParameters!$B$13</f>
         <v>0</v>
       </c>
       <c r="D90" s="4">
@@ -7053,8 +7299,8 @@
         <v>7</v>
       </c>
       <c r="C91" s="4">
-        <f>potential_preg_untrt!C91*SimParameters!$B$6</f>
-        <v>0.12000000000000002</v>
+        <f>potential_preg_untrt!C91*SimParameters!$B$13</f>
+        <v>5.6249999999999994E-2</v>
       </c>
       <c r="D91" s="4">
         <f>potential_preg_untrt!D91</f>
@@ -7062,7 +7308,7 @@
       </c>
       <c r="E91" s="4">
         <f t="shared" si="2"/>
-        <v>0.88</v>
+        <v>0.94374999999999998</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -7073,8 +7319,8 @@
         <v>8</v>
       </c>
       <c r="C92" s="4">
-        <f>potential_preg_untrt!C92*SimParameters!$B$6</f>
-        <v>4.8000000000000001E-2</v>
+        <f>potential_preg_untrt!C92*SimParameters!$B$13</f>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="D92" s="4">
         <f>potential_preg_untrt!D92</f>
@@ -7082,7 +7328,7 @@
       </c>
       <c r="E92" s="4">
         <f t="shared" si="2"/>
-        <v>0.95199999999999996</v>
+        <v>0.97750000000000004</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -7093,8 +7339,8 @@
         <v>9</v>
       </c>
       <c r="C93" s="4">
-        <f>potential_preg_untrt!C93*SimParameters!$B$6</f>
-        <v>4.8000000000000001E-2</v>
+        <f>potential_preg_untrt!C93*SimParameters!$B$13</f>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="D93" s="4">
         <f>potential_preg_untrt!D93</f>
@@ -7102,7 +7348,7 @@
       </c>
       <c r="E93" s="4">
         <f t="shared" si="2"/>
-        <v>0.95199999999999996</v>
+        <v>0.97750000000000004</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -7113,7 +7359,7 @@
         <v>10</v>
       </c>
       <c r="C94" s="4">
-        <f>potential_preg_untrt!C94*SimParameters!$B$6</f>
+        <f>potential_preg_untrt!C94*SimParameters!$B$14</f>
         <v>2.4E-2</v>
       </c>
       <c r="D94" s="4">
@@ -7133,7 +7379,7 @@
         <v>11</v>
       </c>
       <c r="C95" s="4">
-        <f>potential_preg_untrt!C95*SimParameters!$B$6</f>
+        <f>potential_preg_untrt!C95*SimParameters!$B$14</f>
         <v>1.2E-2</v>
       </c>
       <c r="D95" s="4">
@@ -7153,7 +7399,7 @@
         <v>12</v>
       </c>
       <c r="C96" s="4">
-        <f>potential_preg_untrt!C96*SimParameters!$B$6</f>
+        <f>potential_preg_untrt!C96*SimParameters!$B$14</f>
         <v>9.6000000000000009E-3</v>
       </c>
       <c r="D96" s="4">
@@ -7173,7 +7419,7 @@
         <v>13</v>
       </c>
       <c r="C97" s="4">
-        <f>potential_preg_untrt!C97*SimParameters!$B$6</f>
+        <f>potential_preg_untrt!C97*SimParameters!$B$14</f>
         <v>9.6000000000000009E-3</v>
       </c>
       <c r="D97" s="4">
@@ -7193,8 +7439,8 @@
         <v>14</v>
       </c>
       <c r="C98" s="4">
-        <f>potential_preg_untrt!C98*SimParameters!$B$6</f>
-        <v>9.6000000000000009E-3</v>
+        <f>potential_preg_untrt!C98*SimParameters!$B$15</f>
+        <v>1.8239999999999999E-2</v>
       </c>
       <c r="D98" s="4">
         <f>potential_preg_untrt!D98</f>
@@ -7202,7 +7448,7 @@
       </c>
       <c r="E98" s="4">
         <f t="shared" si="2"/>
-        <v>0.99039999999999995</v>
+        <v>0.98175999999999997</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -7213,8 +7459,8 @@
         <v>15</v>
       </c>
       <c r="C99" s="4">
-        <f>potential_preg_untrt!C99*SimParameters!$B$6</f>
-        <v>9.6000000000000009E-3</v>
+        <f>potential_preg_untrt!C99*SimParameters!$B$15</f>
+        <v>1.8239999999999999E-2</v>
       </c>
       <c r="D99" s="4">
         <f>potential_preg_untrt!D99</f>
@@ -7222,7 +7468,7 @@
       </c>
       <c r="E99" s="4">
         <f t="shared" si="2"/>
-        <v>0.99039999999999995</v>
+        <v>0.98175999999999997</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -7233,8 +7479,8 @@
         <v>16</v>
       </c>
       <c r="C100" s="4">
-        <f>potential_preg_untrt!C100*SimParameters!$B$6</f>
-        <v>1.9200000000000003E-3</v>
+        <f>potential_preg_untrt!C100*SimParameters!$B$15</f>
+        <v>3.6479999999999998E-3</v>
       </c>
       <c r="D100" s="4">
         <f>potential_preg_untrt!D100</f>
@@ -7242,7 +7488,7 @@
       </c>
       <c r="E100" s="4">
         <f t="shared" si="2"/>
-        <v>0.99807999999999997</v>
+        <v>0.99635200000000002</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -7734,8 +7980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6870C18B-8ADE-814A-BF98-16981C435EF7}">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E119" sqref="E119:E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8071,7 +8317,7 @@
         <v>-7.9862248825409621</v>
       </c>
       <c r="E19" s="15">
-        <f>D19+LN(SimParameters!$B$25)</f>
+        <f>D19+LN(SimParameters!$B$55)</f>
         <v>-7.9862248825409621</v>
       </c>
       <c r="F19" s="15">
@@ -8094,7 +8340,7 @@
         <v>-7.7058128739195233</v>
       </c>
       <c r="E20" s="15">
-        <f>D20+LN(SimParameters!$B$25)</f>
+        <f>D20+LN(SimParameters!$B$55)</f>
         <v>-7.7058128739195233</v>
       </c>
       <c r="F20" s="15">
@@ -8117,7 +8363,7 @@
         <v>-7.7058128739195233</v>
       </c>
       <c r="E21" s="15">
-        <f>D21+LN(SimParameters!$B$25)</f>
+        <f>D21+LN(SimParameters!$B$55)</f>
         <v>-7.7058128739195233</v>
       </c>
       <c r="F21" s="15">
@@ -8140,7 +8386,7 @@
         <v>-6.7933059660064306</v>
       </c>
       <c r="E22" s="15">
-        <f>D22+LN(SimParameters!$B$25)</f>
+        <f>D22+LN(SimParameters!$B$55)</f>
         <v>-6.7933059660064306</v>
       </c>
       <c r="F22" s="15">
@@ -8163,7 +8409,7 @@
         <v>-6.699510352526949</v>
       </c>
       <c r="E23" s="15">
-        <f>D23+LN(SimParameters!$B$25)</f>
+        <f>D23+LN(SimParameters!$B$55)</f>
         <v>-6.699510352526949</v>
       </c>
       <c r="F23" s="15">
@@ -8186,7 +8432,7 @@
         <v>-6.5210217966814827</v>
       </c>
       <c r="E24" s="15">
-        <f>D24+LN(SimParameters!$B$25)</f>
+        <f>D24+LN(SimParameters!$B$55)</f>
         <v>-6.5210217966814827</v>
       </c>
       <c r="F24" s="15">
@@ -8209,7 +8455,7 @@
         <v>-6.5210217966814827</v>
       </c>
       <c r="E25" s="15">
-        <f>D25+LN(SimParameters!$B$25)</f>
+        <f>D25+LN(SimParameters!$B$55)</f>
         <v>-6.5210217966814827</v>
       </c>
       <c r="F25" s="15">
@@ -8232,7 +8478,7 @@
         <v>-6.3992762972870185</v>
       </c>
       <c r="E26" s="15">
-        <f>D26+LN(SimParameters!$B$25)</f>
+        <f>D26+LN(SimParameters!$B$55)</f>
         <v>-6.3992762972870185</v>
       </c>
       <c r="F26" s="15">
@@ -8255,7 +8501,7 @@
         <v>-5.796158059717027</v>
       </c>
       <c r="E27" s="15">
-        <f>D27+LN(SimParameters!$B$25)</f>
+        <f>D27+LN(SimParameters!$B$55)</f>
         <v>-5.796158059717027</v>
       </c>
       <c r="F27" s="15">
@@ -8278,7 +8524,7 @@
         <v>-5.3969379247357949</v>
       </c>
       <c r="E28" s="15">
-        <f>D28+LN(SimParameters!$B$25)</f>
+        <f>D28+LN(SimParameters!$B$55)</f>
         <v>-5.3969379247357949</v>
       </c>
       <c r="F28" s="15">
@@ -8301,7 +8547,7 @@
         <v>-5.3969379247357949</v>
       </c>
       <c r="E29" s="15">
-        <f>D29+LN(SimParameters!$B$25)</f>
+        <f>D29+LN(SimParameters!$B$55)</f>
         <v>-5.3969379247357949</v>
       </c>
       <c r="F29" s="15">
@@ -8324,7 +8570,7 @@
         <v>-5.096652024542192</v>
       </c>
       <c r="E30" s="15">
-        <f>D30+LN(SimParameters!$B$25)</f>
+        <f>D30+LN(SimParameters!$B$55)</f>
         <v>-5.096652024542192</v>
       </c>
       <c r="F30" s="15">
@@ -8347,7 +8593,7 @@
         <v>-4.3982016945728564</v>
       </c>
       <c r="E31" s="15">
-        <f>D31+LN(SimParameters!$B$25)</f>
+        <f>D31+LN(SimParameters!$B$55)</f>
         <v>-4.3982016945728564</v>
       </c>
       <c r="F31" s="15">
@@ -8370,7 +8616,7 @@
         <v>-3.9207910380006168</v>
       </c>
       <c r="E32" s="15">
-        <f>D32+LN(SimParameters!$B$25)</f>
+        <f>D32+LN(SimParameters!$B$55)</f>
         <v>-3.9207910380006168</v>
       </c>
       <c r="F32" s="15">
@@ -8393,7 +8639,7 @@
         <v>-3.6986002654815322</v>
       </c>
       <c r="E33" s="15">
-        <f>D33+LN(SimParameters!$B$25)</f>
+        <f>D33+LN(SimParameters!$B$55)</f>
         <v>-3.6986002654815322</v>
       </c>
       <c r="F33" s="15">
@@ -8416,7 +8662,7 @@
         <v>-3.6193733146385059</v>
       </c>
       <c r="E34" s="15">
-        <f>D34+LN(SimParameters!$B$25)</f>
+        <f>D34+LN(SimParameters!$B$55)</f>
         <v>-3.6193733146385059</v>
       </c>
       <c r="F34" s="15">
@@ -8439,7 +8685,7 @@
         <v>-2.2086096453965043</v>
       </c>
       <c r="E35" s="15">
-        <f>D35+LN(SimParameters!$B$25)</f>
+        <f>D35+LN(SimParameters!$B$55)</f>
         <v>-2.2086096453965043</v>
       </c>
       <c r="F35" s="15">
@@ -8462,7 +8708,7 @@
         <v>-2.0791490749458421</v>
       </c>
       <c r="E36" s="15">
-        <f>D36+LN(SimParameters!$B$25)</f>
+        <f>D36+LN(SimParameters!$B$55)</f>
         <v>-2.0791490749458421</v>
       </c>
       <c r="F36" s="15">
@@ -8485,7 +8731,7 @@
         <v>-1.9777396390105</v>
       </c>
       <c r="E37" s="15">
-        <f>D37+LN(SimParameters!$B$25)</f>
+        <f>D37+LN(SimParameters!$B$55)</f>
         <v>-1.9777396390105</v>
       </c>
       <c r="F37" s="15">
@@ -8508,7 +8754,7 @@
         <v>-1.8939038093591762</v>
       </c>
       <c r="E38" s="15">
-        <f>D38+LN(SimParameters!$B$25)</f>
+        <f>D38+LN(SimParameters!$B$55)</f>
         <v>-1.8939038093591762</v>
       </c>
       <c r="F38" s="15">
@@ -8531,7 +8777,7 @@
         <v>-1.6531772306954129</v>
       </c>
       <c r="E39" s="15">
-        <f>D39+LN(SimParameters!$B$25)</f>
+        <f>D39+LN(SimParameters!$B$55)</f>
         <v>-1.6531772306954129</v>
       </c>
       <c r="F39" s="15">
@@ -8554,7 +8800,7 @@
         <v>-1.524566929608417</v>
       </c>
       <c r="E40" s="15">
-        <f>D40+LN(SimParameters!$B$25)</f>
+        <f>D40+LN(SimParameters!$B$55)</f>
         <v>-1.524566929608417</v>
       </c>
       <c r="F40" s="15">
@@ -8577,7 +8823,7 @@
         <v>-1.4522859849692205</v>
       </c>
       <c r="E41" s="15">
-        <f>D41+LN(SimParameters!$B$25)</f>
+        <f>D41+LN(SimParameters!$B$55)</f>
         <v>-1.4522859849692205</v>
       </c>
       <c r="F41" s="15">
@@ -8600,7 +8846,7 @@
         <v>-1.3010402300365282</v>
       </c>
       <c r="E42" s="15">
-        <f>D42+LN(SimParameters!$B$25)</f>
+        <f>D42+LN(SimParameters!$B$55)</f>
         <v>-1.3010402300365282</v>
       </c>
       <c r="F42" s="15">
@@ -8930,12 +9176,12 @@
         <v>-7.9862248825409621</v>
       </c>
       <c r="E60" s="14">
-        <f>D60+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-7.5807597744327975</v>
+        <f>D60+LN(SimParameters!$B$55)+LN(SimParameters!$B$46)</f>
+        <v>-7.069934150666807</v>
       </c>
       <c r="F60" s="14">
         <f t="shared" si="2"/>
-        <v>5.0991331473649497E-4</v>
+        <v>8.4956672097230449E-4</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -8954,12 +9200,12 @@
         <v>-7.7058128739195233</v>
       </c>
       <c r="E61" s="14">
-        <f>D61+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-7.3003477658113587</v>
+        <f>D61+LN(SimParameters!$B$55)+LN(SimParameters!$B$46)</f>
+        <v>-6.7895221420453682</v>
       </c>
       <c r="F61" s="14">
         <f t="shared" si="2"/>
-        <v>6.7484815916418826E-4</v>
+        <v>1.1242411372323685E-3</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -8978,12 +9224,12 @@
         <v>-7.7058128739195233</v>
       </c>
       <c r="E62" s="14">
-        <f>D62+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-7.3003477658113587</v>
+        <f>D62+LN(SimParameters!$B$55)+LN(SimParameters!$B$46)</f>
+        <v>-6.7895221420453682</v>
       </c>
       <c r="F62" s="14">
         <f t="shared" si="2"/>
-        <v>6.7484815916418826E-4</v>
+        <v>1.1242411372323685E-3</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -9002,12 +9248,12 @@
         <v>-6.7933059660064306</v>
       </c>
       <c r="E63" s="14">
-        <f>D63+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-6.3878408578982659</v>
+        <f>D63+LN(SimParameters!$B$55)+LN(SimParameters!$B$46)</f>
+        <v>-5.8770152341322754</v>
       </c>
       <c r="F63" s="14">
         <f t="shared" si="2"/>
-        <v>1.6790597265531311E-3</v>
+        <v>2.7953038894656984E-3</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -9026,12 +9272,12 @@
         <v>-6.699510352526949</v>
       </c>
       <c r="E64" s="14">
-        <f>D64+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-6.2940452444187844</v>
+        <f>D64+LN(SimParameters!$B$55)+LN(SimParameters!$B$46)</f>
+        <v>-5.7832196206527939</v>
       </c>
       <c r="F64" s="14">
         <f t="shared" si="2"/>
-        <v>1.843866022396227E-3</v>
+        <v>3.0693370731001307E-3</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -9050,12 +9296,12 @@
         <v>-6.5210217966814827</v>
       </c>
       <c r="E65" s="14">
-        <f>D65+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-6.1155566885733181</v>
+        <f>D65+LN(SimParameters!$B$55)+LN(SimParameters!$B$46)</f>
+        <v>-5.6047310648073276</v>
       </c>
       <c r="F65" s="14">
         <f t="shared" si="2"/>
-        <v>2.2033805153212384E-3</v>
+        <v>3.6669144536297456E-3</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -9074,12 +9320,12 @@
         <v>-6.5210217966814827</v>
       </c>
       <c r="E66" s="14">
-        <f>D66+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-6.1155566885733181</v>
+        <f>D66+LN(SimParameters!$B$55)+LN(SimParameters!$B$46)</f>
+        <v>-5.6047310648073276</v>
       </c>
       <c r="F66" s="14">
         <f t="shared" si="2"/>
-        <v>2.2033805153212384E-3</v>
+        <v>3.6669144536297456E-3</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -9098,12 +9344,12 @@
         <v>-6.3992762972870185</v>
       </c>
       <c r="E67" s="14">
-        <f>D67+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-5.9938111891788539</v>
+        <f>D67+LN(SimParameters!$B$55)+LN(SimParameters!$B$46)</f>
+        <v>-5.4829855654128634</v>
       </c>
       <c r="F67" s="14">
         <f t="shared" si="2"/>
-        <v>2.487935013938433E-3</v>
+        <v>4.1396921665054036E-3</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -9122,12 +9368,12 @@
         <v>-5.796158059717027</v>
       </c>
       <c r="E68" s="14">
-        <f>D68+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-5.3906929516088624</v>
+        <f>D68+LN(SimParameters!$B$55)+LN(SimParameters!$B$46)</f>
+        <v>-4.8798673278428719</v>
       </c>
       <c r="F68" s="14">
         <f t="shared" si="2"/>
-        <v>4.5381247410173587E-3</v>
+        <v>7.5407273939942943E-3</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -9146,12 +9392,12 @@
         <v>-5.3969379247357949</v>
       </c>
       <c r="E69" s="14">
-        <f>D69+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-4.9914728166276303</v>
+        <f>D69+LN(SimParameters!$B$55)+LN(SimParameters!$B$47)</f>
+        <v>-4.8373221368003723</v>
       </c>
       <c r="F69" s="14">
         <f t="shared" si="2"/>
-        <v>6.7497792477962219E-3</v>
+        <v>7.8658936148477791E-3</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -9170,12 +9416,12 @@
         <v>-5.3969379247357949</v>
       </c>
       <c r="E70" s="14">
-        <f>D70+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-4.9914728166276303</v>
+        <f>D70+LN(SimParameters!$B$55)+LN(SimParameters!$B$47)</f>
+        <v>-4.8373221368003723</v>
       </c>
       <c r="F70" s="14">
         <f t="shared" si="2"/>
-        <v>6.7497792477962219E-3</v>
+        <v>7.8658936148477791E-3</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -9194,12 +9440,12 @@
         <v>-5.096652024542192</v>
       </c>
       <c r="E71" s="14">
-        <f>D71+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-4.6911869164340274</v>
+        <f>D71+LN(SimParameters!$B$55)+LN(SimParameters!$B$47)</f>
+        <v>-4.5370362366067694</v>
       </c>
       <c r="F71" s="14">
         <f t="shared" si="2"/>
-        <v>9.092359227947041E-3</v>
+        <v>1.059170183961137E-2</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -9218,12 +9464,12 @@
         <v>-4.3982016945728564</v>
       </c>
       <c r="E72" s="14">
-        <f>D72+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-3.9927365864646918</v>
+        <f>D72+LN(SimParameters!$B$55)+LN(SimParameters!$B$47)</f>
+        <v>-3.8385859066374337</v>
       </c>
       <c r="F72" s="14">
         <f t="shared" si="2"/>
-        <v>1.8114951668613183E-2</v>
+        <v>2.1070495113280241E-2</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -9242,12 +9488,12 @@
         <v>-3.9207910380006168</v>
       </c>
       <c r="E73" s="14">
-        <f>D73+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-3.5153259298924526</v>
+        <f>D73+LN(SimParameters!$B$55)+LN(SimParameters!$B$47)</f>
+        <v>-3.3611752500651941</v>
       </c>
       <c r="F73" s="14">
         <f t="shared" si="2"/>
-        <v>2.8879293269421218E-2</v>
+        <v>3.3531116323996135E-2</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -9266,12 +9512,12 @@
         <v>-3.6986002654815322</v>
       </c>
       <c r="E74" s="14">
-        <f>D74+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-3.293135157373368</v>
+        <f>D74+LN(SimParameters!$B$55)+LN(SimParameters!$B$47)</f>
+        <v>-3.1389844775461095</v>
       </c>
       <c r="F74" s="14">
         <f t="shared" si="2"/>
-        <v>3.5807446051695509E-2</v>
+        <v>4.1527521313794037E-2</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -9290,12 +9536,12 @@
         <v>-3.6193733146385059</v>
       </c>
       <c r="E75" s="14">
-        <f>D75+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-3.2139082065303413</v>
+        <f>D75+LN(SimParameters!$B$55)+LN(SimParameters!$B$47)</f>
+        <v>-3.0597575267030832</v>
       </c>
       <c r="F75" s="14">
         <f t="shared" si="2"/>
-        <v>3.8645673954888708E-2</v>
+        <v>4.4798077630385208E-2</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -9314,12 +9560,12 @@
         <v>-2.2086096453965043</v>
       </c>
       <c r="E76" s="14">
-        <f>D76+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-1.8031445372883399</v>
+        <f>D76+LN(SimParameters!$B$55)+LN(SimParameters!$B$47)</f>
+        <v>-1.6489938574610816</v>
       </c>
       <c r="F76" s="14">
         <f t="shared" si="2"/>
-        <v>0.14146871337506789</v>
+        <v>0.16124497898504517</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -9338,12 +9584,12 @@
         <v>-2.0791490749458421</v>
       </c>
       <c r="E77" s="14">
-        <f>D77+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-1.6736839668376777</v>
+        <f>D77+LN(SimParameters!$B$55)+LN(SimParameters!$B$47)</f>
+        <v>-1.5195332870104195</v>
       </c>
       <c r="F77" s="14">
         <f t="shared" si="2"/>
-        <v>0.15793362827666566</v>
+        <v>0.17953025554873517</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -9362,12 +9608,12 @@
         <v>-1.9777396390105</v>
       </c>
       <c r="E78" s="14">
-        <f>D78+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-1.5722745309023356</v>
+        <f>D78+LN(SimParameters!$B$55)+LN(SimParameters!$B$48)</f>
+        <v>-1.7545960876962903</v>
       </c>
       <c r="F78" s="14">
         <f t="shared" si="2"/>
-        <v>0.17189238107807461</v>
+        <v>0.14746843428216497</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -9386,12 +9632,12 @@
         <v>-1.8939038093591762</v>
       </c>
       <c r="E79" s="14">
-        <f>D79+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-1.4884387012510119</v>
+        <f>D79+LN(SimParameters!$B$55)+LN(SimParameters!$B$48)</f>
+        <v>-1.6707602580449665</v>
       </c>
       <c r="F79" s="14">
         <f t="shared" si="2"/>
-        <v>0.18415618547024593</v>
+        <v>0.15832284303282657</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -9410,12 +9656,12 @@
         <v>-1.6531772306954129</v>
       </c>
       <c r="E80" s="14">
-        <f>D80+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-1.2477121225872485</v>
+        <f>D80+LN(SimParameters!$B$55)+LN(SimParameters!$B$48)</f>
+        <v>-1.4300336793812032</v>
       </c>
       <c r="F80" s="14">
         <f t="shared" si="2"/>
-        <v>0.22309643260455042</v>
+        <v>0.19309343664977838</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -9434,12 +9680,12 @@
         <v>-1.524566929608417</v>
       </c>
       <c r="E81" s="14">
-        <f>D81+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-1.1191018215002526</v>
+        <f>D81+LN(SimParameters!$B$55)+LN(SimParameters!$B$48)</f>
+        <v>-1.3014233782942073</v>
       </c>
       <c r="F81" s="14">
         <f t="shared" si="2"/>
-        <v>0.24617792444430164</v>
+        <v>0.21392556218426864</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -9458,12 +9704,12 @@
         <v>-1.4522859849692205</v>
       </c>
       <c r="E82" s="14">
-        <f>D82+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-1.0468208768610561</v>
+        <f>D82+LN(SimParameters!$B$55)+LN(SimParameters!$B$48)</f>
+        <v>-1.2291424336550107</v>
       </c>
       <c r="F82" s="14">
         <f t="shared" si="2"/>
-        <v>0.25983604685680362</v>
+        <v>0.22633155514183764</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -9482,12 +9728,12 @@
         <v>-1.3010402300365282</v>
       </c>
       <c r="E83" s="14">
-        <f>D83+LN(SimParameters!$B$25)+LN(SimParameters!$B$21)</f>
-        <v>-0.89557512192836386</v>
+        <f>D83+LN(SimParameters!$B$55)+LN(SimParameters!$B$48)</f>
+        <v>-1.0778966787223185</v>
       </c>
       <c r="F83" s="14">
         <f t="shared" si="2"/>
-        <v>0.28996065926223696</v>
+        <v>0.25390425701057667</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -9812,12 +10058,12 @@
         <v>-7.9862248825409621</v>
       </c>
       <c r="E101" s="13">
-        <f>D101+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-7.2930777019810167</v>
+        <f>D101+LN(SimParameters!$B$55)+LN(SimParameters!$B$50)</f>
+        <v>-6.5999305214210713</v>
       </c>
       <c r="F101" s="13">
         <f t="shared" ref="F101:F124" si="9">EXP(E101)/(1+EXP(E101))</f>
-        <v>6.7976887858128268E-4</v>
+        <v>1.3586142135022284E-3</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -9836,12 +10082,12 @@
         <v>-7.7058128739195233</v>
       </c>
       <c r="E102" s="13">
-        <f>D102+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-7.0126656933595779</v>
+        <f>D102+LN(SimParameters!$B$55)+LN(SimParameters!$B$50)</f>
+        <v>-6.3195185127996325</v>
       </c>
       <c r="F102" s="13">
         <f t="shared" si="9"/>
-        <v>8.9959518216802458E-4</v>
+        <v>1.7975732760772962E-3</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -9860,12 +10106,12 @@
         <v>-7.7058128739195233</v>
       </c>
       <c r="E103" s="13">
-        <f>D103+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-7.0126656933595779</v>
+        <f>D103+LN(SimParameters!$B$55)+LN(SimParameters!$B$50)</f>
+        <v>-6.3195185127996325</v>
       </c>
       <c r="F103" s="13">
         <f t="shared" si="9"/>
-        <v>8.9959518216802458E-4</v>
+        <v>1.7975732760772962E-3</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -9884,12 +10130,12 @@
         <v>-6.7933059660064306</v>
       </c>
       <c r="E104" s="13">
-        <f>D104+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-6.1001587854464852</v>
+        <f>D104+LN(SimParameters!$B$55)+LN(SimParameters!$B$50)</f>
+        <v>-5.4070116048865398</v>
       </c>
       <c r="F104" s="13">
         <f t="shared" si="9"/>
-        <v>2.237494006712483E-3</v>
+        <v>4.4649976080369976E-3</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -9908,12 +10154,12 @@
         <v>-6.699510352526949</v>
       </c>
       <c r="E105" s="13">
-        <f>D105+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-6.0063631719670036</v>
+        <f>D105+LN(SimParameters!$B$55)+LN(SimParameters!$B$50)</f>
+        <v>-5.3132159914070582</v>
       </c>
       <c r="F105" s="13">
         <f t="shared" si="9"/>
-        <v>2.456977917161892E-3</v>
+        <v>4.9019119449232344E-3</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -9932,12 +10178,12 @@
         <v>-6.5210217966814827</v>
       </c>
       <c r="E106" s="13">
-        <f>D106+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-5.8278746161215373</v>
+        <f>D106+LN(SimParameters!$B$55)+LN(SimParameters!$B$50)</f>
+        <v>-5.1347274355615919</v>
       </c>
       <c r="F106" s="13">
         <f t="shared" si="9"/>
-        <v>2.9356845437207299E-3</v>
+        <v>5.8541830527374262E-3</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -9956,12 +10202,12 @@
         <v>-6.5210217966814827</v>
       </c>
       <c r="E107" s="13">
-        <f>D107+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-5.8278746161215373</v>
+        <f>D107+LN(SimParameters!$B$55)+LN(SimParameters!$B$50)</f>
+        <v>-5.1347274355615919</v>
       </c>
       <c r="F107" s="13">
         <f t="shared" si="9"/>
-        <v>2.9356845437207299E-3</v>
+        <v>5.8541830527374262E-3</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -9980,12 +10226,12 @@
         <v>-6.3992762972870185</v>
       </c>
       <c r="E108" s="13">
-        <f>D108+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-5.7061291167270731</v>
+        <f>D108+LN(SimParameters!$B$55)+LN(SimParameters!$B$50)</f>
+        <v>-5.0129819361671277</v>
       </c>
       <c r="F108" s="13">
         <f t="shared" si="9"/>
-        <v>3.3144979334305074E-3</v>
+        <v>6.6070966586399766E-3</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -10004,12 +10250,12 @@
         <v>-5.796158059717027</v>
       </c>
       <c r="E109" s="13">
-        <f>D109+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-5.1030108791570816</v>
+        <f>D109+LN(SimParameters!$B$55)+LN(SimParameters!$B$50)</f>
+        <v>-4.4098636985971362</v>
       </c>
       <c r="F109" s="13">
         <f t="shared" si="9"/>
-        <v>6.0416936681853984E-3</v>
+        <v>1.2010821631370839E-2</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -10028,12 +10274,12 @@
         <v>-5.3969379247357949</v>
       </c>
       <c r="E110" s="13">
-        <f>D110+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-4.7037907441758495</v>
+        <f>D110+LN(SimParameters!$B$55)+LN(SimParameters!$B$51)</f>
+        <v>-4.4414264797083582</v>
       </c>
       <c r="F110" s="13">
         <f t="shared" si="9"/>
-        <v>8.9795024439776622E-3</v>
+        <v>1.1641991390128838E-2</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -10052,12 +10298,12 @@
         <v>-5.3969379247357949</v>
       </c>
       <c r="E111" s="13">
-        <f>D111+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-4.7037907441758495</v>
+        <f>D111+LN(SimParameters!$B$55)+LN(SimParameters!$B$51)</f>
+        <v>-4.4414264797083582</v>
       </c>
       <c r="F111" s="13">
         <f t="shared" si="9"/>
-        <v>8.9795024439776622E-3</v>
+        <v>1.1641991390128838E-2</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -10076,12 +10322,12 @@
         <v>-5.096652024542192</v>
       </c>
       <c r="E112" s="13">
-        <f>D112+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-4.4035048439822466</v>
+        <f>D112+LN(SimParameters!$B$55)+LN(SimParameters!$B$51)</f>
+        <v>-4.1411405795147553</v>
       </c>
       <c r="F112" s="13">
         <f t="shared" si="9"/>
-        <v>1.2086513994910942E-2</v>
+        <v>1.5655701337389877E-2</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -10100,12 +10346,12 @@
         <v>-4.3982016945728564</v>
       </c>
       <c r="E113" s="13">
-        <f>D113+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-3.705054514012911</v>
+        <f>D113+LN(SimParameters!$B$55)+LN(SimParameters!$B$51)</f>
+        <v>-3.4426902495454201</v>
       </c>
       <c r="F113" s="13">
         <f t="shared" si="9"/>
-        <v>2.400829916514351E-2</v>
+        <v>3.0987601035862834E-2</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -10124,12 +10370,12 @@
         <v>-3.9207910380006168</v>
       </c>
       <c r="E114" s="13">
-        <f>D114+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-3.2276438574406714</v>
+        <f>D114+LN(SimParameters!$B$55)+LN(SimParameters!$B$51)</f>
+        <v>-2.9652795929731806</v>
       </c>
       <c r="F114" s="13">
         <f t="shared" si="9"/>
-        <v>3.813858589029271E-2</v>
+        <v>4.9019303581404002E-2</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -10148,12 +10394,12 @@
         <v>-3.6986002654815322</v>
       </c>
       <c r="E115" s="13">
-        <f>D115+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-3.0054530849215868</v>
+        <f>D115+LN(SimParameters!$B$55)+LN(SimParameters!$B$51)</f>
+        <v>-2.743088820454096</v>
       </c>
       <c r="F115" s="13">
         <f t="shared" si="9"/>
-        <v>4.7180128104983593E-2</v>
+        <v>6.047815638671513E-2</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -10172,12 +10418,12 @@
         <v>-3.6193733146385059</v>
       </c>
       <c r="E116" s="13">
-        <f>D116+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-2.9262261340785605</v>
+        <f>D116+LN(SimParameters!$B$55)+LN(SimParameters!$B$51)</f>
+        <v>-2.6638618696110696</v>
       </c>
       <c r="F116" s="13">
         <f t="shared" si="9"/>
-        <v>5.0872234674982947E-2</v>
+        <v>6.5139763477192428E-2</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -10196,12 +10442,12 @@
         <v>-2.2086096453965043</v>
       </c>
       <c r="E117" s="13">
-        <f>D117+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-1.5154624648365589</v>
+        <f>D117+LN(SimParameters!$B$55)+LN(SimParameters!$B$51)</f>
+        <v>-1.253098200369068</v>
       </c>
       <c r="F117" s="13">
         <f t="shared" si="9"/>
-        <v>0.18013066661813684</v>
+        <v>0.22216428630625154</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -10220,12 +10466,12 @@
         <v>-2.0791490749458421</v>
       </c>
       <c r="E118" s="13">
-        <f>D118+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-1.3860018943858967</v>
+        <f>D118+LN(SimParameters!$B$55)+LN(SimParameters!$B$51)</f>
+        <v>-1.1236376299184059</v>
       </c>
       <c r="F118" s="13">
         <f t="shared" si="9"/>
-        <v>0.20004679878323164</v>
+        <v>0.24533716412638895</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -10244,12 +10490,12 @@
         <v>-1.9777396390105</v>
       </c>
       <c r="E119" s="13">
-        <f>D119+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-1.2845924584505548</v>
+        <f>D119+LN(SimParameters!$B$55)+LN(SimParameters!$B$52)</f>
+        <v>-1.4181238510750773</v>
       </c>
       <c r="F119" s="13">
         <f t="shared" si="9"/>
-        <v>0.21676949962552158</v>
+        <v>0.19495587305369466</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -10268,12 +10514,12 @@
         <v>-1.8939038093591762</v>
       </c>
       <c r="E120" s="13">
-        <f>D120+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-1.2007566287992311</v>
+        <f>D120+LN(SimParameters!$B$55)+LN(SimParameters!$B$52)</f>
+        <v>-1.3342880214237536</v>
       </c>
       <c r="F120" s="13">
         <f t="shared" si="9"/>
-        <v>0.23134064379200564</v>
+        <v>0.20845096075038702</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -10292,12 +10538,12 @@
         <v>-1.6531772306954129</v>
       </c>
       <c r="E121" s="13">
-        <f>D121+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-0.96003005013546761</v>
+        <f>D121+LN(SimParameters!$B$55)+LN(SimParameters!$B$52)</f>
+        <v>-1.0935614427599902</v>
       </c>
       <c r="F121" s="13">
         <f t="shared" si="9"/>
-        <v>0.27687217837819206</v>
+        <v>0.25094822893146868</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -10316,12 +10562,12 @@
         <v>-1.524566929608417</v>
       </c>
       <c r="E122" s="13">
-        <f>D122+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-0.83141974904847171</v>
+        <f>D122+LN(SimParameters!$B$55)+LN(SimParameters!$B$52)</f>
+        <v>-0.96495114167299434</v>
       </c>
       <c r="F122" s="13">
         <f t="shared" si="9"/>
-        <v>0.3033449554203887</v>
+        <v>0.27588798973628692</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -10340,12 +10586,12 @@
         <v>-1.4522859849692205</v>
       </c>
       <c r="E123" s="13">
-        <f>D123+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-0.75913880440927517</v>
+        <f>D123+LN(SimParameters!$B$55)+LN(SimParameters!$B$52)</f>
+        <v>-0.8926701970337978</v>
       </c>
       <c r="F123" s="13">
         <f t="shared" si="9"/>
-        <v>0.31883327028958103</v>
+        <v>0.29055910001203777</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -10364,12 +10610,12 @@
         <v>-1.3010402300365282</v>
       </c>
       <c r="E124" s="13">
-        <f>D124+LN(SimParameters!$B$25)+LN(SimParameters!$B$22)</f>
-        <v>-0.60789304947658296</v>
+        <f>D124+LN(SimParameters!$B$55)+LN(SimParameters!$B$52)</f>
+        <v>-0.74142444210110559</v>
       </c>
       <c r="F124" s="13">
         <f t="shared" si="9"/>
-        <v>0.35253997149894151</v>
+        <v>0.32269273605818222</v>
       </c>
     </row>
   </sheetData>
@@ -10382,8 +10628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBCDA1E-E196-5243-A50A-855DF45BB886}">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E122" sqref="E122"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="E119" sqref="E119:E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10423,7 +10669,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <f>potential_preec_untrt!C2*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C2*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D2" s="11"/>
@@ -10441,7 +10687,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <f>potential_preec_untrt!C3*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C3*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D3" s="11"/>
@@ -10459,7 +10705,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <f>potential_preec_untrt!C4*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C4*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D4" s="11"/>
@@ -10477,7 +10723,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2">
-        <f>potential_preec_untrt!C5*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C5*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D5" s="11"/>
@@ -10495,7 +10741,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="2">
-        <f>potential_preec_untrt!C6*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C6*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D6" s="11"/>
@@ -10513,7 +10759,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="2">
-        <f>potential_preec_untrt!C7*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C7*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D7" s="11"/>
@@ -10531,7 +10777,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="2">
-        <f>potential_preec_untrt!C8*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C8*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D8" s="11"/>
@@ -10549,7 +10795,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="2">
-        <f>potential_preec_untrt!C9*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C9*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D9" s="11"/>
@@ -10567,7 +10813,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2">
-        <f>potential_preec_untrt!C10*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C10*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D10" s="11"/>
@@ -10585,7 +10831,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="2">
-        <f>potential_preec_untrt!C11*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C11*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D11" s="11"/>
@@ -10603,7 +10849,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="2">
-        <f>potential_preec_untrt!C12*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C12*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D12" s="11"/>
@@ -10621,7 +10867,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="2">
-        <f>potential_preec_untrt!C13*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C13*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D13" s="11"/>
@@ -10639,7 +10885,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="2">
-        <f>potential_preec_untrt!C14*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C14*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D14" s="11"/>
@@ -10657,7 +10903,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="2">
-        <f>potential_preec_untrt!C15*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C15*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D15" s="11"/>
@@ -10675,7 +10921,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="2">
-        <f>potential_preec_untrt!C16*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C16*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D16" s="11"/>
@@ -10693,7 +10939,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="2">
-        <f>potential_preec_untrt!C17*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C17*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D17" s="11"/>
@@ -10711,7 +10957,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="2">
-        <f>potential_preec_untrt!C18*SimParameters!$B$8</f>
+        <f>potential_preec_untrt!C18*SimParameters!$B$18</f>
         <v>0</v>
       </c>
       <c r="D18" s="11"/>
@@ -10737,12 +10983,12 @@
         <v>-7.9862248825409621</v>
       </c>
       <c r="E19" s="15">
-        <f>D19+LN(SimParameters!$B$8)</f>
-        <v>-9.5956627949750626</v>
+        <f>D19+LN(SimParameters!$B$18)</f>
+        <v>-9.8833448674268425</v>
       </c>
       <c r="F19" s="15">
         <f>EXP(E19)/(1+EXP(E19))</f>
-        <v>6.801850103228078E-5</v>
+        <v>5.1014743260802429E-5</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -10761,12 +11007,12 @@
         <v>-7.7058128739195233</v>
       </c>
       <c r="E20" s="15">
-        <f>D20+LN(SimParameters!$B$8)</f>
-        <v>-9.3152507863536229</v>
+        <f>D20+LN(SimParameters!$B$18)</f>
+        <v>-9.6029328588054046</v>
       </c>
       <c r="F20" s="15">
         <f t="shared" ref="F20:F83" si="2">EXP(E20)/(1+EXP(E20))</f>
-        <v>9.0032411668200635E-5</v>
+        <v>6.7525828629450783E-5</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -10785,12 +11031,12 @@
         <v>-7.7058128739195233</v>
       </c>
       <c r="E21" s="15">
-        <f>D21+LN(SimParameters!$B$8)</f>
-        <v>-9.3152507863536229</v>
+        <f>D21+LN(SimParameters!$B$18)</f>
+        <v>-9.6029328588054046</v>
       </c>
       <c r="F21" s="15">
         <f t="shared" si="2"/>
-        <v>9.0032411668200635E-5</v>
+        <v>6.7525828629450783E-5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -10809,12 +11055,12 @@
         <v>-6.7933059660064306</v>
       </c>
       <c r="E22" s="15">
-        <f>D22+LN(SimParameters!$B$8)</f>
-        <v>-8.4027438784405302</v>
+        <f>D22+LN(SimParameters!$B$18)</f>
+        <v>-8.6904259508923118</v>
       </c>
       <c r="F22" s="15">
         <f t="shared" si="2"/>
-        <v>2.242008839920571E-4</v>
+        <v>1.681600884041608E-4</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -10833,12 +11079,12 @@
         <v>-6.699510352526949</v>
       </c>
       <c r="E23" s="15">
-        <f>D23+LN(SimParameters!$B$8)</f>
-        <v>-8.3089482649610495</v>
+        <f>D23+LN(SimParameters!$B$18)</f>
+        <v>-8.5966303374128294</v>
       </c>
       <c r="F23" s="15">
         <f t="shared" si="2"/>
-        <v>2.4624230242558672E-4</v>
+        <v>1.8469309663252949E-4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -10857,12 +11103,12 @@
         <v>-6.5210217966814827</v>
       </c>
       <c r="E24" s="15">
-        <f>D24+LN(SimParameters!$B$8)</f>
-        <v>-8.1304597091155824</v>
+        <f>D24+LN(SimParameters!$B$18)</f>
+        <v>-8.418141781567364</v>
       </c>
       <c r="F24" s="15">
         <f t="shared" si="2"/>
-        <v>2.9434615107366271E-4</v>
+        <v>2.2077585943636562E-4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -10881,12 +11127,12 @@
         <v>-6.5210217966814827</v>
       </c>
       <c r="E25" s="15">
-        <f>D25+LN(SimParameters!$B$8)</f>
-        <v>-8.1304597091155824</v>
+        <f>D25+LN(SimParameters!$B$18)</f>
+        <v>-8.418141781567364</v>
       </c>
       <c r="F25" s="15">
         <f t="shared" si="2"/>
-        <v>2.9434615107366271E-4</v>
+        <v>2.2077585943636562E-4</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -10905,12 +11151,12 @@
         <v>-6.3992762972870185</v>
       </c>
       <c r="E26" s="15">
-        <f>D26+LN(SimParameters!$B$8)</f>
-        <v>-8.0087142097211181</v>
+        <f>D26+LN(SimParameters!$B$18)</f>
+        <v>-8.2963962821728998</v>
       </c>
       <c r="F26" s="15">
         <f t="shared" si="2"/>
-        <v>3.3244148228847955E-4</v>
+        <v>2.4935183543980569E-4</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -10929,12 +11175,12 @@
         <v>-5.796158059717027</v>
       </c>
       <c r="E27" s="15">
-        <f>D27+LN(SimParameters!$B$8)</f>
-        <v>-7.4055959721511275</v>
+        <f>D27+LN(SimParameters!$B$18)</f>
+        <v>-7.6932780446029083</v>
       </c>
       <c r="F27" s="15">
         <f t="shared" si="2"/>
-        <v>6.0747251337241453E-4</v>
+        <v>4.5567358732415331E-4</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -10953,7 +11199,7 @@
         <v>-5.3969379247357949</v>
       </c>
       <c r="E28" s="15">
-        <f>D28+LN(SimParameters!$B$8)</f>
+        <f>D28+LN(SimParameters!$B$19)</f>
         <v>-7.0063758371698954</v>
       </c>
       <c r="F28" s="15">
@@ -10977,7 +11223,7 @@
         <v>-5.3969379247357949</v>
       </c>
       <c r="E29" s="15">
-        <f>D29+LN(SimParameters!$B$8)</f>
+        <f>D29+LN(SimParameters!$B$19)</f>
         <v>-7.0063758371698954</v>
       </c>
       <c r="F29" s="15">
@@ -11001,7 +11247,7 @@
         <v>-5.096652024542192</v>
       </c>
       <c r="E30" s="15">
-        <f>D30+LN(SimParameters!$B$8)</f>
+        <f>D30+LN(SimParameters!$B$19)</f>
         <v>-6.7060899369762925</v>
       </c>
       <c r="F30" s="15">
@@ -11025,7 +11271,7 @@
         <v>-4.3982016945728564</v>
       </c>
       <c r="E31" s="15">
-        <f>D31+LN(SimParameters!$B$8)</f>
+        <f>D31+LN(SimParameters!$B$19)</f>
         <v>-6.0076396070069569</v>
       </c>
       <c r="F31" s="15">
@@ -11049,7 +11295,7 @@
         <v>-3.9207910380006168</v>
       </c>
       <c r="E32" s="15">
-        <f>D32+LN(SimParameters!$B$8)</f>
+        <f>D32+LN(SimParameters!$B$19)</f>
         <v>-5.5302289504347169</v>
       </c>
       <c r="F32" s="15">
@@ -11073,7 +11319,7 @@
         <v>-3.6986002654815322</v>
       </c>
       <c r="E33" s="15">
-        <f>D33+LN(SimParameters!$B$8)</f>
+        <f>D33+LN(SimParameters!$B$19)</f>
         <v>-5.3080381779156323</v>
       </c>
       <c r="F33" s="15">
@@ -11097,7 +11343,7 @@
         <v>-3.6193733146385059</v>
       </c>
       <c r="E34" s="15">
-        <f>D34+LN(SimParameters!$B$8)</f>
+        <f>D34+LN(SimParameters!$B$19)</f>
         <v>-5.2288112270726064</v>
       </c>
       <c r="F34" s="15">
@@ -11121,7 +11367,7 @@
         <v>-2.2086096453965043</v>
       </c>
       <c r="E35" s="15">
-        <f>D35+LN(SimParameters!$B$8)</f>
+        <f>D35+LN(SimParameters!$B$19)</f>
         <v>-3.8180475578306048</v>
       </c>
       <c r="F35" s="15">
@@ -11145,7 +11391,7 @@
         <v>-2.0791490749458421</v>
       </c>
       <c r="E36" s="15">
-        <f>D36+LN(SimParameters!$B$8)</f>
+        <f>D36+LN(SimParameters!$B$19)</f>
         <v>-3.6885869873799422</v>
       </c>
       <c r="F36" s="15">
@@ -11169,12 +11415,12 @@
         <v>-1.9777396390105</v>
       </c>
       <c r="E37" s="15">
-        <f>D37+LN(SimParameters!$B$8)</f>
-        <v>-3.5871775514446003</v>
+        <f>D37+LN(SimParameters!$B$20)</f>
+        <v>-3.1817124433364361</v>
       </c>
       <c r="F37" s="15">
         <f t="shared" si="2"/>
-        <v>2.6930984367799796E-2</v>
+        <v>3.9859745460745777E-2</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -11193,12 +11439,12 @@
         <v>-1.8939038093591762</v>
       </c>
       <c r="E38" s="15">
-        <f>D38+LN(SimParameters!$B$8)</f>
-        <v>-3.5033417217932765</v>
+        <f>D38+LN(SimParameters!$B$20)</f>
+        <v>-3.0978766136851124</v>
       </c>
       <c r="F38" s="15">
         <f t="shared" si="2"/>
-        <v>2.9217298070050034E-2</v>
+        <v>4.3194927568138787E-2</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -11217,12 +11463,12 @@
         <v>-1.6531772306954129</v>
       </c>
       <c r="E39" s="15">
-        <f>D39+LN(SimParameters!$B$8)</f>
-        <v>-3.262615143129513</v>
+        <f>D39+LN(SimParameters!$B$20)</f>
+        <v>-2.8571500350213492</v>
       </c>
       <c r="F39" s="15">
         <f t="shared" si="2"/>
-        <v>3.6876216355157358E-2</v>
+        <v>5.4312897454040665E-2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -11241,12 +11487,12 @@
         <v>-1.5245669296084168</v>
       </c>
       <c r="E40" s="15">
-        <f>D40+LN(SimParameters!$B$8)</f>
-        <v>-3.1340048420425171</v>
+        <f>D40+LN(SimParameters!$B$20)</f>
+        <v>-2.7285397339343529</v>
       </c>
       <c r="F40" s="15">
         <f t="shared" si="2"/>
-        <v>4.1726178807143341E-2</v>
+        <v>6.1310149088926416E-2</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -11265,12 +11511,12 @@
         <v>-1.4522859849692202</v>
       </c>
       <c r="E41" s="15">
-        <f>D41+LN(SimParameters!$B$8)</f>
-        <v>-3.0617238974033203</v>
+        <f>D41+LN(SimParameters!$B$20)</f>
+        <v>-2.6562587892951566</v>
       </c>
       <c r="F41" s="15">
         <f t="shared" si="2"/>
-        <v>4.471400952515682E-2</v>
+        <v>6.5604298669926023E-2</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -11289,12 +11535,12 @@
         <v>-1.3010402300365285</v>
       </c>
       <c r="E42" s="15">
-        <f>D42+LN(SimParameters!$B$8)</f>
-        <v>-2.9104781424706285</v>
+        <f>D42+LN(SimParameters!$B$20)</f>
+        <v>-2.5050130343624648</v>
       </c>
       <c r="F42" s="15">
         <f t="shared" si="2"/>
-        <v>5.1638015077074557E-2</v>
+        <v>7.5507494057329538E-2</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -11612,19 +11858,19 @@
       </c>
       <c r="C60" s="3">
         <f>potential_preec_untrt!F60</f>
-        <v>5.0991331473649497E-4</v>
+        <v>8.4956672097230449E-4</v>
       </c>
       <c r="D60" s="14">
         <f>LN(C60/(1-C60))</f>
-        <v>-7.5807597744327975</v>
+        <v>-7.069934150666807</v>
       </c>
       <c r="E60" s="14">
-        <f>D60+LN(SimParameters!$B$9)</f>
-        <v>-8.2739069549927429</v>
+        <f>D60+LN(SimParameters!$B$22)</f>
+        <v>-8.050763403678534</v>
       </c>
       <c r="F60" s="14">
         <f t="shared" si="2"/>
-        <v>2.5502167684253175E-4</v>
+        <v>3.1875677358143839E-4</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -11636,19 +11882,19 @@
       </c>
       <c r="C61" s="3">
         <f>potential_preec_untrt!F61</f>
-        <v>6.7484815916418826E-4</v>
+        <v>1.1242411372323685E-3</v>
       </c>
       <c r="D61" s="14">
         <f t="shared" ref="D61:D83" si="4">LN(C61/(1-C61))</f>
-        <v>-7.3003477658113587</v>
+        <v>-6.7895221420453682</v>
       </c>
       <c r="E61" s="14">
-        <f>D61+LN(SimParameters!$B$9)</f>
-        <v>-7.9934949463713041</v>
+        <f>D61+LN(SimParameters!$B$22)</f>
+        <v>-7.7703513950570944</v>
       </c>
       <c r="F61" s="14">
         <f t="shared" si="2"/>
-        <v>3.3753797302196509E-4</v>
+        <v>4.218868655680942E-4</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -11660,19 +11906,19 @@
       </c>
       <c r="C62" s="3">
         <f>potential_preec_untrt!F62</f>
-        <v>6.7484815916418826E-4</v>
+        <v>1.1242411372323685E-3</v>
       </c>
       <c r="D62" s="14">
         <f t="shared" si="4"/>
-        <v>-7.3003477658113587</v>
+        <v>-6.7895221420453682</v>
       </c>
       <c r="E62" s="14">
-        <f>D62+LN(SimParameters!$B$9)</f>
-        <v>-7.9934949463713041</v>
+        <f>D62+LN(SimParameters!$B$22)</f>
+        <v>-7.7703513950570944</v>
       </c>
       <c r="F62" s="14">
         <f t="shared" si="2"/>
-        <v>3.3753797302196509E-4</v>
+        <v>4.218868655680942E-4</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -11684,19 +11930,19 @@
       </c>
       <c r="C63" s="3">
         <f>potential_preec_untrt!F63</f>
-        <v>1.6790597265531311E-3</v>
+        <v>2.7953038894656984E-3</v>
       </c>
       <c r="D63" s="14">
         <f t="shared" si="4"/>
-        <v>-6.3878408578982659</v>
+        <v>-5.8770152341322754</v>
       </c>
       <c r="E63" s="14">
-        <f>D63+LN(SimParameters!$B$9)</f>
-        <v>-7.0809880384582113</v>
+        <f>D63+LN(SimParameters!$B$22)</f>
+        <v>-6.8578444871440016</v>
       </c>
       <c r="F63" s="14">
         <f t="shared" si="2"/>
-        <v>8.4023526587444523E-4</v>
+        <v>1.0500735051453605E-3</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -11708,19 +11954,19 @@
       </c>
       <c r="C64" s="3">
         <f>potential_preec_untrt!F64</f>
-        <v>1.843866022396227E-3</v>
+        <v>3.0693370731001307E-3</v>
       </c>
       <c r="D64" s="14">
         <f t="shared" si="4"/>
-        <v>-6.2940452444187844</v>
+        <v>-5.7832196206527939</v>
       </c>
       <c r="E64" s="14">
-        <f>D64+LN(SimParameters!$B$9)</f>
-        <v>-6.9871924249787298</v>
+        <f>D64+LN(SimParameters!$B$22)</f>
+        <v>-6.7640488736645201</v>
       </c>
       <c r="F64" s="14">
         <f t="shared" si="2"/>
-        <v>9.2278375600497178E-4</v>
+        <v>1.1532136532995975E-3</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -11732,19 +11978,19 @@
       </c>
       <c r="C65" s="3">
         <f>potential_preec_untrt!F65</f>
-        <v>2.2033805153212384E-3</v>
+        <v>3.6669144536297456E-3</v>
       </c>
       <c r="D65" s="14">
         <f t="shared" si="4"/>
-        <v>-6.1155566885733181</v>
+        <v>-5.6047310648073276</v>
       </c>
       <c r="E65" s="14">
-        <f>D65+LN(SimParameters!$B$9)</f>
-        <v>-6.8087038691332635</v>
+        <f>D65+LN(SimParameters!$B$22)</f>
+        <v>-6.5855603178190538</v>
       </c>
       <c r="F65" s="14">
         <f t="shared" si="2"/>
-        <v>1.1029053177042561E-3</v>
+        <v>1.378251626868218E-3</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -11756,19 +12002,19 @@
       </c>
       <c r="C66" s="3">
         <f>potential_preec_untrt!F66</f>
-        <v>2.2033805153212384E-3</v>
+        <v>3.6669144536297456E-3</v>
       </c>
       <c r="D66" s="14">
         <f t="shared" si="4"/>
-        <v>-6.1155566885733181</v>
+        <v>-5.6047310648073276</v>
       </c>
       <c r="E66" s="14">
-        <f>D66+LN(SimParameters!$B$9)</f>
-        <v>-6.8087038691332635</v>
+        <f>D66+LN(SimParameters!$B$22)</f>
+        <v>-6.5855603178190538</v>
       </c>
       <c r="F66" s="14">
         <f t="shared" si="2"/>
-        <v>1.1029053177042561E-3</v>
+        <v>1.378251626868218E-3</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -11780,19 +12026,19 @@
       </c>
       <c r="C67" s="3">
         <f>potential_preec_untrt!F67</f>
-        <v>2.487935013938433E-3</v>
+        <v>4.1396921665054036E-3</v>
       </c>
       <c r="D67" s="14">
         <f t="shared" si="4"/>
-        <v>-5.9938111891788539</v>
+        <v>-5.4829855654128634</v>
       </c>
       <c r="E67" s="14">
-        <f>D67+LN(SimParameters!$B$9)</f>
-        <v>-6.6869583697387993</v>
+        <f>D67+LN(SimParameters!$B$22)</f>
+        <v>-6.4638148184245896</v>
       </c>
       <c r="F67" s="14">
         <f t="shared" si="2"/>
-        <v>1.245516889509147E-3</v>
+        <v>1.5564114776908113E-3</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -11804,19 +12050,19 @@
       </c>
       <c r="C68" s="3">
         <f>potential_preec_untrt!F68</f>
-        <v>4.5381247410173587E-3</v>
+        <v>7.5407273939942943E-3</v>
       </c>
       <c r="D68" s="14">
         <f t="shared" si="4"/>
-        <v>-5.3906929516088624</v>
+        <v>-4.8798673278428719</v>
       </c>
       <c r="E68" s="14">
-        <f>D68+LN(SimParameters!$B$9)</f>
-        <v>-6.0838401321688078</v>
+        <f>D68+LN(SimParameters!$B$22)</f>
+        <v>-5.8606965808545981</v>
       </c>
       <c r="F68" s="14">
         <f t="shared" si="2"/>
-        <v>2.2742227237132128E-3</v>
+        <v>2.8411630452516942E-3</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -11828,19 +12074,19 @@
       </c>
       <c r="C69" s="3">
         <f>potential_preec_untrt!F69</f>
-        <v>6.7497792477962219E-3</v>
+        <v>7.8658936148477791E-3</v>
       </c>
       <c r="D69" s="14">
         <f t="shared" si="4"/>
-        <v>-4.9914728166276303</v>
+        <v>-4.8373221368003723</v>
       </c>
       <c r="E69" s="14">
-        <f>D69+LN(SimParameters!$B$9)</f>
-        <v>-5.6846199971875757</v>
+        <f>D69+LN(SimParameters!$B$23)</f>
+        <v>-5.5304693173603177</v>
       </c>
       <c r="F69" s="14">
         <f t="shared" si="2"/>
-        <v>3.386318073628017E-3</v>
+        <v>3.9484759533186852E-3</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -11852,19 +12098,19 @@
       </c>
       <c r="C70" s="3">
         <f>potential_preec_untrt!F70</f>
-        <v>6.7497792477962219E-3</v>
+        <v>7.8658936148477791E-3</v>
       </c>
       <c r="D70" s="14">
         <f t="shared" si="4"/>
-        <v>-4.9914728166276303</v>
+        <v>-4.8373221368003723</v>
       </c>
       <c r="E70" s="14">
-        <f>D70+LN(SimParameters!$B$9)</f>
-        <v>-5.6846199971875757</v>
+        <f>D70+LN(SimParameters!$B$23)</f>
+        <v>-5.5304693173603177</v>
       </c>
       <c r="F70" s="14">
         <f t="shared" si="2"/>
-        <v>3.386318073628017E-3</v>
+        <v>3.9484759533186852E-3</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -11876,19 +12122,19 @@
       </c>
       <c r="C71" s="3">
         <f>potential_preec_untrt!F71</f>
-        <v>9.092359227947041E-3</v>
+        <v>1.059170183961137E-2</v>
       </c>
       <c r="D71" s="14">
         <f t="shared" si="4"/>
-        <v>-4.6911869164340274</v>
+        <v>-4.5370362366067694</v>
       </c>
       <c r="E71" s="14">
-        <f>D71+LN(SimParameters!$B$9)</f>
-        <v>-5.3843340969939728</v>
+        <f>D71+LN(SimParameters!$B$23)</f>
+        <v>-5.2301834171667148</v>
       </c>
       <c r="F71" s="14">
         <f t="shared" si="2"/>
-        <v>4.5669417514622238E-3</v>
+        <v>5.3240462751691277E-3</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -11900,19 +12146,19 @@
       </c>
       <c r="C72" s="3">
         <f>potential_preec_untrt!F72</f>
-        <v>1.8114951668613183E-2</v>
+        <v>2.1070495113280241E-2</v>
       </c>
       <c r="D72" s="14">
         <f t="shared" si="4"/>
-        <v>-3.9927365864646918</v>
+        <v>-3.8385859066374337</v>
       </c>
       <c r="E72" s="14">
-        <f>D72+LN(SimParameters!$B$9)</f>
-        <v>-4.6858837670246372</v>
+        <f>D72+LN(SimParameters!$B$23)</f>
+        <v>-4.5317330871973791</v>
       </c>
       <c r="F72" s="14">
         <f t="shared" si="2"/>
-        <v>9.1402635505347524E-3</v>
+        <v>1.0647420770294886E-2</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -11924,19 +12170,19 @@
       </c>
       <c r="C73" s="3">
         <f>potential_preec_untrt!F73</f>
-        <v>2.8879293269421218E-2</v>
+        <v>3.3531116323996135E-2</v>
       </c>
       <c r="D73" s="14">
         <f t="shared" si="4"/>
-        <v>-3.5153259298924526</v>
+        <v>-3.3611752500651941</v>
       </c>
       <c r="E73" s="14">
-        <f>D73+LN(SimParameters!$B$9)</f>
-        <v>-4.208473110452398</v>
+        <f>D73+LN(SimParameters!$B$23)</f>
+        <v>-4.0543224306251391</v>
       </c>
       <c r="F73" s="14">
         <f t="shared" si="2"/>
-        <v>1.4651204855598203E-2</v>
+        <v>1.7051434987018457E-2</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -11948,19 +12194,19 @@
       </c>
       <c r="C74" s="3">
         <f>potential_preec_untrt!F74</f>
-        <v>3.5807446051695509E-2</v>
+        <v>4.1527521313794037E-2</v>
       </c>
       <c r="D74" s="14">
         <f t="shared" si="4"/>
-        <v>-3.293135157373368</v>
+        <v>-3.1389844775461095</v>
       </c>
       <c r="E74" s="14">
-        <f>D74+LN(SimParameters!$B$9)</f>
-        <v>-3.9862823379333134</v>
+        <f>D74+LN(SimParameters!$B$23)</f>
+        <v>-3.8321316581060549</v>
       </c>
       <c r="F74" s="14">
         <f t="shared" si="2"/>
-        <v>1.8230109863575993E-2</v>
+        <v>2.1204036189291651E-2</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -11972,19 +12218,19 @@
       </c>
       <c r="C75" s="3">
         <f>potential_preec_untrt!F75</f>
-        <v>3.8645673954888708E-2</v>
+        <v>4.4798077630385208E-2</v>
       </c>
       <c r="D75" s="14">
         <f t="shared" si="4"/>
-        <v>-3.2139082065303413</v>
+        <v>-3.0597575267030832</v>
       </c>
       <c r="E75" s="14">
-        <f>D75+LN(SimParameters!$B$9)</f>
-        <v>-3.9070553870902867</v>
+        <f>D75+LN(SimParameters!$B$23)</f>
+        <v>-3.7529047072630286</v>
       </c>
       <c r="F75" s="14">
         <f t="shared" si="2"/>
-        <v>1.9703565766627247E-2</v>
+        <v>2.2912251219603951E-2</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -11996,19 +12242,19 @@
       </c>
       <c r="C76" s="3">
         <f>potential_preec_untrt!F76</f>
-        <v>0.14146871337506789</v>
+        <v>0.16124497898504517</v>
       </c>
       <c r="D76" s="14">
         <f t="shared" si="4"/>
-        <v>-1.8031445372883401</v>
+        <v>-1.6489938574610816</v>
       </c>
       <c r="E76" s="14">
-        <f>D76+LN(SimParameters!$B$9)</f>
-        <v>-2.4962917178482855</v>
+        <f>D76+LN(SimParameters!$B$23)</f>
+        <v>-2.342141038021027</v>
       </c>
       <c r="F76" s="14">
         <f t="shared" si="2"/>
-        <v>7.6118553609056075E-2</v>
+        <v>8.7692475148778259E-2</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -12020,19 +12266,19 @@
       </c>
       <c r="C77" s="3">
         <f>potential_preec_untrt!F77</f>
-        <v>0.15793362827666566</v>
+        <v>0.17953025554873517</v>
       </c>
       <c r="D77" s="14">
         <f t="shared" si="4"/>
-        <v>-1.6736839668376779</v>
+        <v>-1.5195332870104195</v>
       </c>
       <c r="E77" s="14">
-        <f>D77+LN(SimParameters!$B$9)</f>
-        <v>-2.3668311473976233</v>
+        <f>D77+LN(SimParameters!$B$23)</f>
+        <v>-2.2126804675703649</v>
       </c>
       <c r="F77" s="14">
         <f t="shared" si="2"/>
-        <v>8.5737208333547588E-2</v>
+        <v>9.8617544233260551E-2</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -12044,19 +12290,19 @@
       </c>
       <c r="C78" s="3">
         <f>potential_preec_untrt!F78</f>
-        <v>0.17189238107807461</v>
+        <v>0.14746843428216497</v>
       </c>
       <c r="D78" s="14">
         <f t="shared" si="4"/>
-        <v>-1.5722745309023358</v>
+        <v>-1.7545960876962905</v>
       </c>
       <c r="E78" s="14">
-        <f>D78+LN(SimParameters!$B$9)</f>
-        <v>-2.265421711462281</v>
+        <f>D78+LN(SimParameters!$B$24)</f>
+        <v>-2.1550736542934157</v>
       </c>
       <c r="F78" s="14">
         <f t="shared" si="2"/>
-        <v>9.4027495591010812E-2</v>
+        <v>0.10385806019200271</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -12068,19 +12314,19 @@
       </c>
       <c r="C79" s="3">
         <f>potential_preec_untrt!F79</f>
-        <v>0.18415618547024593</v>
+        <v>0.15832284303282657</v>
       </c>
       <c r="D79" s="14">
         <f t="shared" si="4"/>
-        <v>-1.4884387012510119</v>
+        <v>-1.6707602580449665</v>
       </c>
       <c r="E79" s="14">
-        <f>D79+LN(SimParameters!$B$9)</f>
-        <v>-2.1815858818109573</v>
+        <f>D79+LN(SimParameters!$B$24)</f>
+        <v>-2.0712378246420919</v>
       </c>
       <c r="F79" s="14">
         <f t="shared" si="2"/>
-        <v>0.10141631344980874</v>
+        <v>0.11192394341733543</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -12092,19 +12338,19 @@
       </c>
       <c r="C80" s="3">
         <f>potential_preec_untrt!F80</f>
-        <v>0.22309643260455042</v>
+        <v>0.19309343664977838</v>
       </c>
       <c r="D80" s="14">
         <f t="shared" si="4"/>
-        <v>-1.2477121225872485</v>
+        <v>-1.4300336793812032</v>
       </c>
       <c r="E80" s="14">
-        <f>D80+LN(SimParameters!$B$9)</f>
-        <v>-1.9408593031471937</v>
+        <f>D80+LN(SimParameters!$B$24)</f>
+        <v>-1.8305112459783284</v>
       </c>
       <c r="F80" s="14">
         <f t="shared" si="2"/>
-        <v>0.12555348342935729</v>
+        <v>0.13817738049337216</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -12116,19 +12362,19 @@
       </c>
       <c r="C81" s="3">
         <f>potential_preec_untrt!F81</f>
-        <v>0.24617792444430164</v>
+        <v>0.21392556218426864</v>
       </c>
       <c r="D81" s="14">
         <f t="shared" si="4"/>
-        <v>-1.1191018215002528</v>
+        <v>-1.3014233782942073</v>
       </c>
       <c r="E81" s="14">
-        <f>D81+LN(SimParameters!$B$9)</f>
-        <v>-1.8122490020601982</v>
+        <f>D81+LN(SimParameters!$B$24)</f>
+        <v>-1.7019009448913325</v>
       </c>
       <c r="F81" s="14">
         <f t="shared" si="2"/>
-        <v>0.14036653311385655</v>
+        <v>0.15421715380080755</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -12140,19 +12386,19 @@
       </c>
       <c r="C82" s="3">
         <f>potential_preec_untrt!F82</f>
-        <v>0.25983604685680362</v>
+        <v>0.22633155514183764</v>
       </c>
       <c r="D82" s="14">
         <f t="shared" si="4"/>
-        <v>-1.0468208768610561</v>
+        <v>-1.2291424336550107</v>
       </c>
       <c r="E82" s="14">
-        <f>D82+LN(SimParameters!$B$9)</f>
-        <v>-1.7399680574210015</v>
+        <f>D82+LN(SimParameters!$B$24)</f>
+        <v>-1.6296200002521359</v>
       </c>
       <c r="F82" s="14">
         <f t="shared" si="2"/>
-        <v>0.14931699187738659</v>
+        <v>0.16388242402902969</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -12164,19 +12410,19 @@
       </c>
       <c r="C83" s="3">
         <f>potential_preec_untrt!F83</f>
-        <v>0.28996065926223696</v>
+        <v>0.25390425701057667</v>
       </c>
       <c r="D83" s="14">
         <f t="shared" si="4"/>
-        <v>-0.89557512192836386</v>
+        <v>-1.0778966787223185</v>
       </c>
       <c r="E83" s="14">
-        <f>D83+LN(SimParameters!$B$9)</f>
-        <v>-1.5887223024883093</v>
+        <f>D83+LN(SimParameters!$B$24)</f>
+        <v>-1.4783742453194437</v>
       </c>
       <c r="F83" s="14">
         <f t="shared" si="2"/>
-        <v>0.16956373596477559</v>
+        <v>0.18567310552586552</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -12494,19 +12740,19 @@
       </c>
       <c r="C101" s="4">
         <f>potential_preec_untrt!F101</f>
-        <v>6.7976887858128268E-4</v>
+        <v>1.3586142135022284E-3</v>
       </c>
       <c r="D101" s="13">
         <f>LN(C101/(1-C101))</f>
-        <v>-7.2930777019810167</v>
+        <v>-6.5999305214210713</v>
       </c>
       <c r="E101" s="13">
-        <f>D101+LN(SimParameters!$B$10)</f>
-        <v>-7.5162212532952264</v>
+        <f>D101+LN(SimParameters!$B$26)</f>
+        <v>-7.1107561451870618</v>
       </c>
       <c r="F101" s="13">
         <f t="shared" ref="F101:F124" si="6">EXP(E101)/(1+EXP(E101))</f>
-        <v>5.4388904663448673E-4</v>
+        <v>8.1561176879805272E-4</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -12518,19 +12764,19 @@
       </c>
       <c r="C102" s="4">
         <f>potential_preec_untrt!F102</f>
-        <v>8.9959518216802458E-4</v>
+        <v>1.7975732760772962E-3</v>
       </c>
       <c r="D102" s="13">
         <f t="shared" ref="D102:D124" si="7">LN(C102/(1-C102))</f>
-        <v>-7.0126656933595779</v>
+        <v>-6.3195185127996325</v>
       </c>
       <c r="E102" s="13">
-        <f>D102+LN(SimParameters!$B$10)</f>
-        <v>-7.2358092446737876</v>
+        <f>D102+LN(SimParameters!$B$26)</f>
+        <v>-6.830344136565623</v>
       </c>
       <c r="F102" s="13">
         <f t="shared" si="6"/>
-        <v>7.1980565247383235E-4</v>
+        <v>1.0793200283821197E-3</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -12542,19 +12788,19 @@
       </c>
       <c r="C103" s="4">
         <f>potential_preec_untrt!F103</f>
-        <v>8.9959518216802458E-4</v>
+        <v>1.7975732760772962E-3</v>
       </c>
       <c r="D103" s="13">
         <f t="shared" si="7"/>
-        <v>-7.0126656933595779</v>
+        <v>-6.3195185127996325</v>
       </c>
       <c r="E103" s="13">
-        <f>D103+LN(SimParameters!$B$10)</f>
-        <v>-7.2358092446737876</v>
+        <f>D103+LN(SimParameters!$B$26)</f>
+        <v>-6.830344136565623</v>
       </c>
       <c r="F103" s="13">
         <f t="shared" si="6"/>
-        <v>7.1980565247383235E-4</v>
+        <v>1.0793200283821197E-3</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -12566,19 +12812,19 @@
       </c>
       <c r="C104" s="4">
         <f>potential_preec_untrt!F104</f>
-        <v>2.237494006712483E-3</v>
+        <v>4.4649976080369976E-3</v>
       </c>
       <c r="D104" s="13">
         <f t="shared" si="7"/>
-        <v>-6.1001587854464852</v>
+        <v>-5.4070116048865398</v>
       </c>
       <c r="E104" s="13">
-        <f>D104+LN(SimParameters!$B$10)</f>
-        <v>-6.3233023367606949</v>
+        <f>D104+LN(SimParameters!$B$26)</f>
+        <v>-5.9178372286525303</v>
       </c>
       <c r="F104" s="13">
         <f t="shared" si="6"/>
-        <v>1.7907965846950856E-3</v>
+        <v>2.6837918144349679E-3</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -12590,19 +12836,19 @@
       </c>
       <c r="C105" s="4">
         <f>potential_preec_untrt!F105</f>
-        <v>2.456977917161892E-3</v>
+        <v>4.9019119449232344E-3</v>
       </c>
       <c r="D105" s="13">
         <f t="shared" si="7"/>
-        <v>-6.0063631719670036</v>
+        <v>-5.3132159914070582</v>
       </c>
       <c r="E105" s="13">
-        <f>D105+LN(SimParameters!$B$10)</f>
-        <v>-6.2295067232812134</v>
+        <f>D105+LN(SimParameters!$B$26)</f>
+        <v>-5.8240416151730487</v>
       </c>
       <c r="F105" s="13">
         <f t="shared" si="6"/>
-        <v>1.9665486870689441E-3</v>
+        <v>2.9469253944707226E-3</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -12614,19 +12860,19 @@
       </c>
       <c r="C106" s="4">
         <f>potential_preec_untrt!F106</f>
-        <v>2.9356845437207299E-3</v>
+        <v>5.8541830527374262E-3</v>
       </c>
       <c r="D106" s="13">
         <f t="shared" si="7"/>
-        <v>-5.8278746161215373</v>
+        <v>-5.1347274355615919</v>
       </c>
       <c r="E106" s="13">
-        <f>D106+LN(SimParameters!$B$10)</f>
-        <v>-6.0510181674357471</v>
+        <f>D106+LN(SimParameters!$B$26)</f>
+        <v>-5.6455530593275824</v>
       </c>
       <c r="F106" s="13">
         <f t="shared" si="6"/>
-        <v>2.349927364064894E-3</v>
+        <v>3.520754287675963E-3</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -12638,19 +12884,19 @@
       </c>
       <c r="C107" s="4">
         <f>potential_preec_untrt!F107</f>
-        <v>2.9356845437207299E-3</v>
+        <v>5.8541830527374262E-3</v>
       </c>
       <c r="D107" s="13">
         <f t="shared" si="7"/>
-        <v>-5.8278746161215373</v>
+        <v>-5.1347274355615919</v>
       </c>
       <c r="E107" s="13">
-        <f>D107+LN(SimParameters!$B$10)</f>
-        <v>-6.0510181674357471</v>
+        <f>D107+LN(SimParameters!$B$26)</f>
+        <v>-5.6455530593275824</v>
       </c>
       <c r="F107" s="13">
         <f t="shared" si="6"/>
-        <v>2.349927364064894E-3</v>
+        <v>3.520754287675963E-3</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -12662,19 +12908,19 @@
       </c>
       <c r="C108" s="4">
         <f>potential_preec_untrt!F108</f>
-        <v>3.3144979334305074E-3</v>
+        <v>6.6070966586399766E-3</v>
       </c>
       <c r="D108" s="13">
         <f t="shared" si="7"/>
-        <v>-5.7061291167270731</v>
+        <v>-5.0129819361671277</v>
       </c>
       <c r="E108" s="13">
-        <f>D108+LN(SimParameters!$B$10)</f>
-        <v>-5.9292726680412828</v>
+        <f>D108+LN(SimParameters!$B$26)</f>
+        <v>-5.5238075599331182</v>
       </c>
       <c r="F108" s="13">
         <f t="shared" si="6"/>
-        <v>2.6533572561728536E-3</v>
+        <v>3.9747626515976905E-3</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -12686,19 +12932,19 @@
       </c>
       <c r="C109" s="4">
         <f>potential_preec_untrt!F109</f>
-        <v>6.0416936681853984E-3</v>
+        <v>1.2010821631370839E-2</v>
       </c>
       <c r="D109" s="13">
         <f t="shared" si="7"/>
-        <v>-5.1030108791570816</v>
+        <v>-4.4098636985971362</v>
       </c>
       <c r="E109" s="13">
-        <f>D109+LN(SimParameters!$B$10)</f>
-        <v>-5.3261544304712913</v>
+        <f>D109+LN(SimParameters!$B$26)</f>
+        <v>-4.9206893223631267</v>
       </c>
       <c r="F109" s="13">
         <f t="shared" si="6"/>
-        <v>4.8392023301637617E-3</v>
+        <v>7.241282479721025E-3</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -12710,19 +12956,19 @@
       </c>
       <c r="C110" s="4">
         <f>potential_preec_untrt!F110</f>
-        <v>8.9795024439776622E-3</v>
+        <v>1.1641991390128838E-2</v>
       </c>
       <c r="D110" s="13">
         <f t="shared" si="7"/>
-        <v>-4.7037907441758495</v>
+        <v>-4.4414264797083582</v>
       </c>
       <c r="E110" s="13">
-        <f>D110+LN(SimParameters!$B$10)</f>
-        <v>-4.9269342954900592</v>
+        <f>D110+LN(SimParameters!$B$27)</f>
+        <v>-4.664570031022568</v>
       </c>
       <c r="F110" s="13">
         <f t="shared" si="6"/>
-        <v>7.1965262001025265E-3</v>
+        <v>9.3353294771825451E-3</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -12734,19 +12980,19 @@
       </c>
       <c r="C111" s="4">
         <f>potential_preec_untrt!F111</f>
-        <v>8.9795024439776622E-3</v>
+        <v>1.1641991390128838E-2</v>
       </c>
       <c r="D111" s="13">
         <f t="shared" si="7"/>
-        <v>-4.7037907441758495</v>
+        <v>-4.4414264797083582</v>
       </c>
       <c r="E111" s="13">
-        <f>D111+LN(SimParameters!$B$10)</f>
-        <v>-4.9269342954900592</v>
+        <f>D111+LN(SimParameters!$B$27)</f>
+        <v>-4.664570031022568</v>
       </c>
       <c r="F111" s="13">
         <f t="shared" si="6"/>
-        <v>7.1965262001025265E-3</v>
+        <v>9.3353294771825451E-3</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -12758,19 +13004,19 @@
       </c>
       <c r="C112" s="4">
         <f>potential_preec_untrt!F112</f>
-        <v>1.2086513994910942E-2</v>
+        <v>1.5655701337389877E-2</v>
       </c>
       <c r="D112" s="13">
         <f t="shared" si="7"/>
-        <v>-4.4035048439822466</v>
+        <v>-4.1411405795147553</v>
       </c>
       <c r="E112" s="13">
-        <f>D112+LN(SimParameters!$B$10)</f>
-        <v>-4.6266483952964563</v>
+        <f>D112+LN(SimParameters!$B$27)</f>
+        <v>-4.364284130828965</v>
       </c>
       <c r="F112" s="13">
         <f t="shared" si="6"/>
-        <v>9.6926412447391908E-3</v>
+        <v>1.2563900404384652E-2</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -12782,19 +13028,19 @@
       </c>
       <c r="C113" s="4">
         <f>potential_preec_untrt!F113</f>
-        <v>2.400829916514351E-2</v>
+        <v>3.0987601035862834E-2</v>
       </c>
       <c r="D113" s="13">
         <f t="shared" si="7"/>
-        <v>-3.705054514012911</v>
+        <v>-3.4426902495454201</v>
       </c>
       <c r="E113" s="13">
-        <f>D113+LN(SimParameters!$B$10)</f>
-        <v>-3.9281980653271207</v>
+        <f>D113+LN(SimParameters!$B$27)</f>
+        <v>-3.6658338008596298</v>
       </c>
       <c r="F113" s="13">
         <f t="shared" si="6"/>
-        <v>1.9299308044356648E-2</v>
+        <v>2.4944675962026295E-2</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -12806,19 +13052,19 @@
       </c>
       <c r="C114" s="4">
         <f>potential_preec_untrt!F114</f>
-        <v>3.813858589029271E-2</v>
+        <v>4.9019303581404002E-2</v>
       </c>
       <c r="D114" s="13">
         <f t="shared" si="7"/>
-        <v>-3.2276438574406714</v>
+        <v>-2.9652795929731806</v>
       </c>
       <c r="E114" s="13">
-        <f>D114+LN(SimParameters!$B$10)</f>
-        <v>-3.4507874087548811</v>
+        <f>D114+LN(SimParameters!$B$27)</f>
+        <v>-3.1884231442873903</v>
       </c>
       <c r="F114" s="13">
         <f t="shared" si="6"/>
-        <v>3.0745385819797879E-2</v>
+        <v>3.9603712142819082E-2</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -12830,19 +13076,19 @@
       </c>
       <c r="C115" s="4">
         <f>potential_preec_untrt!F115</f>
-        <v>4.7180128104983593E-2</v>
+        <v>6.047815638671513E-2</v>
       </c>
       <c r="D115" s="13">
         <f t="shared" si="7"/>
-        <v>-3.0054530849215868</v>
+        <v>-2.7430888204540955</v>
       </c>
       <c r="E115" s="13">
-        <f>D115+LN(SimParameters!$B$10)</f>
-        <v>-3.2285966362357965</v>
+        <f>D115+LN(SimParameters!$B$27)</f>
+        <v>-2.9662323717683052</v>
       </c>
       <c r="F115" s="13">
         <f t="shared" si="6"/>
-        <v>3.8103649496893037E-2</v>
+        <v>4.897490753272999E-2</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -12854,19 +13100,19 @@
       </c>
       <c r="C116" s="4">
         <f>potential_preec_untrt!F116</f>
-        <v>5.0872234674982947E-2</v>
+        <v>6.5139763477192428E-2</v>
       </c>
       <c r="D116" s="13">
         <f t="shared" si="7"/>
-        <v>-2.9262261340785605</v>
+        <v>-2.6638618696110696</v>
       </c>
       <c r="E116" s="13">
-        <f>D116+LN(SimParameters!$B$10)</f>
-        <v>-3.1493696853927702</v>
+        <f>D116+LN(SimParameters!$B$27)</f>
+        <v>-2.8870054209252793</v>
       </c>
       <c r="F116" s="13">
         <f t="shared" si="6"/>
-        <v>4.1116121536734739E-2</v>
+        <v>5.2799682548327731E-2</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -12878,19 +13124,19 @@
       </c>
       <c r="C117" s="4">
         <f>potential_preec_untrt!F117</f>
-        <v>0.18013066661813684</v>
+        <v>0.22216428630625154</v>
       </c>
       <c r="D117" s="13">
         <f t="shared" si="7"/>
-        <v>-1.5154624648365589</v>
+        <v>-1.253098200369068</v>
       </c>
       <c r="E117" s="13">
-        <f>D117+LN(SimParameters!$B$10)</f>
-        <v>-1.7386060161507686</v>
+        <f>D117+LN(SimParameters!$B$27)</f>
+        <v>-1.4762417516832778</v>
       </c>
       <c r="F117" s="13">
         <f t="shared" si="6"/>
-        <v>0.14949008295355434</v>
+        <v>0.18599575173295038</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -12902,19 +13148,19 @@
       </c>
       <c r="C118" s="4">
         <f>potential_preec_untrt!F118</f>
-        <v>0.20004679878323164</v>
+        <v>0.24533716412638895</v>
       </c>
       <c r="D118" s="13">
         <f t="shared" si="7"/>
-        <v>-1.3860018943858967</v>
+        <v>-1.1236376299184059</v>
       </c>
       <c r="E118" s="13">
-        <f>D118+LN(SimParameters!$B$10)</f>
-        <v>-1.6091454457001064</v>
+        <f>D118+LN(SimParameters!$B$27)</f>
+        <v>-1.3467811812326156</v>
       </c>
       <c r="F118" s="13">
         <f t="shared" si="6"/>
-        <v>0.16670729100652112</v>
+        <v>0.20639710750914791</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -12926,19 +13172,19 @@
       </c>
       <c r="C119" s="4">
         <f>potential_preec_untrt!F119</f>
-        <v>0.21676949962552158</v>
+        <v>0.19495587305369466</v>
       </c>
       <c r="D119" s="13">
         <f t="shared" si="7"/>
-        <v>-1.2845924584505546</v>
+        <v>-1.4181238510750771</v>
       </c>
       <c r="E119" s="13">
-        <f>D119+LN(SimParameters!$B$10)</f>
-        <v>-1.5077360097647643</v>
+        <f>D119+LN(SimParameters!$B$28)</f>
+        <v>-1.4694171454626277</v>
       </c>
       <c r="F119" s="13">
         <f t="shared" si="6"/>
-        <v>0.18127455878076607</v>
+        <v>0.18703122115140347</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -12950,19 +13196,19 @@
       </c>
       <c r="C120" s="4">
         <f>potential_preec_untrt!F120</f>
-        <v>0.23134064379200564</v>
+        <v>0.20845096075038702</v>
       </c>
       <c r="D120" s="13">
         <f t="shared" si="7"/>
-        <v>-1.2007566287992311</v>
+        <v>-1.3342880214237536</v>
       </c>
       <c r="E120" s="13">
-        <f>D120+LN(SimParameters!$B$10)</f>
-        <v>-1.4239001801134408</v>
+        <f>D120+LN(SimParameters!$B$28)</f>
+        <v>-1.3855813158113042</v>
       </c>
       <c r="F120" s="13">
         <f t="shared" si="6"/>
-        <v>0.1940508864327572</v>
+        <v>0.20011411165457296</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -12974,19 +13220,19 @@
       </c>
       <c r="C121" s="4">
         <f>potential_preec_untrt!F121</f>
-        <v>0.27687217837819206</v>
+        <v>0.25094822893146868</v>
       </c>
       <c r="D121" s="13">
         <f t="shared" si="7"/>
-        <v>-0.96003005013546761</v>
+        <v>-1.0935614427599902</v>
       </c>
       <c r="E121" s="13">
-        <f>D121+LN(SimParameters!$B$10)</f>
-        <v>-1.1831736014496772</v>
+        <f>D121+LN(SimParameters!$B$28)</f>
+        <v>-1.1448547371475408</v>
       </c>
       <c r="F121" s="13">
         <f t="shared" si="6"/>
-        <v>0.23448205412583636</v>
+        <v>0.24143014079708033</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -12998,19 +13244,19 @@
       </c>
       <c r="C122" s="4">
         <f>potential_preec_untrt!F122</f>
-        <v>0.3033449554203887</v>
+        <v>0.27588798973628692</v>
       </c>
       <c r="D122" s="13">
         <f t="shared" si="7"/>
-        <v>-0.83141974904847182</v>
+        <v>-0.96495114167299456</v>
       </c>
       <c r="E122" s="13">
-        <f>D122+LN(SimParameters!$B$10)</f>
-        <v>-1.0545633003626815</v>
+        <f>D122+LN(SimParameters!$B$28)</f>
+        <v>-1.0162444360605452</v>
       </c>
       <c r="F122" s="13">
         <f t="shared" si="6"/>
-        <v>0.2583497851480302</v>
+        <v>0.26575958412027728</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -13022,19 +13268,19 @@
       </c>
       <c r="C123" s="4">
         <f>potential_preec_untrt!F123</f>
-        <v>0.31883327028958103</v>
+        <v>0.29055910001203777</v>
       </c>
       <c r="D123" s="13">
         <f t="shared" si="7"/>
-        <v>-0.75913880440927506</v>
+        <v>-0.89267019703379802</v>
       </c>
       <c r="E123" s="13">
-        <f>D123+LN(SimParameters!$B$10)</f>
-        <v>-0.98228235572348477</v>
+        <f>D123+LN(SimParameters!$B$28)</f>
+        <v>-0.94396349142134861</v>
       </c>
       <c r="F123" s="13">
         <f t="shared" si="6"/>
-        <v>0.27243914921125173</v>
+        <v>0.28010043147556202</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -13046,19 +13292,19 @@
       </c>
       <c r="C124" s="4">
         <f>potential_preec_untrt!F124</f>
-        <v>0.35253997149894151</v>
+        <v>0.32269273605818222</v>
       </c>
       <c r="D124" s="13">
         <f t="shared" si="7"/>
-        <v>-0.60789304947658318</v>
+        <v>-0.7414244421011057</v>
       </c>
       <c r="E124" s="13">
-        <f>D124+LN(SimParameters!$B$10)</f>
-        <v>-0.83103660079079289</v>
+        <f>D124+LN(SimParameters!$B$28)</f>
+        <v>-0.79271773648865629</v>
       </c>
       <c r="F124" s="13">
         <f t="shared" si="6"/>
-        <v>0.30342593101345805</v>
+        <v>0.31158541678823426</v>
       </c>
     </row>
   </sheetData>
@@ -13367,7 +13613,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="2">
-        <f>potential_preg_untrt!C26*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C26*SimParameters!$B$58</f>
         <v>1.5E-6</v>
       </c>
     </row>
@@ -13379,7 +13625,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="2">
-        <f>potential_preg_untrt!C27*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C27*SimParameters!$B$58</f>
         <v>1.5E-6</v>
       </c>
     </row>
@@ -13391,7 +13637,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="2">
-        <f>potential_preg_untrt!C28*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C28*SimParameters!$B$58</f>
         <v>1.5E-6</v>
       </c>
     </row>
@@ -13403,7 +13649,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="2">
-        <f>potential_preg_untrt!C29*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C29*SimParameters!$B$58</f>
         <v>1.5E-5</v>
       </c>
     </row>
@@ -13415,7 +13661,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="2">
-        <f>potential_preg_untrt!C30*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C30*SimParameters!$B$58</f>
         <v>6.2500000000000001E-5</v>
       </c>
     </row>
@@ -13427,7 +13673,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="2">
-        <f>potential_preg_untrt!C31*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C31*SimParameters!$B$58</f>
         <v>6.2500000000000001E-5</v>
       </c>
     </row>
@@ -13439,7 +13685,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="2">
-        <f>potential_preg_untrt!C32*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C32*SimParameters!$B$58</f>
         <v>6.2500000000000001E-5</v>
       </c>
     </row>
@@ -13451,7 +13697,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="2">
-        <f>potential_preg_untrt!C33*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C33*SimParameters!$B$58</f>
         <v>3.7499999999999995E-4</v>
       </c>
     </row>
@@ -13463,7 +13709,7 @@
         <v>32</v>
       </c>
       <c r="C34" s="2">
-        <f>potential_preg_untrt!C34*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C34*SimParameters!$B$58</f>
         <v>8.7500000000000002E-4</v>
       </c>
     </row>
@@ -13475,7 +13721,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="2">
-        <f>potential_preg_untrt!C35*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C35*SimParameters!$B$58</f>
         <v>1.3750000000000001E-3</v>
       </c>
     </row>
@@ -13487,7 +13733,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="2">
-        <f>potential_preg_untrt!C36*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C36*SimParameters!$B$58</f>
         <v>8.7500000000000008E-3</v>
       </c>
     </row>
@@ -13499,7 +13745,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="2">
-        <f>potential_preg_untrt!C37*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C37*SimParameters!$B$58</f>
         <v>3.7499999999999999E-3</v>
       </c>
     </row>
@@ -13511,7 +13757,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="2">
-        <f>potential_preg_untrt!C38*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C38*SimParameters!$B$58</f>
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
@@ -13523,7 +13769,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="2">
-        <f>potential_preg_untrt!C39*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C39*SimParameters!$B$58</f>
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -13535,7 +13781,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="2">
-        <f>potential_preg_untrt!C40*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C40*SimParameters!$B$58</f>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -13547,7 +13793,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="2">
-        <f>potential_preg_untrt!C41*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C41*SimParameters!$B$58</f>
         <v>0.5</v>
       </c>
     </row>
@@ -13559,7 +13805,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="2">
-        <f>potential_preg_untrt!C42*SimParameters!$B$28</f>
+        <f>potential_preg_untrt!C42*SimParameters!$B$58</f>
         <v>0.5</v>
       </c>
     </row>
@@ -16032,6 +16278,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -16256,16 +16511,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16282,12 +16536,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>